<commit_message>
20/11/2017 - Code review comment fixes.
</commit_message>
<xml_diff>
--- a/src/main/resources/config/stageSA/TestData/TestData.xlsx
+++ b/src/main/resources/config/stageSA/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7728" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7728" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="S181372" sheetId="1" r:id="rId1"/>
@@ -14,21 +14,21 @@
     <sheet name="HelpDesk" sheetId="15" r:id="rId5"/>
     <sheet name="CurrencyExchangeRates" sheetId="16" r:id="rId6"/>
     <sheet name="CurrencyExchangeRateMapping" sheetId="17" r:id="rId7"/>
-    <sheet name="AccountMaster_S205195" sheetId="7" r:id="rId8"/>
-    <sheet name="AccountHeadMapping_S205175" sheetId="18" r:id="rId9"/>
-    <sheet name="AccountHead_S205168" sheetId="9" r:id="rId10"/>
-    <sheet name="Events Configuration" sheetId="14" r:id="rId11"/>
-    <sheet name="SuspenseAccount_S205193" sheetId="10" r:id="rId12"/>
-    <sheet name="Institute" sheetId="5" r:id="rId13"/>
-    <sheet name="QMRReporting" sheetId="12" r:id="rId14"/>
+    <sheet name="CardHolder" sheetId="19" r:id="rId8"/>
+    <sheet name="AccountMaster_S205195" sheetId="7" r:id="rId9"/>
+    <sheet name="AccountHeadMapping_S205175" sheetId="18" r:id="rId10"/>
+    <sheet name="AccountHead_S205168" sheetId="9" r:id="rId11"/>
+    <sheet name="Events Configuration" sheetId="14" r:id="rId12"/>
+    <sheet name="SuspenseAccount_S205193" sheetId="10" r:id="rId13"/>
+    <sheet name="Institute" sheetId="5" r:id="rId14"/>
+    <sheet name="QMRReporting" sheetId="12" r:id="rId15"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H25"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1899" uniqueCount="605">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1520,6 +1520,330 @@
   </si>
   <si>
     <t>5130003313500015</t>
+  </si>
+  <si>
+    <t>TranSactionType</t>
+  </si>
+  <si>
+    <t>TransactionAmount</t>
+  </si>
+  <si>
+    <t>TransactionCurrency</t>
+  </si>
+  <si>
+    <t>ConversionRate</t>
+  </si>
+  <si>
+    <t>CardNumber</t>
+  </si>
+  <si>
+    <t>TransferAmount</t>
+  </si>
+  <si>
+    <t>CurrencyName</t>
+  </si>
+  <si>
+    <t>ContactNumber</t>
+  </si>
+  <si>
+    <t>TransfererName</t>
+  </si>
+  <si>
+    <t>Memo</t>
+  </si>
+  <si>
+    <t>TransactionPassword</t>
+  </si>
+  <si>
+    <t>TransactionRemarks</t>
+  </si>
+  <si>
+    <t>AmountToTransferWalletToWallet</t>
+  </si>
+  <si>
+    <t>WalletTransferCurrecny</t>
+  </si>
+  <si>
+    <t>WalletNumberFromTransferMoney</t>
+  </si>
+  <si>
+    <t>WalletToWalletTransferSucessMsg</t>
+  </si>
+  <si>
+    <t>NoOfTransactionsCount</t>
+  </si>
+  <si>
+    <t>FromDate</t>
+  </si>
+  <si>
+    <t>ToDate</t>
+  </si>
+  <si>
+    <t>ReplacementResone</t>
+  </si>
+  <si>
+    <t>ReplaceConfirmMessage</t>
+  </si>
+  <si>
+    <t>BlockCardRemark</t>
+  </si>
+  <si>
+    <t>BlockConfirmationMsg</t>
+  </si>
+  <si>
+    <t>UnblockCardRemark</t>
+  </si>
+  <si>
+    <t>UnblockConfirmationMsg</t>
+  </si>
+  <si>
+    <t>WalletActivationRemark</t>
+  </si>
+  <si>
+    <t>WalletDeactivateRemark</t>
+  </si>
+  <si>
+    <t>WalletActivateConfirmMsg</t>
+  </si>
+  <si>
+    <t>WalletDeactivateConfirmMsg</t>
+  </si>
+  <si>
+    <t>eComActivationConfirmMsg</t>
+  </si>
+  <si>
+    <t>beneficiaryID</t>
+  </si>
+  <si>
+    <t>beneficiaryFirstName</t>
+  </si>
+  <si>
+    <t>beneficiaryMiddleName</t>
+  </si>
+  <si>
+    <t>beneficiaryLastName</t>
+  </si>
+  <si>
+    <t>beneficiaryAddressLine1</t>
+  </si>
+  <si>
+    <t>beneficiaryAddressLine2</t>
+  </si>
+  <si>
+    <t>beneficiaryAddressLine3</t>
+  </si>
+  <si>
+    <t>beneficiaryCountryName</t>
+  </si>
+  <si>
+    <t>beneficiaryStateName</t>
+  </si>
+  <si>
+    <t>beneficiaryCityName</t>
+  </si>
+  <si>
+    <t>beneficiaryZIPCode</t>
+  </si>
+  <si>
+    <t>beneficiaryEmailAddress</t>
+  </si>
+  <si>
+    <t>beneficiaryMobileNumber</t>
+  </si>
+  <si>
+    <t>beneficiaryRemittanceAamount</t>
+  </si>
+  <si>
+    <t>beneficiaryRemittanceCurrency</t>
+  </si>
+  <si>
+    <t>newPassword</t>
+  </si>
+  <si>
+    <t>CardHolderTransPassword</t>
+  </si>
+  <si>
+    <t>FirstSequrityQuestion</t>
+  </si>
+  <si>
+    <t>FirstSequrityAnswer</t>
+  </si>
+  <si>
+    <t>SecondSequrityQuestion</t>
+  </si>
+  <si>
+    <t>SecondSequrityAnswer</t>
+  </si>
+  <si>
+    <t>TC_walletToWalletTransfer</t>
+  </si>
+  <si>
+    <t>https://stage.sa.cardholder.mastercard.com/mpts/eis/app</t>
+  </si>
+  <si>
+    <t>10000172850000001</t>
+  </si>
+  <si>
+    <t>qweR@1234</t>
+  </si>
+  <si>
+    <t>Fund Transfer</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>0.016000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">454564Done </t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>1000011210179768581</t>
+  </si>
+  <si>
+    <t>Your transaction is successful</t>
+  </si>
+  <si>
+    <t>TC_LoginCardholderPortal</t>
+  </si>
+  <si>
+    <t>TC_viewChargeForRefundOnWalletClosure</t>
+  </si>
+  <si>
+    <t>TC_masterCardMoneyTransfer</t>
+  </si>
+  <si>
+    <t>4564564564654654564</t>
+  </si>
+  <si>
+    <t>Tester</t>
+  </si>
+  <si>
+    <t>CMKO-45</t>
+  </si>
+  <si>
+    <t>TC_checkInterbankTransfer</t>
+  </si>
+  <si>
+    <t>TC_viewTransactionHistoryForWallet</t>
+  </si>
+  <si>
+    <t>05/10/2017</t>
+  </si>
+  <si>
+    <t>31/10/2017</t>
+  </si>
+  <si>
+    <t>TC_deviceReplaceService</t>
+  </si>
+  <si>
+    <t>Emergency Replacement</t>
+  </si>
+  <si>
+    <t>Request is forwarded to institution</t>
+  </si>
+  <si>
+    <t>TC_deviceBlockFromCardHolder</t>
+  </si>
+  <si>
+    <t>Card need to block as it is stolne</t>
+  </si>
+  <si>
+    <t>Device Blocked Call Reference Number</t>
+  </si>
+  <si>
+    <t>Block my card</t>
+  </si>
+  <si>
+    <t>Unblock Device process successful</t>
+  </si>
+  <si>
+    <t>TC_deviceUnblockFromCardholder</t>
+  </si>
+  <si>
+    <t>TC_walletActivateFromCardHolder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activate Wallet </t>
+  </si>
+  <si>
+    <t>Request has been processed successfully with reference number</t>
+  </si>
+  <si>
+    <t>TC_walletDeActivateFromCardHolder</t>
+  </si>
+  <si>
+    <t>Deactivate Wallet</t>
+  </si>
+  <si>
+    <t>TC_activateEcomForLifeLong</t>
+  </si>
+  <si>
+    <t>DEVICE is already activated for life long use</t>
+  </si>
+  <si>
+    <t>TC_activationEcomForDuration</t>
+  </si>
+  <si>
+    <t>TC_activateEcomForNHours</t>
+  </si>
+  <si>
+    <t>TC_cashRemittanceBookting</t>
+  </si>
+  <si>
+    <t>10000173090000012</t>
+  </si>
+  <si>
+    <t>000000070</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>Fname</t>
+  </si>
+  <si>
+    <t>Mname</t>
+  </si>
+  <si>
+    <t>Lname</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Address3</t>
+  </si>
+  <si>
+    <t>INDIA</t>
+  </si>
+  <si>
+    <t>MAHARASTHRA</t>
+  </si>
+  <si>
+    <t>mastercard@mastercard.com</t>
+  </si>
+  <si>
+    <t>INR</t>
+  </si>
+  <si>
+    <t>TC_signUpCardholderPortal</t>
+  </si>
+  <si>
+    <t>aBcd1234*</t>
+  </si>
+  <si>
+    <t>TC_activationForInternationalUse</t>
+  </si>
+  <si>
+    <t>TC_activationNHoursForInternationalUse</t>
+  </si>
+  <si>
+    <t>TC_activationLifeLongForInternationalUse</t>
   </si>
 </sst>
 </file>
@@ -1629,7 +1953,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1695,6 +2019,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2644,7 +2979,363 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:O9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" customWidth="1"/>
+    <col min="11" max="15" width="17.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>351</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>349</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>350</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>476</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>477</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>271</v>
+      </c>
+      <c r="I1" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="J1" s="30" t="s">
+        <v>272</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>273</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>478</v>
+      </c>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+    </row>
+    <row r="2" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="32" t="s">
+        <v>280</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>495</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>454</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="E2" s="32">
+        <v>4656</v>
+      </c>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>479</v>
+      </c>
+      <c r="J2" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+    </row>
+    <row r="3" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="32" t="s">
+        <v>480</v>
+      </c>
+      <c r="B3" s="32" t="s">
+        <v>495</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>454</v>
+      </c>
+      <c r="D3" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="E3" s="32">
+        <v>4656</v>
+      </c>
+      <c r="F3" s="32" t="s">
+        <v>481</v>
+      </c>
+      <c r="G3" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="H3" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+    </row>
+    <row r="4" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="32" t="s">
+        <v>482</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>495</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>454</v>
+      </c>
+      <c r="D4" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="E4" s="32">
+        <v>4656</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>483</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="I4" s="32" t="s">
+        <v>484</v>
+      </c>
+      <c r="J4" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="K4" s="32"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="32"/>
+      <c r="O4" s="32"/>
+    </row>
+    <row r="5" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="32" t="s">
+        <v>485</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>495</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>454</v>
+      </c>
+      <c r="D5" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="E5" s="32">
+        <v>4656</v>
+      </c>
+      <c r="F5" s="32" t="s">
+        <v>481</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="K5" s="32"/>
+      <c r="L5" s="32"/>
+      <c r="M5" s="32"/>
+      <c r="N5" s="32"/>
+      <c r="O5" s="32"/>
+    </row>
+    <row r="6" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="32" t="s">
+        <v>486</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>495</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>454</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="E6" s="32">
+        <v>4656</v>
+      </c>
+      <c r="F6" s="32" t="s">
+        <v>481</v>
+      </c>
+      <c r="G6" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="H6" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="I6" s="32" t="s">
+        <v>487</v>
+      </c>
+      <c r="J6" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
+      <c r="N6" s="32"/>
+      <c r="O6" s="32"/>
+    </row>
+    <row r="7" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="32" t="s">
+        <v>488</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>495</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>454</v>
+      </c>
+      <c r="D7" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="E7" s="32">
+        <v>4656</v>
+      </c>
+      <c r="F7" s="32" t="s">
+        <v>481</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="H7" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="I7" s="32"/>
+      <c r="J7" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="K7" s="32"/>
+      <c r="L7" s="32" t="s">
+        <v>489</v>
+      </c>
+      <c r="M7" s="32"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+    </row>
+    <row r="8" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="32" t="s">
+        <v>490</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>495</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>454</v>
+      </c>
+      <c r="D8" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="E8" s="32">
+        <v>4656</v>
+      </c>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="I8" s="32" t="s">
+        <v>491</v>
+      </c>
+      <c r="J8" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="K8" s="32" t="s">
+        <v>492</v>
+      </c>
+      <c r="L8" s="32"/>
+      <c r="M8" s="32"/>
+      <c r="N8" s="32"/>
+      <c r="O8" s="32"/>
+    </row>
+    <row r="9" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="32" t="s">
+        <v>493</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>495</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>454</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>353</v>
+      </c>
+      <c r="E9" s="32">
+        <v>4656</v>
+      </c>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32" t="s">
+        <v>467</v>
+      </c>
+      <c r="H9" s="32" t="s">
+        <v>390</v>
+      </c>
+      <c r="I9" s="32" t="s">
+        <v>494</v>
+      </c>
+      <c r="J9" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
@@ -2664,7 +3355,7 @@
     <col min="11" max="11" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
@@ -2695,7 +3386,7 @@
       <c r="J1" s="30"/>
       <c r="K1" s="34"/>
     </row>
-    <row r="2" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>281</v>
       </c>
@@ -2724,7 +3415,7 @@
       <c r="J2" s="32"/>
       <c r="K2" s="32"/>
     </row>
-    <row r="3" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>283</v>
       </c>
@@ -2753,7 +3444,7 @@
       <c r="J3" s="32"/>
       <c r="K3" s="32"/>
     </row>
-    <row r="4" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
         <v>285</v>
       </c>
@@ -2782,23 +3473,14 @@
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
     </row>
-    <row r="5" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
@@ -2943,10 +3625,6 @@
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:19" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:19" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:19" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:19" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
@@ -2955,9 +3633,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
@@ -2977,7 +3655,7 @@
     <col min="11" max="11" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
@@ -3008,7 +3686,7 @@
       <c r="J1" s="30"/>
       <c r="K1" s="34"/>
     </row>
-    <row r="2" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>274</v>
       </c>
@@ -3039,7 +3717,7 @@
       <c r="J2" s="32"/>
       <c r="K2" s="32"/>
     </row>
-    <row r="3" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>278</v>
       </c>
@@ -3070,22 +3748,12 @@
       <c r="J3" s="32"/>
       <c r="K3" s="32"/>
     </row>
-    <row r="4" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD2"/>
   <sheetViews>
@@ -3310,7 +3978,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S9"/>
   <sheetViews>
@@ -7286,7 +7954,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA23"/>
+  <dimension ref="A1:AA22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
@@ -7311,7 +7979,7 @@
     <col min="28" max="16384" width="8.88671875" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
@@ -7394,7 +8062,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>389</v>
       </c>
@@ -7449,7 +8117,7 @@
       <c r="Z2" s="32"/>
       <c r="AA2" s="32"/>
     </row>
-    <row r="3" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>392</v>
       </c>
@@ -7494,7 +8162,7 @@
       <c r="Z3" s="32"/>
       <c r="AA3" s="32"/>
     </row>
-    <row r="4" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
         <v>396</v>
       </c>
@@ -7539,7 +8207,7 @@
       <c r="Z4" s="32"/>
       <c r="AA4" s="32"/>
     </row>
-    <row r="5" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
         <v>399</v>
       </c>
@@ -7584,7 +8252,7 @@
       <c r="Z5" s="32"/>
       <c r="AA5" s="32"/>
     </row>
-    <row r="6" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
         <v>402</v>
       </c>
@@ -7629,7 +8297,7 @@
       <c r="Z6" s="32"/>
       <c r="AA6" s="32"/>
     </row>
-    <row r="7" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="32" t="s">
         <v>403</v>
       </c>
@@ -7674,7 +8342,7 @@
       <c r="Z7" s="32"/>
       <c r="AA7" s="32"/>
     </row>
-    <row r="8" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="32" t="s">
         <v>404</v>
       </c>
@@ -7715,7 +8383,7 @@
       <c r="Z8" s="32"/>
       <c r="AA8" s="32"/>
     </row>
-    <row r="9" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="32" t="s">
         <v>405</v>
       </c>
@@ -7756,7 +8424,7 @@
       <c r="Z9" s="32"/>
       <c r="AA9" s="32"/>
     </row>
-    <row r="10" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="32" t="s">
         <v>406</v>
       </c>
@@ -7797,7 +8465,7 @@
       <c r="Z10" s="32"/>
       <c r="AA10" s="32"/>
     </row>
-    <row r="11" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
         <v>409</v>
       </c>
@@ -7840,7 +8508,7 @@
       <c r="Z11" s="32"/>
       <c r="AA11" s="32"/>
     </row>
-    <row r="12" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="32" t="s">
         <v>411</v>
       </c>
@@ -7883,7 +8551,7 @@
       <c r="Z12" s="32"/>
       <c r="AA12" s="32"/>
     </row>
-    <row r="13" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="32" t="s">
         <v>413</v>
       </c>
@@ -7926,7 +8594,7 @@
       <c r="Z13" s="32"/>
       <c r="AA13" s="32"/>
     </row>
-    <row r="14" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="32" t="s">
         <v>415</v>
       </c>
@@ -7969,7 +8637,7 @@
       <c r="Z14" s="32"/>
       <c r="AA14" s="32"/>
     </row>
-    <row r="15" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="32" t="s">
         <v>417</v>
       </c>
@@ -8012,7 +8680,7 @@
       <c r="Z15" s="32"/>
       <c r="AA15" s="32"/>
     </row>
-    <row r="16" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="32" t="s">
         <v>418</v>
       </c>
@@ -8055,7 +8723,7 @@
       <c r="Z16" s="32"/>
       <c r="AA16" s="32"/>
     </row>
-    <row r="17" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
         <v>420</v>
       </c>
@@ -8116,7 +8784,7 @@
       </c>
       <c r="AA17" s="32"/>
     </row>
-    <row r="18" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="32" t="s">
         <v>426</v>
       </c>
@@ -8171,7 +8839,7 @@
       </c>
       <c r="AA18" s="32"/>
     </row>
-    <row r="19" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="32" t="s">
         <v>430</v>
       </c>
@@ -8228,7 +8896,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="20" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" s="32" t="s">
         <v>433</v>
       </c>
@@ -8285,7 +8953,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="21" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" s="32" t="s">
         <v>435</v>
       </c>
@@ -8342,7 +9010,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="22" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" s="32" t="s">
         <v>437</v>
       </c>
@@ -8399,7 +9067,6 @@
         <v>432</v>
       </c>
     </row>
-    <row r="23" spans="1:27" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8407,7 +9074,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
@@ -8431,7 +9098,7 @@
     <col min="18" max="16384" width="8.88671875" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
@@ -8474,8 +9141,11 @@
       <c r="N1" s="30" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>447</v>
       </c>
@@ -8514,99 +9184,24 @@
       <c r="N2" s="32" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O5"/>
-      <c r="P5"/>
-      <c r="Q5"/>
-    </row>
-    <row r="6" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
-    </row>
-    <row r="7" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7"/>
-    </row>
-    <row r="8" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O8"/>
-      <c r="P8"/>
-      <c r="Q8"/>
-    </row>
-    <row r="9" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O9"/>
-      <c r="P9"/>
-      <c r="Q9"/>
-    </row>
-    <row r="10" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O10"/>
-      <c r="P10"/>
-      <c r="Q10"/>
-    </row>
-    <row r="11" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O11"/>
-      <c r="P11"/>
-      <c r="Q11"/>
-    </row>
-    <row r="12" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O12"/>
-      <c r="P12"/>
-      <c r="Q12"/>
-    </row>
-    <row r="13" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O14"/>
-      <c r="P14"/>
-      <c r="Q14"/>
-    </row>
-    <row r="15" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O15"/>
-      <c r="P15"/>
-      <c r="Q15"/>
-    </row>
-    <row r="16" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O16"/>
-      <c r="P16"/>
-      <c r="Q16"/>
-    </row>
-    <row r="17" spans="15:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O17"/>
-      <c r="P17"/>
-      <c r="Q17"/>
-    </row>
-    <row r="18" spans="15:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O18"/>
-      <c r="P18"/>
-      <c r="Q18"/>
-    </row>
-    <row r="19" spans="15:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O19"/>
-      <c r="P19"/>
-      <c r="Q19"/>
-    </row>
-    <row r="20" spans="15:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O20"/>
-      <c r="P20"/>
-      <c r="Q20"/>
-    </row>
-    <row r="21" spans="15:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O21"/>
-      <c r="P21"/>
-      <c r="Q21"/>
-    </row>
-    <row r="22" spans="15:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O22"/>
-      <c r="P22"/>
-      <c r="Q22"/>
-    </row>
-    <row r="23" spans="15:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="O23"/>
-      <c r="P23"/>
-      <c r="Q23"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8615,9 +9210,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -8634,7 +9229,7 @@
     <col min="11" max="11" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
@@ -8669,7 +9264,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>459</v>
       </c>
@@ -8702,17 +9297,6 @@
         <v>462</v>
       </c>
     </row>
-    <row r="3" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please select from the dropdown" sqref="J2">
@@ -8725,7 +9309,2023 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:BC20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="40.5546875" customWidth="1"/>
+    <col min="2" max="2" width="49.88671875" customWidth="1"/>
+    <col min="3" max="3" width="24.21875" style="42" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" style="43" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" style="43" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" style="43" customWidth="1"/>
+    <col min="10" max="10" width="18.109375" style="43" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="12" max="12" width="15.44140625" customWidth="1"/>
+    <col min="13" max="13" width="14.77734375" customWidth="1"/>
+    <col min="15" max="15" width="19.6640625" customWidth="1"/>
+    <col min="16" max="16" width="18.21875" customWidth="1"/>
+    <col min="17" max="17" width="30.88671875" customWidth="1"/>
+    <col min="18" max="18" width="22.33203125" customWidth="1"/>
+    <col min="19" max="19" width="30.44140625" customWidth="1"/>
+    <col min="20" max="20" width="31.88671875" customWidth="1"/>
+    <col min="21" max="21" width="23.109375" customWidth="1"/>
+    <col min="22" max="22" width="12.21875" style="43" customWidth="1"/>
+    <col min="23" max="23" width="12.44140625" customWidth="1"/>
+    <col min="24" max="24" width="24.33203125" customWidth="1"/>
+    <col min="25" max="25" width="31.5546875" customWidth="1"/>
+    <col min="26" max="26" width="33.5546875" customWidth="1"/>
+    <col min="27" max="27" width="29.77734375" customWidth="1"/>
+    <col min="28" max="28" width="28" customWidth="1"/>
+    <col min="29" max="29" width="30.5546875" customWidth="1"/>
+    <col min="30" max="30" width="24.6640625" customWidth="1"/>
+    <col min="31" max="31" width="22.88671875" customWidth="1"/>
+    <col min="32" max="32" width="45.21875" customWidth="1"/>
+    <col min="33" max="33" width="56.6640625" customWidth="1"/>
+    <col min="34" max="34" width="41.109375" customWidth="1"/>
+    <col min="35" max="35" width="16.5546875" customWidth="1"/>
+    <col min="36" max="36" width="19.6640625" customWidth="1"/>
+    <col min="37" max="37" width="22.88671875" customWidth="1"/>
+    <col min="38" max="38" width="18.44140625" customWidth="1"/>
+    <col min="39" max="40" width="22.33203125" customWidth="1"/>
+    <col min="41" max="42" width="22.5546875" customWidth="1"/>
+    <col min="43" max="43" width="24.44140625" customWidth="1"/>
+    <col min="44" max="44" width="20.109375" customWidth="1"/>
+    <col min="45" max="45" width="19.109375" customWidth="1"/>
+    <col min="46" max="46" width="23.6640625" customWidth="1"/>
+    <col min="47" max="47" width="23.5546875" customWidth="1"/>
+    <col min="48" max="48" width="29.6640625" customWidth="1"/>
+    <col min="49" max="49" width="28.88671875" customWidth="1"/>
+    <col min="50" max="55" width="24.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>351</v>
+      </c>
+      <c r="C1" s="36" t="s">
+        <v>349</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>350</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>497</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>498</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>499</v>
+      </c>
+      <c r="H1" s="20" t="s">
+        <v>500</v>
+      </c>
+      <c r="I1" s="20" t="s">
+        <v>501</v>
+      </c>
+      <c r="J1" s="20" t="s">
+        <v>502</v>
+      </c>
+      <c r="K1" s="20" t="s">
+        <v>503</v>
+      </c>
+      <c r="L1" s="20" t="s">
+        <v>504</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>505</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>506</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>507</v>
+      </c>
+      <c r="P1" s="20" t="s">
+        <v>508</v>
+      </c>
+      <c r="Q1" s="20" t="s">
+        <v>509</v>
+      </c>
+      <c r="R1" s="20" t="s">
+        <v>510</v>
+      </c>
+      <c r="S1" s="37" t="s">
+        <v>511</v>
+      </c>
+      <c r="T1" s="21" t="s">
+        <v>512</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="Z1" s="20" t="s">
+        <v>518</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="AJ1" s="38" t="s">
+        <v>528</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="AS1" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="2" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F2" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" t="s">
+        <v>551</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="Q2" s="24" t="s">
+        <v>556</v>
+      </c>
+      <c r="R2" s="24" t="s">
+        <v>553</v>
+      </c>
+      <c r="S2" s="24" t="s">
+        <v>557</v>
+      </c>
+      <c r="T2" s="40" t="s">
+        <v>558</v>
+      </c>
+      <c r="U2" s="2"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+      <c r="AG2" s="2"/>
+      <c r="AH2" s="2"/>
+      <c r="AI2" s="2"/>
+      <c r="AJ2" s="2"/>
+      <c r="AK2" s="2"/>
+      <c r="AL2" s="2"/>
+      <c r="AM2" s="2"/>
+      <c r="AN2" s="2"/>
+      <c r="AO2" s="2"/>
+      <c r="AP2" s="2"/>
+      <c r="AQ2" s="2"/>
+      <c r="AR2" s="2"/>
+      <c r="AS2" s="2"/>
+      <c r="AT2" s="2"/>
+      <c r="AU2" s="2"/>
+      <c r="AV2" s="2"/>
+      <c r="AW2" s="2"/>
+      <c r="AX2" s="2"/>
+      <c r="AY2" s="2"/>
+      <c r="AZ2" s="2"/>
+      <c r="BA2" s="2"/>
+      <c r="BB2" s="2"/>
+      <c r="BC2" s="2"/>
+    </row>
+    <row r="3" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F3" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2"/>
+      <c r="AT3" s="2"/>
+      <c r="AU3" s="2"/>
+      <c r="AV3" s="2"/>
+      <c r="AW3" s="2"/>
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="2"/>
+      <c r="AZ3" s="2"/>
+      <c r="BA3" s="2"/>
+      <c r="BB3" s="2"/>
+      <c r="BC3" s="2"/>
+    </row>
+    <row r="4" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>588</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="2"/>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2"/>
+      <c r="AO4" s="2"/>
+      <c r="AP4" s="2"/>
+      <c r="AQ4" s="2"/>
+      <c r="AR4" s="2"/>
+      <c r="AS4" s="2"/>
+      <c r="AT4" s="2"/>
+      <c r="AU4" s="2"/>
+      <c r="AV4" s="2"/>
+      <c r="AW4" s="2"/>
+      <c r="AX4" s="2"/>
+      <c r="AY4" s="2"/>
+      <c r="AZ4" s="2"/>
+      <c r="BA4" s="2"/>
+      <c r="BB4" s="2"/>
+      <c r="BC4" s="2"/>
+    </row>
+    <row r="5" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F5" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>562</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>556</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="L5" s="2">
+        <v>955689456</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="O5" t="s">
+        <v>551</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="2"/>
+      <c r="AB5" s="2"/>
+      <c r="AC5" s="2"/>
+      <c r="AD5" s="2"/>
+      <c r="AE5" s="2"/>
+      <c r="AF5" s="2"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+      <c r="AJ5" s="2"/>
+      <c r="AK5" s="2"/>
+      <c r="AL5" s="2"/>
+      <c r="AM5" s="2"/>
+      <c r="AN5" s="2"/>
+      <c r="AO5" s="2"/>
+      <c r="AP5" s="2"/>
+      <c r="AQ5" s="2"/>
+      <c r="AR5" s="2"/>
+      <c r="AS5" s="2"/>
+      <c r="AT5" s="2"/>
+      <c r="AU5" s="2"/>
+      <c r="AV5" s="2"/>
+      <c r="AW5" s="2"/>
+      <c r="AX5" s="2"/>
+      <c r="AY5" s="2"/>
+      <c r="AZ5" s="2"/>
+      <c r="BA5" s="2"/>
+      <c r="BB5" s="2"/>
+      <c r="BC5" s="2"/>
+    </row>
+    <row r="6" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F6" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
+      <c r="Y6" s="2"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="2"/>
+      <c r="AB6" s="2"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="2"/>
+      <c r="AE6" s="2"/>
+      <c r="AF6" s="2"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+      <c r="AJ6" s="2"/>
+      <c r="AK6" s="2"/>
+      <c r="AL6" s="2"/>
+      <c r="AM6" s="2"/>
+      <c r="AN6" s="2"/>
+      <c r="AO6" s="2"/>
+      <c r="AP6" s="2"/>
+      <c r="AQ6" s="2"/>
+      <c r="AR6" s="2"/>
+      <c r="AS6" s="2"/>
+      <c r="AT6" s="2"/>
+      <c r="AU6" s="2"/>
+      <c r="AV6" s="2"/>
+      <c r="AW6" s="2"/>
+      <c r="AX6" s="2"/>
+      <c r="AY6" s="2"/>
+      <c r="AZ6" s="2"/>
+      <c r="BA6" s="2"/>
+      <c r="BB6" s="2"/>
+      <c r="BC6" s="2"/>
+    </row>
+    <row r="7" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F7" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2">
+        <v>10</v>
+      </c>
+      <c r="V7" s="9" t="s">
+        <v>567</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="X7" s="2"/>
+      <c r="Y7" s="2"/>
+      <c r="Z7" s="2"/>
+      <c r="AA7" s="2"/>
+      <c r="AB7" s="2"/>
+      <c r="AC7" s="2"/>
+      <c r="AD7" s="2"/>
+      <c r="AE7" s="2"/>
+      <c r="AF7" s="2"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+      <c r="AJ7" s="2"/>
+      <c r="AK7" s="2"/>
+      <c r="AL7" s="2"/>
+      <c r="AM7" s="2"/>
+      <c r="AN7" s="2"/>
+      <c r="AO7" s="2"/>
+      <c r="AP7" s="2"/>
+      <c r="AQ7" s="2"/>
+      <c r="AR7" s="2"/>
+      <c r="AS7" s="2"/>
+      <c r="AT7" s="2"/>
+      <c r="AU7" s="2"/>
+      <c r="AV7" s="2"/>
+      <c r="AW7" s="2"/>
+      <c r="AX7" s="2"/>
+      <c r="AY7" s="2"/>
+      <c r="AZ7" s="2"/>
+      <c r="BA7" s="2"/>
+      <c r="BB7" s="2"/>
+      <c r="BC7" s="2"/>
+    </row>
+    <row r="8" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F8" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="2"/>
+      <c r="S8" s="2"/>
+      <c r="T8" s="2"/>
+      <c r="U8" s="2">
+        <v>10</v>
+      </c>
+      <c r="V8" s="9" t="s">
+        <v>567</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="X8" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="Y8" s="40" t="s">
+        <v>571</v>
+      </c>
+      <c r="Z8" s="2"/>
+      <c r="AA8" s="2"/>
+      <c r="AB8" s="2"/>
+      <c r="AC8" s="2"/>
+      <c r="AD8" s="2"/>
+      <c r="AE8" s="2"/>
+      <c r="AF8" s="2"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+      <c r="AJ8" s="2"/>
+      <c r="AK8" s="2"/>
+      <c r="AL8" s="2"/>
+      <c r="AM8" s="2"/>
+      <c r="AN8" s="2"/>
+      <c r="AO8" s="2"/>
+      <c r="AP8" s="2"/>
+      <c r="AQ8" s="2"/>
+      <c r="AR8" s="2"/>
+      <c r="AS8" s="2"/>
+      <c r="AT8" s="2"/>
+      <c r="AU8" s="2"/>
+      <c r="AV8" s="2"/>
+      <c r="AW8" s="2"/>
+      <c r="AX8" s="2"/>
+      <c r="AY8" s="2"/>
+      <c r="AZ8" s="2"/>
+      <c r="BA8" s="2"/>
+      <c r="BB8" s="2"/>
+      <c r="BC8" s="2"/>
+    </row>
+    <row r="9" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F9" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2">
+        <v>10</v>
+      </c>
+      <c r="V9" s="9" t="s">
+        <v>567</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="Y9" s="40" t="s">
+        <v>571</v>
+      </c>
+      <c r="Z9" s="40" t="s">
+        <v>573</v>
+      </c>
+      <c r="AA9" s="40" t="s">
+        <v>574</v>
+      </c>
+      <c r="AB9" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="AC9" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="AD9" s="2"/>
+      <c r="AE9" s="2"/>
+      <c r="AF9" s="2"/>
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2"/>
+      <c r="AJ9" s="2"/>
+      <c r="AK9" s="2"/>
+      <c r="AL9" s="2"/>
+      <c r="AM9" s="2"/>
+      <c r="AN9" s="2"/>
+      <c r="AO9" s="2"/>
+      <c r="AP9" s="2"/>
+      <c r="AQ9" s="2"/>
+      <c r="AR9" s="2"/>
+      <c r="AS9" s="2"/>
+      <c r="AT9" s="2"/>
+      <c r="AU9" s="2"/>
+      <c r="AV9" s="2"/>
+      <c r="AW9" s="2"/>
+      <c r="AX9" s="2"/>
+      <c r="AY9" s="2"/>
+      <c r="AZ9" s="2"/>
+      <c r="BA9" s="2"/>
+      <c r="BB9" s="2"/>
+      <c r="BC9" s="2"/>
+    </row>
+    <row r="10" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F10" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+      <c r="U10" s="2">
+        <v>10</v>
+      </c>
+      <c r="V10" s="9" t="s">
+        <v>567</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="Y10" s="40" t="s">
+        <v>571</v>
+      </c>
+      <c r="Z10" s="40" t="s">
+        <v>573</v>
+      </c>
+      <c r="AA10" s="40" t="s">
+        <v>574</v>
+      </c>
+      <c r="AB10" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="AC10" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="AD10" s="2"/>
+      <c r="AE10" s="2"/>
+      <c r="AF10" s="2"/>
+      <c r="AG10" s="2"/>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="2"/>
+      <c r="AJ10" s="2"/>
+      <c r="AK10" s="2"/>
+      <c r="AL10" s="2"/>
+      <c r="AM10" s="2"/>
+      <c r="AN10" s="2"/>
+      <c r="AO10" s="2"/>
+      <c r="AP10" s="2"/>
+      <c r="AQ10" s="2"/>
+      <c r="AR10" s="2"/>
+      <c r="AS10" s="2"/>
+      <c r="AT10" s="2"/>
+      <c r="AU10" s="2"/>
+      <c r="AV10" s="2"/>
+      <c r="AW10" s="2"/>
+      <c r="AX10" s="2"/>
+      <c r="AY10" s="2"/>
+      <c r="AZ10" s="2"/>
+      <c r="BA10" s="2"/>
+      <c r="BB10" s="2"/>
+      <c r="BC10" s="2"/>
+    </row>
+    <row r="11" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F11" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+      <c r="U11" s="2">
+        <v>10</v>
+      </c>
+      <c r="V11" s="9" t="s">
+        <v>567</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="X11" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="Y11" s="40" t="s">
+        <v>571</v>
+      </c>
+      <c r="Z11" s="40" t="s">
+        <v>573</v>
+      </c>
+      <c r="AA11" s="40" t="s">
+        <v>574</v>
+      </c>
+      <c r="AB11" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="AC11" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="AD11" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="AE11" s="2"/>
+      <c r="AF11" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AG11" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AH11" s="2"/>
+      <c r="AI11" s="2"/>
+      <c r="AJ11" s="2"/>
+      <c r="AK11" s="2"/>
+      <c r="AL11" s="2"/>
+      <c r="AM11" s="2"/>
+      <c r="AN11" s="2"/>
+      <c r="AO11" s="2"/>
+      <c r="AP11" s="2"/>
+      <c r="AQ11" s="2"/>
+      <c r="AR11" s="2"/>
+      <c r="AS11" s="2"/>
+      <c r="AT11" s="2"/>
+      <c r="AU11" s="2"/>
+      <c r="AV11" s="2"/>
+      <c r="AW11" s="2"/>
+      <c r="AX11" s="2"/>
+      <c r="AY11" s="2"/>
+      <c r="AZ11" s="2"/>
+      <c r="BA11" s="2"/>
+      <c r="BB11" s="2"/>
+      <c r="BC11" s="2"/>
+    </row>
+    <row r="12" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F12" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2">
+        <v>10</v>
+      </c>
+      <c r="V12" s="9" t="s">
+        <v>567</v>
+      </c>
+      <c r="W12" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="X12" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="Y12" s="40" t="s">
+        <v>571</v>
+      </c>
+      <c r="Z12" s="40" t="s">
+        <v>573</v>
+      </c>
+      <c r="AA12" s="40" t="s">
+        <v>574</v>
+      </c>
+      <c r="AB12" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="AC12" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="AD12" s="2"/>
+      <c r="AE12" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="AF12" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AG12" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AH12" s="2"/>
+      <c r="AI12" s="2"/>
+      <c r="AJ12" s="2"/>
+      <c r="AK12" s="2"/>
+      <c r="AL12" s="2"/>
+      <c r="AM12" s="2"/>
+      <c r="AN12" s="2"/>
+      <c r="AO12" s="2"/>
+      <c r="AP12" s="2"/>
+      <c r="AQ12" s="2"/>
+      <c r="AR12" s="2"/>
+      <c r="AS12" s="2"/>
+      <c r="AT12" s="2"/>
+      <c r="AU12" s="2"/>
+      <c r="AV12" s="2"/>
+      <c r="AW12" s="2"/>
+      <c r="AX12" s="2"/>
+      <c r="AY12" s="2"/>
+      <c r="AZ12" s="2"/>
+      <c r="BA12" s="2"/>
+      <c r="BB12" s="2"/>
+      <c r="BC12" s="2"/>
+    </row>
+    <row r="13" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F13" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="2"/>
+      <c r="S13" s="2"/>
+      <c r="T13" s="2"/>
+      <c r="U13" s="2">
+        <v>10</v>
+      </c>
+      <c r="V13" s="9" t="s">
+        <v>567</v>
+      </c>
+      <c r="W13" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="X13" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="Y13" s="40" t="s">
+        <v>571</v>
+      </c>
+      <c r="Z13" s="40" t="s">
+        <v>573</v>
+      </c>
+      <c r="AA13" s="40" t="s">
+        <v>574</v>
+      </c>
+      <c r="AB13" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="AC13" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="AF13" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AG13" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AH13" s="40" t="s">
+        <v>584</v>
+      </c>
+      <c r="AI13" s="2"/>
+      <c r="AJ13" s="2"/>
+      <c r="AK13" s="2"/>
+      <c r="AL13" s="2"/>
+      <c r="AM13" s="2"/>
+      <c r="AN13" s="2"/>
+      <c r="AO13" s="2"/>
+      <c r="AP13" s="2"/>
+      <c r="AQ13" s="2"/>
+      <c r="AR13" s="2"/>
+      <c r="AS13" s="2"/>
+      <c r="AT13" s="2"/>
+      <c r="AU13" s="2"/>
+      <c r="AV13" s="2"/>
+      <c r="AW13" s="2"/>
+      <c r="AX13" s="2"/>
+      <c r="AY13" s="2"/>
+      <c r="AZ13" s="2"/>
+      <c r="BA13" s="2"/>
+      <c r="BB13" s="2"/>
+      <c r="BC13" s="2"/>
+    </row>
+    <row r="14" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F14" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2">
+        <v>10</v>
+      </c>
+      <c r="V14" s="9" t="s">
+        <v>567</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="X14" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="Y14" s="40" t="s">
+        <v>571</v>
+      </c>
+      <c r="Z14" s="40" t="s">
+        <v>573</v>
+      </c>
+      <c r="AA14" s="40" t="s">
+        <v>574</v>
+      </c>
+      <c r="AB14" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="AC14" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="AF14" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AG14" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AH14" s="40" t="s">
+        <v>584</v>
+      </c>
+      <c r="AI14" s="2"/>
+      <c r="AJ14" s="2"/>
+      <c r="AK14" s="2"/>
+      <c r="AL14" s="2"/>
+      <c r="AM14" s="2"/>
+      <c r="AN14" s="2"/>
+      <c r="AO14" s="2"/>
+      <c r="AP14" s="2"/>
+      <c r="AQ14" s="2"/>
+      <c r="AR14" s="2"/>
+      <c r="AS14" s="2"/>
+      <c r="AT14" s="2"/>
+      <c r="AU14" s="2"/>
+      <c r="AV14" s="2"/>
+      <c r="AW14" s="2"/>
+      <c r="AX14" s="2"/>
+      <c r="AY14" s="2"/>
+      <c r="AZ14" s="2"/>
+      <c r="BA14" s="2"/>
+      <c r="BB14" s="2"/>
+      <c r="BC14" s="2"/>
+    </row>
+    <row r="15" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="B15" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F15" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2"/>
+      <c r="T15" s="2"/>
+      <c r="U15" s="2">
+        <v>10</v>
+      </c>
+      <c r="V15" s="9" t="s">
+        <v>567</v>
+      </c>
+      <c r="W15" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="X15" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="Y15" s="40" t="s">
+        <v>571</v>
+      </c>
+      <c r="Z15" s="40" t="s">
+        <v>573</v>
+      </c>
+      <c r="AA15" s="40" t="s">
+        <v>574</v>
+      </c>
+      <c r="AB15" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="AC15" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="AD15" s="2"/>
+      <c r="AE15" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="AF15" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AG15" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="AH15" s="40" t="s">
+        <v>584</v>
+      </c>
+      <c r="AI15" s="2"/>
+      <c r="AJ15" s="2"/>
+      <c r="AK15" s="2"/>
+      <c r="AL15" s="2"/>
+      <c r="AM15" s="2"/>
+      <c r="AN15" s="2"/>
+      <c r="AO15" s="2"/>
+      <c r="AP15" s="2"/>
+      <c r="AQ15" s="2"/>
+      <c r="AR15" s="2"/>
+      <c r="AS15" s="2"/>
+      <c r="AT15" s="2"/>
+      <c r="AU15" s="2"/>
+      <c r="AV15" s="2"/>
+      <c r="AW15" s="2"/>
+      <c r="AX15" s="2"/>
+      <c r="AY15" s="2"/>
+      <c r="AZ15" s="2"/>
+      <c r="BA15" s="2"/>
+      <c r="BB15" s="2"/>
+      <c r="BC15" s="2"/>
+    </row>
+    <row r="16" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>588</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>589</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F16" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
+      <c r="AA16" s="2"/>
+      <c r="AB16" s="2"/>
+      <c r="AC16" s="2"/>
+      <c r="AD16" s="2"/>
+      <c r="AE16" s="2"/>
+      <c r="AF16" s="2"/>
+      <c r="AG16" s="2"/>
+      <c r="AH16" s="2"/>
+      <c r="AI16" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="AJ16" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="AK16" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="AL16" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="AM16" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="AN16" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="AO16" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="AP16" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="AQ16" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="AR16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AS16" s="2">
+        <v>411033</v>
+      </c>
+      <c r="AT16" s="41" t="s">
+        <v>598</v>
+      </c>
+      <c r="AU16" s="2">
+        <v>7896543215</v>
+      </c>
+      <c r="AV16" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AW16" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="AX16" s="2"/>
+      <c r="AY16" s="2"/>
+      <c r="AZ16" s="2"/>
+      <c r="BA16" s="2"/>
+      <c r="BB16" s="2"/>
+      <c r="BC16" s="2"/>
+    </row>
+    <row r="17" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>600</v>
+      </c>
+      <c r="B17" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F17" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="2"/>
+      <c r="S17" s="2"/>
+      <c r="T17" s="2"/>
+      <c r="U17" s="2"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="2"/>
+      <c r="X17" s="2"/>
+      <c r="Y17" s="2"/>
+      <c r="Z17" s="2"/>
+      <c r="AA17" s="2"/>
+      <c r="AB17" s="2"/>
+      <c r="AC17" s="2"/>
+      <c r="AD17" s="2"/>
+      <c r="AE17" s="2"/>
+      <c r="AF17" s="2"/>
+      <c r="AG17" s="2"/>
+      <c r="AH17" s="2"/>
+      <c r="AI17" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="AJ17" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="AK17" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="AL17" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="AM17" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="AN17" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="AO17" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="AP17" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="AQ17" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="AR17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AS17" s="2">
+        <v>411033</v>
+      </c>
+      <c r="AT17" s="41" t="s">
+        <v>598</v>
+      </c>
+      <c r="AU17" s="2">
+        <v>7896543215</v>
+      </c>
+      <c r="AV17" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AW17" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="AX17" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="AY17" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="AZ17" s="2"/>
+      <c r="BA17" s="2"/>
+      <c r="BB17" s="2"/>
+      <c r="BC17" s="2"/>
+    </row>
+    <row r="18" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>602</v>
+      </c>
+      <c r="B18" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F18" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
+      <c r="AA18" s="2"/>
+      <c r="AB18" s="2"/>
+      <c r="AC18" s="2"/>
+      <c r="AD18" s="2"/>
+      <c r="AE18" s="2"/>
+      <c r="AF18" s="2"/>
+      <c r="AG18" s="2"/>
+      <c r="AH18" s="2"/>
+      <c r="AI18" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="AJ18" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="AK18" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="AL18" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="AM18" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="AN18" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="AO18" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="AP18" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="AQ18" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="AR18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AS18" s="2">
+        <v>411033</v>
+      </c>
+      <c r="AT18" s="41" t="s">
+        <v>598</v>
+      </c>
+      <c r="AU18" s="2">
+        <v>7896543215</v>
+      </c>
+      <c r="AV18" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AW18" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="AX18" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="AY18" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="AZ18" s="2"/>
+      <c r="BA18" s="2"/>
+      <c r="BB18" s="2"/>
+      <c r="BC18" s="2"/>
+    </row>
+    <row r="19" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>603</v>
+      </c>
+      <c r="B19" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F19" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+      <c r="AA19" s="2"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="2"/>
+      <c r="AE19" s="2"/>
+      <c r="AF19" s="2"/>
+      <c r="AG19" s="2"/>
+      <c r="AH19" s="2"/>
+      <c r="AI19" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="AJ19" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="AK19" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="AL19" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="AM19" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="AN19" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="AO19" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="AP19" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="AQ19" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="AR19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AS19" s="2">
+        <v>411033</v>
+      </c>
+      <c r="AT19" s="41" t="s">
+        <v>598</v>
+      </c>
+      <c r="AU19" s="2">
+        <v>7896543215</v>
+      </c>
+      <c r="AV19" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AW19" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="AX19" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="AY19" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="AZ19" s="2"/>
+      <c r="BA19" s="2"/>
+      <c r="BB19" s="2"/>
+      <c r="BC19" s="2"/>
+    </row>
+    <row r="20" spans="1:55" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>604</v>
+      </c>
+      <c r="B20" s="39" t="s">
+        <v>549</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="F20" s="2">
+        <v>5000</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="2"/>
+      <c r="AD20" s="2"/>
+      <c r="AE20" s="2"/>
+      <c r="AF20" s="2"/>
+      <c r="AG20" s="2"/>
+      <c r="AH20" s="2"/>
+      <c r="AI20" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="AJ20" s="2" t="s">
+        <v>591</v>
+      </c>
+      <c r="AK20" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="AL20" s="2" t="s">
+        <v>593</v>
+      </c>
+      <c r="AM20" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="AN20" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="AO20" s="2" t="s">
+        <v>595</v>
+      </c>
+      <c r="AP20" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="AQ20" s="2" t="s">
+        <v>597</v>
+      </c>
+      <c r="AR20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AS20" s="2">
+        <v>411033</v>
+      </c>
+      <c r="AT20" s="41" t="s">
+        <v>598</v>
+      </c>
+      <c r="AU20" s="2">
+        <v>7896543215</v>
+      </c>
+      <c r="AV20" s="2">
+        <v>5000</v>
+      </c>
+      <c r="AW20" s="2" t="s">
+        <v>599</v>
+      </c>
+      <c r="AX20" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="AY20" s="2" t="s">
+        <v>601</v>
+      </c>
+      <c r="AZ20" s="2"/>
+      <c r="BA20" s="2"/>
+      <c r="BB20" s="2"/>
+      <c r="BC20" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B16" r:id="rId4"/>
+    <hyperlink ref="B6" r:id="rId5"/>
+    <hyperlink ref="B2" r:id="rId6"/>
+    <hyperlink ref="B7" r:id="rId7"/>
+    <hyperlink ref="B8" r:id="rId8"/>
+    <hyperlink ref="B9" r:id="rId9"/>
+    <hyperlink ref="B10" r:id="rId10"/>
+    <hyperlink ref="B11" r:id="rId11"/>
+    <hyperlink ref="B12" r:id="rId12"/>
+    <hyperlink ref="B13" r:id="rId13"/>
+    <hyperlink ref="B14" r:id="rId14"/>
+    <hyperlink ref="B15" r:id="rId15"/>
+    <hyperlink ref="AT16" r:id="rId16"/>
+    <hyperlink ref="B17" r:id="rId17"/>
+    <hyperlink ref="AT17" r:id="rId18"/>
+    <hyperlink ref="B18" r:id="rId19"/>
+    <hyperlink ref="AT18" r:id="rId20"/>
+    <hyperlink ref="B19" r:id="rId21"/>
+    <hyperlink ref="AT19" r:id="rId22"/>
+    <hyperlink ref="B20" r:id="rId23"/>
+    <hyperlink ref="AT20" r:id="rId24"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
@@ -8744,7 +11344,7 @@
     <col min="11" max="15" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
         <v>1</v>
       </c>
@@ -8791,7 +11391,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="32" t="s">
         <v>465</v>
       </c>
@@ -8834,7 +11434,7 @@
       </c>
       <c r="O2" s="32"/>
     </row>
-    <row r="3" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="32" t="s">
         <v>468</v>
       </c>
@@ -8877,7 +11477,7 @@
       </c>
       <c r="O3" s="32"/>
     </row>
-    <row r="4" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
         <v>470</v>
       </c>
@@ -8922,7 +11522,7 @@
       </c>
       <c r="O4" s="32"/>
     </row>
-    <row r="5" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="32" t="s">
         <v>472</v>
       </c>
@@ -8965,7 +11565,7 @@
       </c>
       <c r="O5" s="32"/>
     </row>
-    <row r="6" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="32" t="s">
         <v>473</v>
       </c>
@@ -9010,373 +11610,6 @@
         <v>474</v>
       </c>
     </row>
-    <row r="7" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="16.21875" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" customWidth="1"/>
-    <col min="11" max="15" width="17.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="30" t="s">
-        <v>351</v>
-      </c>
-      <c r="D1" s="30" t="s">
-        <v>349</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>350</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>476</v>
-      </c>
-      <c r="G1" s="30" t="s">
-        <v>477</v>
-      </c>
-      <c r="H1" s="30" t="s">
-        <v>271</v>
-      </c>
-      <c r="I1" s="30" t="s">
-        <v>270</v>
-      </c>
-      <c r="J1" s="30" t="s">
-        <v>272</v>
-      </c>
-      <c r="K1" s="30" t="s">
-        <v>273</v>
-      </c>
-      <c r="L1" s="30" t="s">
-        <v>478</v>
-      </c>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-    </row>
-    <row r="2" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="32" t="s">
-        <v>280</v>
-      </c>
-      <c r="B2" s="32" t="s">
-        <v>495</v>
-      </c>
-      <c r="C2" s="32" t="s">
-        <v>454</v>
-      </c>
-      <c r="D2" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="E2" s="32">
-        <v>4656</v>
-      </c>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32" t="s">
-        <v>467</v>
-      </c>
-      <c r="H2" s="32" t="s">
-        <v>390</v>
-      </c>
-      <c r="I2" s="32" t="s">
-        <v>479</v>
-      </c>
-      <c r="J2" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-    </row>
-    <row r="3" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
-        <v>480</v>
-      </c>
-      <c r="B3" s="32" t="s">
-        <v>495</v>
-      </c>
-      <c r="C3" s="32" t="s">
-        <v>454</v>
-      </c>
-      <c r="D3" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="E3" s="32">
-        <v>4656</v>
-      </c>
-      <c r="F3" s="32" t="s">
-        <v>481</v>
-      </c>
-      <c r="G3" s="32" t="s">
-        <v>467</v>
-      </c>
-      <c r="H3" s="32" t="s">
-        <v>390</v>
-      </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-    </row>
-    <row r="4" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="32" t="s">
-        <v>482</v>
-      </c>
-      <c r="B4" s="32" t="s">
-        <v>495</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>454</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="E4" s="32">
-        <v>4656</v>
-      </c>
-      <c r="F4" s="32" t="s">
-        <v>483</v>
-      </c>
-      <c r="G4" s="32" t="s">
-        <v>467</v>
-      </c>
-      <c r="H4" s="32" t="s">
-        <v>390</v>
-      </c>
-      <c r="I4" s="32" t="s">
-        <v>484</v>
-      </c>
-      <c r="J4" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-    </row>
-    <row r="5" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="32" t="s">
-        <v>485</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>495</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>454</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="E5" s="32">
-        <v>4656</v>
-      </c>
-      <c r="F5" s="32" t="s">
-        <v>481</v>
-      </c>
-      <c r="G5" s="32" t="s">
-        <v>467</v>
-      </c>
-      <c r="H5" s="32" t="s">
-        <v>390</v>
-      </c>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-    </row>
-    <row r="6" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="32" t="s">
-        <v>486</v>
-      </c>
-      <c r="B6" s="32" t="s">
-        <v>495</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>454</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="E6" s="32">
-        <v>4656</v>
-      </c>
-      <c r="F6" s="32" t="s">
-        <v>481</v>
-      </c>
-      <c r="G6" s="32" t="s">
-        <v>467</v>
-      </c>
-      <c r="H6" s="32" t="s">
-        <v>390</v>
-      </c>
-      <c r="I6" s="32" t="s">
-        <v>487</v>
-      </c>
-      <c r="J6" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="K6" s="32"/>
-      <c r="L6" s="32"/>
-      <c r="M6" s="32"/>
-      <c r="N6" s="32"/>
-      <c r="O6" s="32"/>
-    </row>
-    <row r="7" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="32" t="s">
-        <v>488</v>
-      </c>
-      <c r="B7" s="32" t="s">
-        <v>495</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>454</v>
-      </c>
-      <c r="D7" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="E7" s="32">
-        <v>4656</v>
-      </c>
-      <c r="F7" s="32" t="s">
-        <v>481</v>
-      </c>
-      <c r="G7" s="32" t="s">
-        <v>467</v>
-      </c>
-      <c r="H7" s="32" t="s">
-        <v>390</v>
-      </c>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="K7" s="32"/>
-      <c r="L7" s="32" t="s">
-        <v>489</v>
-      </c>
-      <c r="M7" s="32"/>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-    </row>
-    <row r="8" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="32" t="s">
-        <v>490</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>495</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>454</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="E8" s="32">
-        <v>4656</v>
-      </c>
-      <c r="F8" s="32"/>
-      <c r="G8" s="32" t="s">
-        <v>467</v>
-      </c>
-      <c r="H8" s="32" t="s">
-        <v>390</v>
-      </c>
-      <c r="I8" s="32" t="s">
-        <v>491</v>
-      </c>
-      <c r="J8" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="K8" s="32" t="s">
-        <v>492</v>
-      </c>
-      <c r="L8" s="32"/>
-      <c r="M8" s="32"/>
-      <c r="N8" s="32"/>
-      <c r="O8" s="32"/>
-    </row>
-    <row r="9" spans="1:17" s="31" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="32" t="s">
-        <v>493</v>
-      </c>
-      <c r="B9" s="32" t="s">
-        <v>495</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>454</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>353</v>
-      </c>
-      <c r="E9" s="32">
-        <v>4656</v>
-      </c>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32" t="s">
-        <v>467</v>
-      </c>
-      <c r="H9" s="32" t="s">
-        <v>390</v>
-      </c>
-      <c r="I9" s="32" t="s">
-        <v>494</v>
-      </c>
-      <c r="J9" s="32" t="s">
-        <v>276</v>
-      </c>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-    </row>
-    <row r="10" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:17" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
FileUpload,BVT and Loyalty Scenarios
</commit_message>
<xml_diff>
--- a/src/main/resources/config/stageSA/TestData/TestData.xlsx
+++ b/src/main/resources/config/stageSA/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7728" firstSheet="11" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7728" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="S181372" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,14 @@
     <sheet name="Institute" sheetId="5" r:id="rId13"/>
     <sheet name="QMRReporting" sheetId="12" r:id="rId14"/>
     <sheet name="CreditScenarios" sheetId="19" r:id="rId15"/>
+    <sheet name="LoyaltyPlan" sheetId="20" r:id="rId16"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1576" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1899" uniqueCount="592">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1574,6 +1575,238 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>LoyaltyPlanCode</t>
+  </si>
+  <si>
+    <t>Currency1</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>MaximumPointsEachPeriod</t>
+  </si>
+  <si>
+    <t>PeriodUnit</t>
+  </si>
+  <si>
+    <t>PlanValidityPeriod</t>
+  </si>
+  <si>
+    <t>MinimumPointsRequiredToRedeem</t>
+  </si>
+  <si>
+    <t>GraceDaysForRedemption</t>
+  </si>
+  <si>
+    <t>PointsEarned</t>
+  </si>
+  <si>
+    <t>ValueOfPoints</t>
+  </si>
+  <si>
+    <t>MinimumPointsRequiredToRedeemAutoRedemption</t>
+  </si>
+  <si>
+    <t>AutoRedemptionDate</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>SMSIssuerBIN</t>
+  </si>
+  <si>
+    <t>DMSIssuerBIN</t>
+  </si>
+  <si>
+    <t>programDeviceRange</t>
+  </si>
+  <si>
+    <t>addressLines2</t>
+  </si>
+  <si>
+    <t>PromotionPlanDesc</t>
+  </si>
+  <si>
+    <t>transactionDate</t>
+  </si>
+  <si>
+    <t>memo</t>
+  </si>
+  <si>
+    <t>minutes</t>
+  </si>
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>AdjustmentAmount</t>
+  </si>
+  <si>
+    <t>AdjustmentType</t>
+  </si>
+  <si>
+    <t>promotionCurrency</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>noOfTransactions</t>
+  </si>
+  <si>
+    <t>thresholdAmount</t>
+  </si>
+  <si>
+    <t>LoyaltyBatchSettlementDays</t>
+  </si>
+  <si>
+    <t>BranchCode</t>
+  </si>
+  <si>
+    <t>pointsEarned</t>
+  </si>
+  <si>
+    <t>AmountSpent</t>
+  </si>
+  <si>
+    <t>PromotionPlanCode</t>
+  </si>
+  <si>
+    <t>TC1LoyaltyPlanCreation</t>
+  </si>
+  <si>
+    <t>LOYALTYAUTOMATION</t>
+  </si>
+  <si>
+    <t>LoyaltyPlanSetup</t>
+  </si>
+  <si>
+    <t>USD [840]</t>
+  </si>
+  <si>
+    <t>15000</t>
+  </si>
+  <si>
+    <t>Year [Y]</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>1500</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Day of Month [0]</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Miss. [3]</t>
+  </si>
+  <si>
+    <t>ABCDDD</t>
+  </si>
+  <si>
+    <t>aaaaa</t>
+  </si>
+  <si>
+    <t>Male [M]</t>
+  </si>
+  <si>
+    <t>ABCDEF</t>
+  </si>
+  <si>
+    <t>General purpose [GP]</t>
+  </si>
+  <si>
+    <t>Atul.Upadhyay@mastercard.com</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>1010</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>20000</t>
+  </si>
+  <si>
+    <t>promotionPlanDescription</t>
+  </si>
+  <si>
+    <t>June/27/2020</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>100000000</t>
+  </si>
+  <si>
+    <t>Miscellaneous Debit [70]</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>OfficeBranch2 [206]</t>
+  </si>
+  <si>
+    <t>800</t>
+  </si>
+  <si>
+    <t>100000</t>
+  </si>
+  <si>
+    <t>PROMOTIONPLAN</t>
+  </si>
+  <si>
+    <t>TC264328_Embossing File Generation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://stage.sa.eis.customer.mastercard.com/mpts/eis/app/
+</t>
+  </si>
+  <si>
+    <t>1000000100000</t>
+  </si>
+  <si>
+    <t>1000000199999</t>
+  </si>
+  <si>
+    <t>111</t>
   </si>
 </sst>
 </file>
@@ -1622,7 +1855,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1678,12 +1911,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1749,6 +1993,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3868,8 +4130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3882,7 +4144,7 @@
     <col min="7" max="7" width="23.77734375" customWidth="1"/>
     <col min="8" max="8" width="26.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="11" width="23.77734375" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21" customWidth="1"/>
     <col min="13" max="13" width="30.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3973,12 +4235,811 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:ED2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="14.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:134" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>528</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="AH1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AI1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AK1" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL1" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="AN1" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="AO1" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="AP1" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="AQ1" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="AR1" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="AS1" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AT1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AV1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AW1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AX1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AY1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AZ1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="BC1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="BD1" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="BE1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="BF1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="BG1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="BH1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="BI1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="BJ1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="BK1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="BL1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="BM1" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="BN1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="BO1" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="BP1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="BQ1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="BR1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="BS1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="BT1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="BU1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="BV1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="BW1" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="BX1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="BY1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="BZ1" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="CA1" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="CB1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="CC1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="CD1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="CE1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="CF1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="CG1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="CH1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="CI1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="CJ1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="CK1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="CL1" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="CM1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="CN1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="CO1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="CP1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="CQ1" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="CR1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="CS1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="CT1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="CU1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="CV1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="CW1" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="CX1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="CY1" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="CZ1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="DA1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="DB1" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="DC1" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="DD1" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="DE1" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="DF1" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="DG1" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="DH1" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="DI1" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="DJ1" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="DK1" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="DL1" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="DM1" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="DN1" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="DO1" s="35" t="s">
+        <v>532</v>
+      </c>
+      <c r="DP1" s="35" t="s">
+        <v>533</v>
+      </c>
+      <c r="DQ1" s="35" t="s">
+        <v>534</v>
+      </c>
+      <c r="DR1" s="35" t="s">
+        <v>535</v>
+      </c>
+      <c r="DS1" s="35" t="s">
+        <v>536</v>
+      </c>
+      <c r="DT1" s="35" t="s">
+        <v>537</v>
+      </c>
+      <c r="DU1" s="35" t="s">
+        <v>538</v>
+      </c>
+      <c r="DV1" s="35" t="s">
+        <v>539</v>
+      </c>
+      <c r="DW1" s="35" t="s">
+        <v>540</v>
+      </c>
+      <c r="DX1" s="35" t="s">
+        <v>541</v>
+      </c>
+      <c r="DY1" s="35" t="s">
+        <v>542</v>
+      </c>
+      <c r="DZ1" s="35" t="s">
+        <v>543</v>
+      </c>
+      <c r="EA1" s="35" t="s">
+        <v>544</v>
+      </c>
+      <c r="EB1" s="35" t="s">
+        <v>545</v>
+      </c>
+      <c r="EC1" s="35" t="s">
+        <v>546</v>
+      </c>
+      <c r="ED1" s="35" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="2" spans="1:134" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>454</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>495</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>552</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="J2" s="37" t="s">
+        <v>554</v>
+      </c>
+      <c r="K2" s="37" t="s">
+        <v>555</v>
+      </c>
+      <c r="L2" s="37" t="s">
+        <v>556</v>
+      </c>
+      <c r="M2" s="27" t="s">
+        <v>557</v>
+      </c>
+      <c r="N2" s="27" t="s">
+        <v>558</v>
+      </c>
+      <c r="O2" s="27" t="s">
+        <v>558</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="Q2" s="27" t="s">
+        <v>560</v>
+      </c>
+      <c r="R2" s="27" t="s">
+        <v>509</v>
+      </c>
+      <c r="S2" s="27" t="s">
+        <v>393</v>
+      </c>
+      <c r="T2" s="11">
+        <v>50</v>
+      </c>
+      <c r="U2" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="V2" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="W2" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="X2" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y2" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z2" s="38"/>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="13"/>
+      <c r="AC2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="11" t="s">
+        <v>561</v>
+      </c>
+      <c r="AF2" s="13" t="s">
+        <v>562</v>
+      </c>
+      <c r="AG2" s="13" t="s">
+        <v>563</v>
+      </c>
+      <c r="AH2" s="13" t="s">
+        <v>564</v>
+      </c>
+      <c r="AI2" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ2" s="13">
+        <v>1989</v>
+      </c>
+      <c r="AK2" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL2" s="15">
+        <v>12345678</v>
+      </c>
+      <c r="AM2" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="AN2" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="AO2" s="13" t="s">
+        <v>565</v>
+      </c>
+      <c r="AP2" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="AQ2" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="AR2" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="AS2" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AT2" s="11"/>
+      <c r="AU2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="AV2" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="AW2" s="11">
+        <v>1</v>
+      </c>
+      <c r="AX2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="AY2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="AZ2" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="BA2" s="13">
+        <v>1</v>
+      </c>
+      <c r="BB2" s="13" t="s">
+        <v>566</v>
+      </c>
+      <c r="BC2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="BD2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="BE2" s="13">
+        <v>12</v>
+      </c>
+      <c r="BF2" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="BG2" s="13">
+        <v>2</v>
+      </c>
+      <c r="BH2" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="BI2" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="BJ2" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="BK2" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="BL2" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="BM2" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="BN2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="BO2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="BP2" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="BQ2" s="25" t="s">
+        <v>362</v>
+      </c>
+      <c r="BR2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="BS2" s="13">
+        <v>12345678</v>
+      </c>
+      <c r="BT2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="BU2" s="13">
+        <v>12345678</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>567</v>
+      </c>
+      <c r="BW2" s="39"/>
+      <c r="BX2" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BY2" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="BZ2" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="CA2" s="13" t="s">
+        <v>466</v>
+      </c>
+      <c r="CB2" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="CC2" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="CD2" s="13" t="s">
+        <v>449</v>
+      </c>
+      <c r="CE2" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="CF2" s="39" t="s">
+        <v>568</v>
+      </c>
+      <c r="CG2" s="39" t="s">
+        <v>569</v>
+      </c>
+      <c r="CH2" s="13"/>
+      <c r="CI2" s="38"/>
+      <c r="CJ2" s="38"/>
+      <c r="CK2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="CL2" s="39" t="s">
+        <v>570</v>
+      </c>
+      <c r="CM2" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="CN2" s="11" t="s">
+        <v>364</v>
+      </c>
+      <c r="CO2" s="38" t="s">
+        <v>571</v>
+      </c>
+      <c r="CP2" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="CQ2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="CR2" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="CS2" s="11"/>
+      <c r="CT2" s="11"/>
+      <c r="CU2" s="38" t="s">
+        <v>558</v>
+      </c>
+      <c r="CV2" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="CW2" s="38" t="s">
+        <v>572</v>
+      </c>
+      <c r="CX2" s="38" t="s">
+        <v>568</v>
+      </c>
+      <c r="CY2" s="38" t="s">
+        <v>573</v>
+      </c>
+      <c r="CZ2" s="38" t="s">
+        <v>574</v>
+      </c>
+      <c r="DA2" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="DB2" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="DC2" s="13"/>
+      <c r="DD2" s="13"/>
+      <c r="DE2" s="13"/>
+      <c r="DF2" s="13"/>
+      <c r="DG2" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="DH2" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="DI2" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="DJ2" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="DK2" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="DL2" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="DM2" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="DN2" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="DO2" s="40" t="s">
+        <v>575</v>
+      </c>
+      <c r="DP2" s="40" t="s">
+        <v>576</v>
+      </c>
+      <c r="DQ2" s="40" t="s">
+        <v>577</v>
+      </c>
+      <c r="DR2" s="41" t="s">
+        <v>578</v>
+      </c>
+      <c r="DS2" s="41" t="s">
+        <v>568</v>
+      </c>
+      <c r="DT2" s="41" t="s">
+        <v>579</v>
+      </c>
+      <c r="DU2" s="40" t="s">
+        <v>580</v>
+      </c>
+      <c r="DV2" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="DW2" s="41" t="s">
+        <v>514</v>
+      </c>
+      <c r="DX2" s="41" t="s">
+        <v>581</v>
+      </c>
+      <c r="DY2" s="41" t="s">
+        <v>582</v>
+      </c>
+      <c r="DZ2" s="41" t="s">
+        <v>556</v>
+      </c>
+      <c r="EA2" s="41" t="s">
+        <v>583</v>
+      </c>
+      <c r="EB2" s="41" t="s">
+        <v>584</v>
+      </c>
+      <c r="EC2" s="41" t="s">
+        <v>585</v>
+      </c>
+      <c r="ED2" s="40" t="s">
+        <v>586</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CV177"/>
+  <dimension ref="A1:CV9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AS1" sqref="AS1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3990,6 +5051,7 @@
     <col min="7" max="7" width="11.109375" customWidth="1"/>
     <col min="8" max="8" width="17.44140625" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" customWidth="1"/>
     <col min="22" max="22" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="7.44140625" customWidth="1"/>
     <col min="69" max="69" width="14.109375" bestFit="1" customWidth="1"/>
@@ -6009,806 +7071,585 @@
         <v>255</v>
       </c>
     </row>
-    <row r="8" spans="1:100" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>371</v>
+    <row r="8" spans="1:100" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>587</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>588</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>361</v>
+        <v>509</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>354</v>
+        <v>393</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>372</v>
-      </c>
-      <c r="F8" s="2">
+        <v>495</v>
+      </c>
+      <c r="F8" s="11">
         <v>50</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="G8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="L8" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="O8" s="2" t="s">
+      <c r="L8" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="N8" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="O8" s="11" t="s">
         <v>259</v>
       </c>
-      <c r="P8" s="3" t="s">
+      <c r="P8" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="Q8" s="3" t="s">
+      <c r="Q8" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="R8" s="3" t="s">
+      <c r="R8" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="S8" s="3" t="s">
+      <c r="S8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="T8" s="3">
+      <c r="T8" s="13">
         <v>1989</v>
       </c>
-      <c r="U8" s="3" t="s">
+      <c r="U8" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="V8" s="16">
+      <c r="V8" s="15">
         <v>12345678</v>
       </c>
-      <c r="W8" s="3" t="s">
+      <c r="W8" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="X8" s="3" t="s">
+      <c r="X8" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="Y8" s="3" t="s">
+      <c r="Y8" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="Z8" s="3" t="s">
+      <c r="Z8" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="AA8" s="3" t="s">
+      <c r="AA8" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="AB8" s="3" t="s">
+      <c r="AB8" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="AC8" s="3" t="s">
+      <c r="AC8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="AD8" s="2">
-        <v>777</v>
-      </c>
-      <c r="AE8" s="2" t="s">
+      <c r="AD8" s="26" t="s">
+        <v>591</v>
+      </c>
+      <c r="AE8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="AF8" s="3" t="s">
+      <c r="AF8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="AG8" s="2">
+      <c r="AG8" s="11">
         <v>1</v>
       </c>
-      <c r="AH8" s="3" t="s">
+      <c r="AH8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="AI8" s="3" t="s">
+      <c r="AI8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="AJ8" s="3" t="s">
+      <c r="AJ8" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="AK8" s="3">
+      <c r="AK8" s="13">
         <v>1</v>
       </c>
-      <c r="AL8" s="3" t="s">
+      <c r="AL8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="AM8" s="3" t="s">
+      <c r="AM8" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="AN8" s="3">
+      <c r="AN8" s="13">
         <v>12</v>
       </c>
-      <c r="AO8" s="3" t="s">
+      <c r="AO8" s="13" t="s">
         <v>364</v>
       </c>
-      <c r="AP8" s="3">
+      <c r="AP8" s="13">
         <v>2</v>
       </c>
-      <c r="AQ8" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="AR8" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="AS8" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="AT8" s="3" t="s">
+      <c r="AQ8" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="AR8" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="AS8" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="AT8" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AU8" s="3" t="s">
+      <c r="AU8" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="AV8" s="3" t="s">
+      <c r="AV8" s="13" t="s">
         <v>206</v>
       </c>
-      <c r="AW8" s="3" t="s">
+      <c r="AW8" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="AX8" s="3" t="s">
+      <c r="AX8" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="AY8" s="3" t="s">
+      <c r="AY8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="AZ8" s="25">
-        <v>411006</v>
-      </c>
-      <c r="BA8" s="3" t="s">
+      <c r="AZ8" s="25" t="s">
+        <v>362</v>
+      </c>
+      <c r="BA8" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="BB8" s="3">
+      <c r="BB8" s="13">
         <v>12345678</v>
       </c>
-      <c r="BC8" s="3" t="s">
+      <c r="BC8" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="BD8" s="3">
+      <c r="BD8" s="13">
         <v>12345678</v>
       </c>
-      <c r="BE8" s="3" t="s">
+      <c r="BE8" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="BF8" s="3">
-        <v>777</v>
-      </c>
-      <c r="BG8" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="BH8" s="3" t="s">
+      <c r="BF8" s="13">
+        <v>111</v>
+      </c>
+      <c r="BG8" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="BH8" s="13" t="s">
         <v>364</v>
       </c>
-      <c r="BI8" s="3" t="s">
+      <c r="BI8" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="BJ8" s="3" t="s">
+      <c r="BJ8" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="BK8" s="3" t="s">
+      <c r="BK8" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="BL8" s="3" t="s">
+      <c r="BL8" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="BM8" s="3" t="s">
+      <c r="BM8" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="BN8" s="3">
+      <c r="BN8" s="13">
         <v>12</v>
       </c>
-      <c r="BO8" s="3">
+      <c r="BO8" s="13">
         <v>26</v>
       </c>
-      <c r="BP8" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="BQ8" s="12">
-        <v>1000000700000</v>
-      </c>
-      <c r="BR8" s="12">
-        <v>1000000799999</v>
-      </c>
-      <c r="BS8" s="2" t="s">
+      <c r="BP8" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="BQ8" s="38" t="s">
+        <v>589</v>
+      </c>
+      <c r="BR8" s="38" t="s">
+        <v>590</v>
+      </c>
+      <c r="BS8" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="BT8" s="3">
-        <v>7777</v>
-      </c>
-      <c r="BU8" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="BV8" s="2" t="s">
+      <c r="BT8" s="39" t="s">
+        <v>570</v>
+      </c>
+      <c r="BU8" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="BV8" s="11" t="s">
         <v>364</v>
       </c>
-      <c r="BW8" s="2">
+      <c r="BW8" s="11">
         <v>2</v>
       </c>
-      <c r="BX8" s="2" t="s">
+      <c r="BX8" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="BY8" s="2" t="s">
+      <c r="BY8" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="BZ8" s="9" t="s">
+      <c r="BZ8" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="CA8" s="9"/>
-      <c r="CB8" s="9"/>
-      <c r="CC8" s="11">
-        <v>100</v>
-      </c>
-      <c r="CD8" s="11" t="s">
+      <c r="CA8" s="11"/>
+      <c r="CB8" s="11"/>
+      <c r="CC8" s="38" t="s">
+        <v>558</v>
+      </c>
+      <c r="CD8" s="13" t="s">
         <v>130</v>
       </c>
       <c r="CE8" s="11">
         <v>10000</v>
       </c>
-      <c r="CF8" s="11">
-        <v>12</v>
-      </c>
-      <c r="CG8" s="11">
-        <v>5000</v>
-      </c>
-      <c r="CH8" s="11">
-        <v>20000</v>
+      <c r="CF8" s="38" t="s">
+        <v>568</v>
+      </c>
+      <c r="CG8" s="38" t="s">
+        <v>573</v>
+      </c>
+      <c r="CH8" s="38" t="s">
+        <v>574</v>
       </c>
       <c r="CI8" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="CJ8" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="CK8" s="13">
-        <v>10000</v>
-      </c>
-      <c r="CL8" s="13">
-        <v>50000</v>
-      </c>
-      <c r="CM8" s="13">
-        <v>12</v>
-      </c>
-      <c r="CN8" s="11">
-        <v>120345</v>
-      </c>
+      <c r="CJ8" s="2"/>
+      <c r="CK8" s="13"/>
+      <c r="CL8" s="13"/>
+      <c r="CM8" s="13"/>
+      <c r="CN8" s="13"/>
       <c r="CO8" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="CP8" s="13" t="s">
+      <c r="CP8" s="11" t="s">
         <v>160</v>
       </c>
       <c r="CQ8" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="CR8" s="13"/>
-      <c r="CS8" s="13"/>
+      <c r="CR8" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="CS8" s="11" t="s">
+        <v>200</v>
+      </c>
       <c r="CT8" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="CU8" s="15"/>
-      <c r="CV8" s="13" t="s">
+      <c r="CU8" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="CV8" s="11" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="9" spans="1:100" x14ac:dyDescent="0.3">
-      <c r="B9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="CV9"/>
-    </row>
-    <row r="10" spans="1:100" x14ac:dyDescent="0.3">
-      <c r="CV10"/>
-    </row>
-    <row r="11" spans="1:100" x14ac:dyDescent="0.3">
-      <c r="CV11"/>
-    </row>
-    <row r="12" spans="1:100" x14ac:dyDescent="0.3">
-      <c r="CV12"/>
-    </row>
-    <row r="13" spans="1:100" x14ac:dyDescent="0.3">
-      <c r="CV13"/>
-    </row>
-    <row r="14" spans="1:100" x14ac:dyDescent="0.3">
-      <c r="CV14"/>
-    </row>
-    <row r="15" spans="1:100" x14ac:dyDescent="0.3">
-      <c r="CV15"/>
-    </row>
-    <row r="16" spans="1:100" x14ac:dyDescent="0.3">
-      <c r="CV16"/>
-    </row>
-    <row r="17" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV17"/>
-    </row>
-    <row r="18" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV18"/>
-    </row>
-    <row r="19" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV19"/>
-    </row>
-    <row r="20" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV20"/>
-    </row>
-    <row r="21" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV21"/>
-    </row>
-    <row r="22" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV22"/>
-    </row>
-    <row r="23" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV23"/>
-    </row>
-    <row r="24" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV24"/>
-    </row>
-    <row r="25" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV25"/>
-    </row>
-    <row r="26" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV26"/>
-    </row>
-    <row r="27" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV27"/>
-    </row>
-    <row r="28" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV28"/>
-    </row>
-    <row r="29" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV29"/>
-    </row>
-    <row r="30" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV30"/>
-    </row>
-    <row r="31" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV31"/>
-    </row>
-    <row r="32" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV32"/>
-    </row>
-    <row r="33" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV33"/>
-    </row>
-    <row r="34" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV34"/>
-    </row>
-    <row r="35" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV35"/>
-    </row>
-    <row r="36" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV36"/>
-    </row>
-    <row r="37" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV37"/>
-    </row>
-    <row r="38" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV38"/>
-    </row>
-    <row r="39" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV39"/>
-    </row>
-    <row r="40" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV40"/>
-    </row>
-    <row r="41" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV41"/>
-    </row>
-    <row r="42" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV42"/>
-    </row>
-    <row r="43" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV43"/>
-    </row>
-    <row r="44" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV44"/>
-    </row>
-    <row r="45" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV45"/>
-    </row>
-    <row r="46" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV46"/>
-    </row>
-    <row r="47" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV47"/>
-    </row>
-    <row r="48" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV48"/>
-    </row>
-    <row r="49" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV49"/>
-    </row>
-    <row r="50" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV50"/>
-    </row>
-    <row r="51" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV51"/>
-    </row>
-    <row r="52" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV52"/>
-    </row>
-    <row r="53" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV53"/>
-    </row>
-    <row r="54" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV54"/>
-    </row>
-    <row r="55" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV55"/>
-    </row>
-    <row r="56" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV56"/>
-    </row>
-    <row r="57" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV57"/>
-    </row>
-    <row r="58" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV58"/>
-    </row>
-    <row r="59" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV59"/>
-    </row>
-    <row r="60" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV60"/>
-    </row>
-    <row r="61" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV61"/>
-    </row>
-    <row r="62" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV62"/>
-    </row>
-    <row r="63" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV63"/>
-    </row>
-    <row r="64" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV64"/>
-    </row>
-    <row r="65" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV65"/>
-    </row>
-    <row r="66" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV66"/>
-    </row>
-    <row r="67" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV67"/>
-    </row>
-    <row r="68" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV68"/>
-    </row>
-    <row r="69" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV69"/>
-    </row>
-    <row r="70" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV70"/>
-    </row>
-    <row r="71" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV71"/>
-    </row>
-    <row r="72" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV72"/>
-    </row>
-    <row r="73" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV73"/>
-    </row>
-    <row r="74" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV74"/>
-    </row>
-    <row r="75" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV75"/>
-    </row>
-    <row r="76" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV76"/>
-    </row>
-    <row r="77" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV77"/>
-    </row>
-    <row r="78" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV78"/>
-    </row>
-    <row r="79" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV79"/>
-    </row>
-    <row r="80" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV80"/>
-    </row>
-    <row r="81" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV81"/>
-    </row>
-    <row r="82" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV82"/>
-    </row>
-    <row r="83" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV83"/>
-    </row>
-    <row r="84" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV84"/>
-    </row>
-    <row r="85" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV85"/>
-    </row>
-    <row r="86" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV86"/>
-    </row>
-    <row r="87" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV87"/>
-    </row>
-    <row r="88" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV88"/>
-    </row>
-    <row r="89" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV89"/>
-    </row>
-    <row r="90" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV90"/>
-    </row>
-    <row r="91" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV91"/>
-    </row>
-    <row r="92" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV92"/>
-    </row>
-    <row r="93" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV93"/>
-    </row>
-    <row r="94" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV94"/>
-    </row>
-    <row r="95" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV95"/>
-    </row>
-    <row r="96" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV96"/>
-    </row>
-    <row r="97" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV97"/>
-    </row>
-    <row r="98" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV98"/>
-    </row>
-    <row r="99" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV99"/>
-    </row>
-    <row r="100" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV100"/>
-    </row>
-    <row r="101" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV101"/>
-    </row>
-    <row r="102" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV102"/>
-    </row>
-    <row r="103" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV103"/>
-    </row>
-    <row r="104" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV104"/>
-    </row>
-    <row r="105" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV105"/>
-    </row>
-    <row r="106" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV106"/>
-    </row>
-    <row r="107" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV107"/>
-    </row>
-    <row r="108" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV108"/>
-    </row>
-    <row r="109" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV109"/>
-    </row>
-    <row r="110" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV110"/>
-    </row>
-    <row r="111" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV111"/>
-    </row>
-    <row r="112" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV112"/>
-    </row>
-    <row r="113" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV113"/>
-    </row>
-    <row r="114" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV114"/>
-    </row>
-    <row r="115" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV115"/>
-    </row>
-    <row r="116" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV116"/>
-    </row>
-    <row r="117" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV117"/>
-    </row>
-    <row r="118" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV118"/>
-    </row>
-    <row r="119" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV119"/>
-    </row>
-    <row r="120" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV120"/>
-    </row>
-    <row r="121" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV121"/>
-    </row>
-    <row r="122" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV122"/>
-    </row>
-    <row r="123" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV123"/>
-    </row>
-    <row r="124" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV124"/>
-    </row>
-    <row r="125" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV125"/>
-    </row>
-    <row r="126" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV126"/>
-    </row>
-    <row r="127" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV127"/>
-    </row>
-    <row r="128" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV128"/>
-    </row>
-    <row r="129" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV129"/>
-    </row>
-    <row r="130" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV130"/>
-    </row>
-    <row r="131" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV131"/>
-    </row>
-    <row r="132" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV132"/>
-    </row>
-    <row r="133" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV133"/>
-    </row>
-    <row r="134" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV134"/>
-    </row>
-    <row r="135" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV135"/>
-    </row>
-    <row r="136" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV136"/>
-    </row>
-    <row r="137" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV137"/>
-    </row>
-    <row r="138" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV138"/>
-    </row>
-    <row r="139" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV139"/>
-    </row>
-    <row r="140" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV140"/>
-    </row>
-    <row r="141" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV141"/>
-    </row>
-    <row r="142" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV142"/>
-    </row>
-    <row r="143" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV143"/>
-    </row>
-    <row r="144" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV144"/>
-    </row>
-    <row r="145" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV145"/>
-    </row>
-    <row r="146" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV146"/>
-    </row>
-    <row r="147" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV147"/>
-    </row>
-    <row r="148" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV148"/>
-    </row>
-    <row r="149" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV149"/>
-    </row>
-    <row r="150" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV150"/>
-    </row>
-    <row r="151" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV151"/>
-    </row>
-    <row r="152" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV152"/>
-    </row>
-    <row r="153" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV153"/>
-    </row>
-    <row r="154" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV154"/>
-    </row>
-    <row r="155" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV155"/>
-    </row>
-    <row r="156" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV156"/>
-    </row>
-    <row r="157" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV157"/>
-    </row>
-    <row r="158" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV158"/>
-    </row>
-    <row r="159" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV159"/>
-    </row>
-    <row r="160" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV160"/>
-    </row>
-    <row r="161" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV161"/>
-    </row>
-    <row r="162" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV162"/>
-    </row>
-    <row r="163" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV163"/>
-    </row>
-    <row r="164" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV164"/>
-    </row>
-    <row r="165" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV165"/>
-    </row>
-    <row r="166" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV166"/>
-    </row>
-    <row r="167" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV167"/>
-    </row>
-    <row r="168" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV168"/>
-    </row>
-    <row r="169" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV169"/>
-    </row>
-    <row r="170" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV170"/>
-    </row>
-    <row r="171" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV171"/>
-    </row>
-    <row r="172" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV172"/>
-    </row>
-    <row r="173" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV173"/>
-    </row>
-    <row r="174" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV174"/>
-    </row>
-    <row r="175" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV175"/>
-    </row>
-    <row r="176" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV176"/>
-    </row>
-    <row r="177" spans="100:100" x14ac:dyDescent="0.3">
-      <c r="CV177"/>
+    <row r="9" spans="1:100" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>371</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>354</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>372</v>
+      </c>
+      <c r="F9" s="2">
+        <v>50</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="N9" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="T9" s="3">
+        <v>1989</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="V9" s="16">
+        <v>12345678</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z9" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA9" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="AB9" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AC9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD9" s="2">
+        <v>777</v>
+      </c>
+      <c r="AE9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG9" s="2">
+        <v>1</v>
+      </c>
+      <c r="AH9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK9" s="3">
+        <v>1</v>
+      </c>
+      <c r="AL9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AM9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AN9" s="3">
+        <v>12</v>
+      </c>
+      <c r="AO9" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="AP9" s="3">
+        <v>2</v>
+      </c>
+      <c r="AQ9" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="AR9" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="AS9" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="AT9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AU9" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="AV9" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="AW9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AX9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AY9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AZ9" s="25">
+        <v>411006</v>
+      </c>
+      <c r="BA9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="BB9" s="3">
+        <v>12345678</v>
+      </c>
+      <c r="BC9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="BD9" s="3">
+        <v>12345678</v>
+      </c>
+      <c r="BE9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="BF9" s="3">
+        <v>777</v>
+      </c>
+      <c r="BG9" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="BH9" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="BI9" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="BJ9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="BK9" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="BL9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="BM9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="BN9" s="3">
+        <v>12</v>
+      </c>
+      <c r="BO9" s="3">
+        <v>26</v>
+      </c>
+      <c r="BP9" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="BQ9" s="12">
+        <v>1000000700000</v>
+      </c>
+      <c r="BR9" s="12">
+        <v>1000000799999</v>
+      </c>
+      <c r="BS9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="BT9" s="3">
+        <v>7777</v>
+      </c>
+      <c r="BU9" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="BV9" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="BW9" s="2">
+        <v>2</v>
+      </c>
+      <c r="BX9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="BY9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="BZ9" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="CA9" s="9"/>
+      <c r="CB9" s="9"/>
+      <c r="CC9" s="11">
+        <v>100</v>
+      </c>
+      <c r="CD9" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="CE9" s="11">
+        <v>10000</v>
+      </c>
+      <c r="CF9" s="11">
+        <v>12</v>
+      </c>
+      <c r="CG9" s="11">
+        <v>5000</v>
+      </c>
+      <c r="CH9" s="11">
+        <v>20000</v>
+      </c>
+      <c r="CI9" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="CJ9" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="CK9" s="13">
+        <v>10000</v>
+      </c>
+      <c r="CL9" s="13">
+        <v>50000</v>
+      </c>
+      <c r="CM9" s="13">
+        <v>12</v>
+      </c>
+      <c r="CN9" s="11">
+        <v>120345</v>
+      </c>
+      <c r="CO9" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="CP9" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="CQ9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="CR9" s="13"/>
+      <c r="CS9" s="13"/>
+      <c r="CT9" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="CU9" s="15"/>
+      <c r="CV9" s="13" t="s">
+        <v>255</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Institution setup Stage changes
</commit_message>
<xml_diff>
--- a/src/main/resources/config/stageSA/TestData/TestData.xlsx
+++ b/src/main/resources/config/stageSA/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15105" windowHeight="8985" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15105" windowHeight="8985" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="S181372" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1974" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2042" uniqueCount="551">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1286,9 +1286,6 @@
     <t>BIN</t>
   </si>
   <si>
-    <t>Custom Code</t>
-  </si>
-  <si>
     <t>Product Currency</t>
   </si>
   <si>
@@ -1479,6 +1476,210 @@
   </si>
   <si>
     <t>WIBMO [002]</t>
+  </si>
+  <si>
+    <t>4656</t>
+  </si>
+  <si>
+    <t>iPKExpiryDate</t>
+  </si>
+  <si>
+    <t>GeneralisationMethod</t>
+  </si>
+  <si>
+    <t>PINlength</t>
+  </si>
+  <si>
+    <t>PVVOffset</t>
+  </si>
+  <si>
+    <t>PVKOffset</t>
+  </si>
+  <si>
+    <t>PINValidationData</t>
+  </si>
+  <si>
+    <t>PINVerificationKey</t>
+  </si>
+  <si>
+    <t>PINVerificationKeyCheck</t>
+  </si>
+  <si>
+    <t>CVVOffsetOnTrack</t>
+  </si>
+  <si>
+    <t>ComponentType</t>
+  </si>
+  <si>
+    <t>CVKACryptogram</t>
+  </si>
+  <si>
+    <t>CVKAKeyCheck</t>
+  </si>
+  <si>
+    <t>CVKBCryptogram</t>
+  </si>
+  <si>
+    <t>CVKBKeyCheck</t>
+  </si>
+  <si>
+    <t>CVV3Cryptogram</t>
+  </si>
+  <si>
+    <t>CVV3KeyCheckvalue</t>
+  </si>
+  <si>
+    <t>ATCOffsetOnTrack</t>
+  </si>
+  <si>
+    <t>UNOffsetOnTrack</t>
+  </si>
+  <si>
+    <t>CVC3OffsetOnTrack</t>
+  </si>
+  <si>
+    <t>NetworkInterface</t>
+  </si>
+  <si>
+    <t>KeyType</t>
+  </si>
+  <si>
+    <t>NetworkCryptogram</t>
+  </si>
+  <si>
+    <t>NetworkCryptogramCheckValue</t>
+  </si>
+  <si>
+    <t>MDKEncryptedUnderLMK</t>
+  </si>
+  <si>
+    <t>MDKKeyCheckValue</t>
+  </si>
+  <si>
+    <t>SMIEncryptedUnderLMKTxt</t>
+  </si>
+  <si>
+    <t>SMIKeyCheckvalues</t>
+  </si>
+  <si>
+    <t>SMCEncryptedUnderLMKTxt</t>
+  </si>
+  <si>
+    <t>SMCKeyCheckvalue</t>
+  </si>
+  <si>
+    <t>MDKKeyType</t>
+  </si>
+  <si>
+    <t>MDKInterchangeType</t>
+  </si>
+  <si>
+    <t>MDKStatus</t>
+  </si>
+  <si>
+    <t>March/10/2050</t>
+  </si>
+  <si>
+    <t>IBM Method [3]</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>1234567890123456</t>
+  </si>
+  <si>
+    <t>181CFD03C3F7385FCA36BF63DDD4BD01</t>
+  </si>
+  <si>
+    <t>829DD2</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>1-Single Component [1]</t>
+  </si>
+  <si>
+    <t>4A43436017024880</t>
+  </si>
+  <si>
+    <t>0EBBE7</t>
+  </si>
+  <si>
+    <t>B4638CBCEC1E6E52</t>
+  </si>
+  <si>
+    <t>985BDD</t>
+  </si>
+  <si>
+    <t>7B634E89DB88BBD9BB33C702FD1C9151</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>MasterCard(CIS) [03]</t>
+  </si>
+  <si>
+    <t>ZMK [6]</t>
+  </si>
+  <si>
+    <t>80F5706D510BF6F7D54D6DA3053CAB8A</t>
+  </si>
+  <si>
+    <t>2A7944</t>
+  </si>
+  <si>
+    <t>E60699F5B9ADE145FF6B0281D6FF7A71</t>
+  </si>
+  <si>
+    <t>2BC1FE</t>
+  </si>
+  <si>
+    <t>3B84D3C46E096114BF1A505A548A88AE</t>
+  </si>
+  <si>
+    <t>55AF3C</t>
+  </si>
+  <si>
+    <t>6B9D441DA33CF04F687C085A0CD9D8F8</t>
+  </si>
+  <si>
+    <t>9855B6</t>
+  </si>
+  <si>
+    <t>MDK Key [00]</t>
+  </si>
+  <si>
+    <t>MASTERCARD [02]</t>
+  </si>
+  <si>
+    <t>Active [0]</t>
+  </si>
+  <si>
+    <t>https://stage.sa.eis.customer.mastercard.com/mpts/eis/app</t>
+  </si>
+  <si>
+    <t>NidhiS</t>
+  </si>
+  <si>
+    <t>LANKA [111777]</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Sequence number</t>
+  </si>
+  <si>
+    <t>Program Code</t>
   </si>
 </sst>
 </file>
@@ -1616,7 +1817,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1688,6 +1889,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3495,15 +3699,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:DN177"/>
+  <dimension ref="A1:ES177"/>
   <sheetViews>
-    <sheetView topLeftCell="BN7" workbookViewId="0">
-      <selection activeCell="CH2" sqref="CH2:CH11"/>
+    <sheetView tabSelected="1" topLeftCell="CL1" workbookViewId="0">
+      <selection activeCell="CX2" sqref="CX2:CX3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="1" max="1" width="40.5703125" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" customWidth="1"/>
     <col min="4" max="4" width="11.140625" customWidth="1"/>
@@ -3516,7 +3720,7 @@
     <col min="97" max="97" width="10.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:118" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:149" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -3719,7 +3923,7 @@
         <v>70</v>
       </c>
       <c r="BP1" s="4" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="BQ1" s="4" t="s">
         <v>73</v>
@@ -3728,10 +3932,10 @@
         <v>74</v>
       </c>
       <c r="BS1" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="BT1" s="4" t="s">
         <v>422</v>
-      </c>
-      <c r="BT1" s="4" t="s">
-        <v>423</v>
       </c>
       <c r="BU1" s="4" t="s">
         <v>83</v>
@@ -3797,10 +4001,10 @@
         <v>89</v>
       </c>
       <c r="CP1" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="CQ1" s="4" t="s">
         <v>424</v>
-      </c>
-      <c r="CQ1" s="4" t="s">
-        <v>425</v>
       </c>
       <c r="CR1" s="1" t="s">
         <v>137</v>
@@ -3868,23 +4072,118 @@
       <c r="DM1" s="4" t="s">
         <v>415</v>
       </c>
-      <c r="DN1" s="4"/>
-    </row>
-    <row r="2" spans="1:118" ht="90" x14ac:dyDescent="0.25">
+      <c r="DN1" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="DO1" s="4" t="s">
+        <v>485</v>
+      </c>
+      <c r="DP1" s="4" t="s">
+        <v>486</v>
+      </c>
+      <c r="DQ1" s="4" t="s">
+        <v>487</v>
+      </c>
+      <c r="DR1" s="4" t="s">
+        <v>488</v>
+      </c>
+      <c r="DS1" s="4" t="s">
+        <v>489</v>
+      </c>
+      <c r="DT1" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="DU1" s="4" t="s">
+        <v>491</v>
+      </c>
+      <c r="DV1" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="DW1" s="4" t="s">
+        <v>493</v>
+      </c>
+      <c r="DX1" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="DY1" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="DZ1" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="EA1" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="EB1" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="EC1" s="4" t="s">
+        <v>499</v>
+      </c>
+      <c r="ED1" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="EE1" s="4" t="s">
+        <v>501</v>
+      </c>
+      <c r="EF1" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="EG1" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="EH1" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="EI1" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="EJ1" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="EK1" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="EL1" s="4" t="s">
+        <v>508</v>
+      </c>
+      <c r="EM1" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="EN1" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="EO1" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="EP1" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="EQ1" s="4" t="s">
+        <v>513</v>
+      </c>
+      <c r="ER1" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="ES1" s="4" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="2" spans="1:149" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>132</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>342</v>
+        <v>545</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>386</v>
+        <v>546</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>387</v>
+        <v>483</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>426</v>
+        <v>547</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>388</v>
@@ -4065,7 +4364,7 @@
         <v>71</v>
       </c>
       <c r="BP2" s="9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="BQ2" s="28" t="s">
         <v>393</v>
@@ -4074,7 +4373,7 @@
         <v>341</v>
       </c>
       <c r="BS2" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="BT2" s="9" t="s">
         <v>341</v>
@@ -4109,7 +4408,7 @@
       </c>
       <c r="CG2" s="36"/>
       <c r="CH2" s="28" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="CI2" s="38"/>
       <c r="CJ2" s="28" t="s">
@@ -4151,19 +4450,19 @@
         <v>188</v>
       </c>
       <c r="CX2" s="9" t="s">
-        <v>162</v>
+        <v>221</v>
       </c>
       <c r="CY2" s="9" t="s">
         <v>53</v>
       </c>
       <c r="CZ2" s="9" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="DA2" s="9" t="s">
         <v>416</v>
       </c>
       <c r="DB2" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="DC2" s="9" t="s">
         <v>393</v>
@@ -4178,33 +4477,129 @@
         <v>418</v>
       </c>
       <c r="DG2" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="DH2" s="9" t="s">
+        <v>549</v>
+      </c>
+      <c r="DI2" s="9" t="s">
+        <v>548</v>
+      </c>
+      <c r="DJ2" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="DK2" s="36" t="s">
+        <v>431</v>
+      </c>
+      <c r="DL2" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="DM2" s="9" t="s">
         <v>432</v>
       </c>
-      <c r="DH2" s="9" t="s">
-        <v>419</v>
-      </c>
-      <c r="DI2" s="9" t="s">
-        <v>341</v>
-      </c>
-      <c r="DJ2" s="9" t="s">
-        <v>192</v>
-      </c>
-      <c r="DK2" s="9" t="s">
+      <c r="DN2" s="9" t="s">
+        <v>516</v>
+      </c>
+      <c r="DO2" s="9" t="s">
+        <v>517</v>
+      </c>
+      <c r="DP2" s="32" t="s">
+        <v>518</v>
+      </c>
+      <c r="DQ2" s="32" t="s">
+        <v>519</v>
+      </c>
+      <c r="DR2" s="32" t="s">
+        <v>520</v>
+      </c>
+      <c r="DS2" s="39" t="s">
+        <v>521</v>
+      </c>
+      <c r="DT2" s="39" t="s">
+        <v>522</v>
+      </c>
+      <c r="DU2" s="39" t="s">
+        <v>523</v>
+      </c>
+      <c r="DV2" s="39" t="s">
+        <v>524</v>
+      </c>
+      <c r="DW2" s="39" t="s">
+        <v>525</v>
+      </c>
+      <c r="DX2" s="39" t="s">
+        <v>526</v>
+      </c>
+      <c r="DY2" s="39" t="s">
+        <v>527</v>
+      </c>
+      <c r="DZ2" s="39" t="s">
+        <v>528</v>
+      </c>
+      <c r="EA2" s="39" t="s">
+        <v>529</v>
+      </c>
+      <c r="EB2" s="39" t="s">
+        <v>530</v>
+      </c>
+      <c r="EC2" s="39" t="s">
+        <v>531</v>
+      </c>
+      <c r="ED2" s="39" t="s">
         <v>392</v>
       </c>
-      <c r="DL2" s="9" t="s">
-        <v>420</v>
-      </c>
-      <c r="DM2" s="9" t="s">
+      <c r="EE2" s="39" t="s">
+        <v>392</v>
+      </c>
+      <c r="EF2" s="39" t="s">
+        <v>392</v>
+      </c>
+      <c r="EG2" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="EH2" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="EI2" s="40" t="s">
+        <v>534</v>
+      </c>
+      <c r="EJ2" s="40" t="s">
+        <v>535</v>
+      </c>
+      <c r="EK2" s="40" t="s">
+        <v>536</v>
+      </c>
+      <c r="EL2" s="40" t="s">
+        <v>537</v>
+      </c>
+      <c r="EM2" s="40" t="s">
+        <v>538</v>
+      </c>
+      <c r="EN2" s="40" t="s">
+        <v>539</v>
+      </c>
+      <c r="EO2" s="40" t="s">
+        <v>540</v>
+      </c>
+      <c r="EP2" s="40" t="s">
+        <v>541</v>
+      </c>
+      <c r="EQ2" s="41" t="s">
+        <v>542</v>
+      </c>
+      <c r="ER2" s="41" t="s">
+        <v>543</v>
+      </c>
+      <c r="ES2" s="41" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="3" spans="1:149" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="3" spans="1:118" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>434</v>
-      </c>
       <c r="B3" s="9" t="s">
-        <v>342</v>
+        <v>545</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>386</v>
@@ -4213,7 +4608,7 @@
         <v>387</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>388</v>
@@ -4394,7 +4789,7 @@
         <v>71</v>
       </c>
       <c r="BP3" s="9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="BQ3" s="28" t="s">
         <v>393</v>
@@ -4403,7 +4798,7 @@
         <v>341</v>
       </c>
       <c r="BS3" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="BT3" s="9" t="s">
         <v>341</v>
@@ -4438,7 +4833,7 @@
       </c>
       <c r="CG3" s="36"/>
       <c r="CH3" s="28" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="CI3" s="38"/>
       <c r="CJ3" s="28" t="s">
@@ -4479,8 +4874,8 @@
       <c r="CW3" s="31" t="s">
         <v>188</v>
       </c>
-      <c r="CX3" s="31" t="s">
-        <v>162</v>
+      <c r="CX3" s="9" t="s">
+        <v>221</v>
       </c>
       <c r="CY3" s="31" t="s">
         <v>53</v>
@@ -4503,37 +4898,37 @@
       <c r="DE3" s="31" t="s">
         <v>417</v>
       </c>
-      <c r="DF3" s="31" t="s">
+      <c r="DF3" s="9" t="s">
         <v>418</v>
       </c>
-      <c r="DG3" s="31">
-        <v>6</v>
-      </c>
-      <c r="DH3" s="31" t="s">
+      <c r="DG3" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="DH3" s="9" t="s">
+        <v>549</v>
+      </c>
+      <c r="DI3" s="9" t="s">
+        <v>548</v>
+      </c>
+      <c r="DJ3" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="DK3" s="36" t="s">
+        <v>431</v>
+      </c>
+      <c r="DL3" s="9" t="s">
         <v>419</v>
       </c>
-      <c r="DI3" s="31">
-        <v>2</v>
-      </c>
-      <c r="DJ3" s="31" t="s">
-        <v>192</v>
-      </c>
-      <c r="DK3" s="31">
-        <v>1</v>
-      </c>
-      <c r="DL3" s="31" t="s">
-        <v>420</v>
-      </c>
-      <c r="DM3" s="31">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:118" ht="90" x14ac:dyDescent="0.25">
+      <c r="DM3" s="9" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="4" spans="1:149" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>140</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>342</v>
+        <v>545</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>386</v>
@@ -4542,7 +4937,7 @@
         <v>387</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>388</v>
@@ -4723,7 +5118,7 @@
         <v>71</v>
       </c>
       <c r="BP4" s="9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="BQ4" s="28" t="s">
         <v>393</v>
@@ -4732,7 +5127,7 @@
         <v>341</v>
       </c>
       <c r="BS4" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="BT4" s="9" t="s">
         <v>341</v>
@@ -4765,7 +5160,7 @@
       <c r="CF4" s="28"/>
       <c r="CG4" s="36"/>
       <c r="CH4" s="28" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="CI4" s="38"/>
       <c r="CJ4" s="28" t="s">
@@ -4829,12 +5224,12 @@
       <c r="DL4" s="31"/>
       <c r="DM4" s="31"/>
     </row>
-    <row r="5" spans="1:118" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:149" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>342</v>
+        <v>545</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>386</v>
@@ -4843,7 +5238,7 @@
         <v>387</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>388</v>
@@ -5024,7 +5419,7 @@
         <v>71</v>
       </c>
       <c r="BP5" s="9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="BQ5" s="28" t="s">
         <v>393</v>
@@ -5033,7 +5428,7 @@
         <v>341</v>
       </c>
       <c r="BS5" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="BT5" s="9" t="s">
         <v>341</v>
@@ -5066,7 +5461,7 @@
       <c r="CF5" s="28"/>
       <c r="CG5" s="36"/>
       <c r="CH5" s="28" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="CI5" s="38"/>
       <c r="CJ5" s="28" t="s">
@@ -5130,12 +5525,12 @@
       <c r="DL5" s="31"/>
       <c r="DM5" s="31"/>
     </row>
-    <row r="6" spans="1:118" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:149" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>150</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>342</v>
+        <v>545</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>386</v>
@@ -5144,7 +5539,7 @@
         <v>387</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>388</v>
@@ -5325,7 +5720,7 @@
         <v>71</v>
       </c>
       <c r="BP6" s="9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="BQ6" s="28" t="s">
         <v>393</v>
@@ -5334,7 +5729,7 @@
         <v>341</v>
       </c>
       <c r="BS6" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="BT6" s="9" t="s">
         <v>341</v>
@@ -5367,7 +5762,7 @@
       <c r="CF6" s="28"/>
       <c r="CG6" s="36"/>
       <c r="CH6" s="28" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="CI6" s="38"/>
       <c r="CJ6" s="28" t="s">
@@ -5431,12 +5826,12 @@
       <c r="DL6" s="31"/>
       <c r="DM6" s="31"/>
     </row>
-    <row r="7" spans="1:118" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:149" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>342</v>
+        <v>545</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>386</v>
@@ -5445,7 +5840,7 @@
         <v>387</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F7" s="9" t="s">
         <v>388</v>
@@ -5626,7 +6021,7 @@
         <v>71</v>
       </c>
       <c r="BP7" s="9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="BQ7" s="28" t="s">
         <v>393</v>
@@ -5635,7 +6030,7 @@
         <v>341</v>
       </c>
       <c r="BS7" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="BT7" s="9" t="s">
         <v>341</v>
@@ -5668,7 +6063,7 @@
       <c r="CF7" s="28"/>
       <c r="CG7" s="36"/>
       <c r="CH7" s="28" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="CI7" s="38"/>
       <c r="CJ7" s="28" t="s">
@@ -5732,12 +6127,12 @@
       <c r="DL7" s="31"/>
       <c r="DM7" s="31"/>
     </row>
-    <row r="8" spans="1:118" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:149" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>156</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>342</v>
+        <v>545</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>386</v>
@@ -5746,7 +6141,7 @@
         <v>387</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F8" s="9" t="s">
         <v>388</v>
@@ -5927,7 +6322,7 @@
         <v>71</v>
       </c>
       <c r="BP8" s="9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="BQ8" s="28" t="s">
         <v>393</v>
@@ -5936,7 +6331,7 @@
         <v>341</v>
       </c>
       <c r="BS8" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="BT8" s="9" t="s">
         <v>341</v>
@@ -5969,7 +6364,7 @@
       <c r="CF8" s="28"/>
       <c r="CG8" s="36"/>
       <c r="CH8" s="28" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="CI8" s="38"/>
       <c r="CJ8" s="28" t="s">
@@ -6033,12 +6428,12 @@
       <c r="DL8" s="31"/>
       <c r="DM8" s="31"/>
     </row>
-    <row r="9" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
-        <v>438</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>342</v>
+        <v>437</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>545</v>
       </c>
       <c r="C9" s="31">
         <v>455854</v>
@@ -6047,7 +6442,7 @@
         <v>8520</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F9" s="31">
         <v>50</v>
@@ -6334,12 +6729,12 @@
       <c r="DL9" s="31"/>
       <c r="DM9" s="31"/>
     </row>
-    <row r="10" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="B10" s="31" t="s">
-        <v>342</v>
+      <c r="B10" s="9" t="s">
+        <v>545</v>
       </c>
       <c r="C10" s="31">
         <v>455854</v>
@@ -6348,7 +6743,7 @@
         <v>8520</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F10" s="31">
         <v>50</v>
@@ -6635,12 +7030,12 @@
       <c r="DL10" s="31"/>
       <c r="DM10" s="31"/>
     </row>
-    <row r="11" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:149" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>439</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>342</v>
+        <v>438</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>545</v>
       </c>
       <c r="C11" s="31">
         <v>455854</v>
@@ -6649,7 +7044,7 @@
         <v>8520</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F11" s="31">
         <v>50</v>
@@ -6936,19 +7331,19 @@
       <c r="DL11" s="31"/>
       <c r="DM11" s="31"/>
     </row>
-    <row r="12" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:149" x14ac:dyDescent="0.25">
       <c r="CS12"/>
     </row>
-    <row r="13" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:149" x14ac:dyDescent="0.25">
       <c r="CS13"/>
     </row>
-    <row r="14" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:149" x14ac:dyDescent="0.25">
       <c r="CS14"/>
     </row>
-    <row r="15" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:149" x14ac:dyDescent="0.25">
       <c r="CS15"/>
     </row>
-    <row r="16" spans="1:118" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:149" x14ac:dyDescent="0.25">
       <c r="CS16"/>
     </row>
     <row r="17" spans="97:97" x14ac:dyDescent="0.25">
@@ -8268,7 +8663,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
@@ -8359,13 +8754,13 @@
         <v>205</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>441</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>442</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>206</v>
@@ -8455,42 +8850,42 @@
         <v>360</v>
       </c>
       <c r="AZ1" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="BA1" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>449</v>
-      </c>
-      <c r="BG1" s="1" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="2" spans="1:59" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
+        <v>450</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>451</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>452</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>453</v>
-      </c>
       <c r="D2" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>218</v>
@@ -8502,7 +8897,7 @@
         <v>218</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I2" s="9" t="s">
         <v>218</v>
@@ -8535,7 +8930,7 @@
         <v>16</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="T2" s="9" t="s">
         <v>218</v>
@@ -8595,7 +8990,7 @@
         <v>124421</v>
       </c>
       <c r="AM2" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AN2" s="9" t="s">
         <v>368</v>
@@ -8630,13 +9025,13 @@
         <v>367</v>
       </c>
       <c r="AZ2" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="BA2" s="9" t="s">
         <v>456</v>
       </c>
-      <c r="BA2" s="9" t="s">
+      <c r="BB2" s="9" t="s">
         <v>457</v>
-      </c>
-      <c r="BB2" s="9" t="s">
-        <v>458</v>
       </c>
       <c r="BC2" s="9"/>
       <c r="BD2" s="9"/>
@@ -8646,28 +9041,28 @@
     </row>
     <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
+        <v>458</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>459</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>460</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>218</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F3" s="28" t="s">
         <v>134</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>218</v>
@@ -8700,7 +9095,7 @@
         <v>16</v>
       </c>
       <c r="S3" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="T3" s="9" t="s">
         <v>218</v>
@@ -8760,7 +9155,7 @@
         <v>124421</v>
       </c>
       <c r="AM3" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AN3" s="9" t="s">
         <v>368</v>
@@ -8795,10 +9190,10 @@
         <v>367</v>
       </c>
       <c r="AZ3" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="BA3" s="9" t="s">
         <v>456</v>
-      </c>
-      <c r="BA3" s="9" t="s">
-        <v>457</v>
       </c>
       <c r="BB3" s="9"/>
       <c r="BC3" s="9"/>
@@ -8809,31 +9204,31 @@
     </row>
     <row r="4" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>460</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>461</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>462</v>
-      </c>
       <c r="C4" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>218</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F4" s="28" t="s">
         <v>134</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H4" s="9" t="s">
         <v>218</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>134</v>
@@ -8863,7 +9258,7 @@
         <v>16</v>
       </c>
       <c r="S4" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="T4" s="9" t="s">
         <v>218</v>
@@ -8923,7 +9318,7 @@
         <v>124421</v>
       </c>
       <c r="AM4" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AN4" s="9" t="s">
         <v>368</v>
@@ -8958,10 +9353,10 @@
         <v>367</v>
       </c>
       <c r="AZ4" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="BA4" s="9" t="s">
         <v>456</v>
-      </c>
-      <c r="BA4" s="9" t="s">
-        <v>457</v>
       </c>
       <c r="BB4" s="9"/>
       <c r="BC4" s="9"/>
@@ -8972,16 +9367,16 @@
     </row>
     <row r="5" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
+        <v>462</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>463</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>464</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>218</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>218</v>
@@ -8993,7 +9388,7 @@
         <v>218</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>218</v>
@@ -9026,7 +9421,7 @@
         <v>16</v>
       </c>
       <c r="S5" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="T5" s="9" t="s">
         <v>218</v>
@@ -9086,7 +9481,7 @@
         <v>124421</v>
       </c>
       <c r="AM5" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AN5" s="9" t="s">
         <v>368</v>
@@ -9121,13 +9516,13 @@
         <v>367</v>
       </c>
       <c r="AZ5" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="BA5" s="9" t="s">
         <v>456</v>
       </c>
-      <c r="BA5" s="9" t="s">
-        <v>457</v>
-      </c>
       <c r="BB5" s="9" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="BC5" s="9"/>
       <c r="BD5" s="9"/>
@@ -9137,13 +9532,13 @@
     </row>
     <row r="6" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
+        <v>465</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>466</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>467</v>
-      </c>
       <c r="C6" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D6" s="9" t="s">
         <v>218</v>
@@ -9191,7 +9586,7 @@
         <v>16</v>
       </c>
       <c r="S6" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="T6" s="9" t="s">
         <v>218</v>
@@ -9251,7 +9646,7 @@
         <v>124421</v>
       </c>
       <c r="AM6" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AN6" s="9" t="s">
         <v>368</v>
@@ -9286,13 +9681,13 @@
         <v>367</v>
       </c>
       <c r="AZ6" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="BA6" s="9" t="s">
         <v>456</v>
       </c>
-      <c r="BA6" s="9" t="s">
+      <c r="BB6" s="9" t="s">
         <v>457</v>
-      </c>
-      <c r="BB6" s="9" t="s">
-        <v>458</v>
       </c>
       <c r="BC6" s="9"/>
       <c r="BD6" s="9"/>
@@ -9302,10 +9697,10 @@
     </row>
     <row r="7" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
+        <v>467</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>468</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>469</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>218</v>
@@ -9314,13 +9709,13 @@
         <v>218</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F7" s="28" t="s">
         <v>134</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>218</v>
@@ -9356,7 +9751,7 @@
         <v>16</v>
       </c>
       <c r="S7" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="T7" s="9" t="s">
         <v>218</v>
@@ -9416,7 +9811,7 @@
         <v>124421</v>
       </c>
       <c r="AM7" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AN7" s="9" t="s">
         <v>368</v>
@@ -9451,13 +9846,13 @@
         <v>367</v>
       </c>
       <c r="AZ7" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="BA7" s="9" t="s">
         <v>456</v>
       </c>
-      <c r="BA7" s="9" t="s">
+      <c r="BB7" s="9" t="s">
         <v>457</v>
-      </c>
-      <c r="BB7" s="9" t="s">
-        <v>458</v>
       </c>
       <c r="BC7" s="9"/>
       <c r="BD7" s="9"/>
@@ -9467,10 +9862,10 @@
     </row>
     <row r="8" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>470</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>471</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>218</v>
@@ -9482,7 +9877,7 @@
         <v>218</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>218</v>
@@ -9494,7 +9889,7 @@
         <v>218</v>
       </c>
       <c r="J8" s="28" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="K8" s="9" t="s">
         <v>218</v>
@@ -9521,7 +9916,7 @@
         <v>16</v>
       </c>
       <c r="S8" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="T8" s="9" t="s">
         <v>218</v>
@@ -9548,7 +9943,7 @@
         <v>34</v>
       </c>
       <c r="AB8" s="32" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="AC8" s="9">
         <v>23564589</v>
@@ -9581,7 +9976,7 @@
         <v>124421</v>
       </c>
       <c r="AM8" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AN8" s="9" t="s">
         <v>368</v>
@@ -9604,7 +9999,7 @@
         <v>364</v>
       </c>
       <c r="AV8" s="9" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="AW8" s="9" t="s">
         <v>366</v>
@@ -9616,13 +10011,13 @@
         <v>367</v>
       </c>
       <c r="AZ8" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="BA8" s="9" t="s">
         <v>456</v>
       </c>
-      <c r="BA8" s="9" t="s">
-        <v>457</v>
-      </c>
       <c r="BB8" s="9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="BC8" s="9"/>
       <c r="BD8" s="9"/>
@@ -9632,28 +10027,28 @@
     </row>
     <row r="9" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
+        <v>475</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>476</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>477</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>218</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F9" s="28" t="s">
         <v>134</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>218</v>
@@ -9686,7 +10081,7 @@
         <v>16</v>
       </c>
       <c r="S9" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="T9" s="9" t="s">
         <v>218</v>
@@ -9746,7 +10141,7 @@
         <v>124421</v>
       </c>
       <c r="AM9" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AN9" s="9" t="s">
         <v>368</v>
@@ -9781,10 +10176,10 @@
         <v>367</v>
       </c>
       <c r="AZ9" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="BA9" s="9" t="s">
         <v>456</v>
-      </c>
-      <c r="BA9" s="9" t="s">
-        <v>457</v>
       </c>
       <c r="BB9" s="9"/>
       <c r="BC9" s="9"/>
@@ -9795,28 +10190,28 @@
     </row>
     <row r="10" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
+        <v>477</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>478</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>479</v>
-      </c>
       <c r="C10" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>218</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="F10" s="28" t="s">
         <v>134</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>218</v>
@@ -9849,7 +10244,7 @@
         <v>16</v>
       </c>
       <c r="S10" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="T10" s="9" t="s">
         <v>218</v>
@@ -9909,7 +10304,7 @@
         <v>124421</v>
       </c>
       <c r="AM10" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AN10" s="9" t="s">
         <v>368</v>
@@ -9944,10 +10339,10 @@
         <v>367</v>
       </c>
       <c r="AZ10" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="BA10" s="9" t="s">
         <v>456</v>
-      </c>
-      <c r="BA10" s="9" t="s">
-        <v>457</v>
       </c>
       <c r="BB10" s="9"/>
       <c r="BC10" s="9"/>
@@ -9958,10 +10353,10 @@
     </row>
     <row r="11" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>480</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>481</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>218</v>
@@ -9976,10 +10371,10 @@
         <v>134</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>218</v>
@@ -10012,7 +10407,7 @@
         <v>16</v>
       </c>
       <c r="S11" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="T11" s="9" t="s">
         <v>218</v>
@@ -10072,7 +10467,7 @@
         <v>124421</v>
       </c>
       <c r="AM11" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AN11" s="9" t="s">
         <v>368</v>
@@ -10107,13 +10502,13 @@
         <v>367</v>
       </c>
       <c r="AZ11" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="BA11" s="9" t="s">
         <v>456</v>
       </c>
-      <c r="BA11" s="9" t="s">
+      <c r="BB11" s="9" t="s">
         <v>457</v>
-      </c>
-      <c r="BB11" s="9" t="s">
-        <v>458</v>
       </c>
       <c r="BC11" s="9"/>
       <c r="BD11" s="9"/>
@@ -10123,10 +10518,10 @@
     </row>
     <row r="12" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C12" s="9" t="s">
         <v>218</v>
@@ -10141,10 +10536,10 @@
         <v>134</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I12" s="9" t="s">
         <v>218</v>
@@ -10177,7 +10572,7 @@
         <v>16</v>
       </c>
       <c r="S12" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="T12" s="9" t="s">
         <v>218</v>
@@ -10237,7 +10632,7 @@
         <v>124421</v>
       </c>
       <c r="AM12" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="AN12" s="9" t="s">
         <v>368</v>
@@ -10272,17 +10667,17 @@
         <v>367</v>
       </c>
       <c r="AZ12" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="BA12" s="9" t="s">
         <v>456</v>
       </c>
-      <c r="BA12" s="9" t="s">
+      <c r="BB12" s="9" t="s">
         <v>457</v>
-      </c>
-      <c r="BB12" s="9" t="s">
-        <v>458</v>
       </c>
       <c r="BC12" s="9"/>
       <c r="BD12" s="9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="BE12" s="9" t="s">
         <v>218</v>

</xml_diff>

<commit_message>
Test data and tag changes
</commit_message>
<xml_diff>
--- a/src/main/resources/config/stageSA/TestData/TestData.xlsx
+++ b/src/main/resources/config/stageSA/TestData/TestData.xlsx
@@ -1670,9 +1670,6 @@
     <t>NidhiS</t>
   </si>
   <si>
-    <t>LANKA [111777]</t>
-  </si>
-  <si>
     <t>9</t>
   </si>
   <si>
@@ -1680,6 +1677,9 @@
   </si>
   <si>
     <t>Program Code</t>
+  </si>
+  <si>
+    <t>ISSAUTO [190525]</t>
   </si>
 </sst>
 </file>
@@ -3701,8 +3701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:ES177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CL1" workbookViewId="0">
-      <selection activeCell="CX2" sqref="CX2:CX3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4183,7 +4183,7 @@
         <v>483</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>388</v>
@@ -4480,13 +4480,13 @@
         <v>431</v>
       </c>
       <c r="DH2" s="9" t="s">
+        <v>548</v>
+      </c>
+      <c r="DI2" s="9" t="s">
+        <v>547</v>
+      </c>
+      <c r="DJ2" s="9" t="s">
         <v>549</v>
-      </c>
-      <c r="DI2" s="9" t="s">
-        <v>548</v>
-      </c>
-      <c r="DJ2" s="9" t="s">
-        <v>550</v>
       </c>
       <c r="DK2" s="36" t="s">
         <v>431</v>
@@ -4905,13 +4905,13 @@
         <v>431</v>
       </c>
       <c r="DH3" s="9" t="s">
+        <v>548</v>
+      </c>
+      <c r="DI3" s="9" t="s">
+        <v>547</v>
+      </c>
+      <c r="DJ3" s="9" t="s">
         <v>549</v>
-      </c>
-      <c r="DI3" s="9" t="s">
-        <v>548</v>
-      </c>
-      <c r="DJ3" s="9" t="s">
-        <v>550</v>
       </c>
       <c r="DK3" s="36" t="s">
         <v>431</v>

</xml_diff>

<commit_message>
instituion creaion Job fixes
</commit_message>
<xml_diff>
--- a/src/main/resources/config/stageSA/TestData/TestData.xlsx
+++ b/src/main/resources/config/stageSA/TestData/TestData.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2780" uniqueCount="686">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2780" uniqueCount="685">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -2005,9 +2005,6 @@
   </si>
   <si>
     <t>Abbrevation</t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
   <si>
     <t>555522</t>
@@ -4244,8 +4241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
-      <selection activeCell="BH12" sqref="BH12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4513,7 +4510,7 @@
         <v>441</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>659</v>
+        <v>481</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -4629,7 +4626,7 @@
         <v>444</v>
       </c>
       <c r="AQ2" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="AR2" s="2" t="s">
         <v>361</v>
@@ -4667,7 +4664,7 @@
         <v>446</v>
       </c>
       <c r="BE2" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="BF2" s="2"/>
       <c r="BG2" s="2"/>
@@ -4716,7 +4713,7 @@
         <v>454</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -4832,7 +4829,7 @@
         <v>444</v>
       </c>
       <c r="AQ3" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="AR3" s="2" t="s">
         <v>361</v>
@@ -4870,7 +4867,7 @@
         <v>446</v>
       </c>
       <c r="BE3" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="BF3" s="2"/>
       <c r="BG3" s="2"/>
@@ -4919,7 +4916,7 @@
         <v>456</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -5035,7 +5032,7 @@
         <v>444</v>
       </c>
       <c r="AQ4" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="AR4" s="2" t="s">
         <v>361</v>
@@ -5073,7 +5070,7 @@
         <v>446</v>
       </c>
       <c r="BE4" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="BF4" s="2"/>
       <c r="BG4" s="2"/>
@@ -5122,7 +5119,7 @@
         <v>458</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -5238,7 +5235,7 @@
         <v>444</v>
       </c>
       <c r="AQ5" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="AR5" s="2" t="s">
         <v>361</v>
@@ -5276,7 +5273,7 @@
         <v>446</v>
       </c>
       <c r="BE5" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="BF5" s="2"/>
       <c r="BG5" s="2"/>
@@ -5325,7 +5322,7 @@
         <v>460</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -5441,7 +5438,7 @@
         <v>444</v>
       </c>
       <c r="AQ6" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="AR6" s="2" t="s">
         <v>361</v>
@@ -5479,7 +5476,7 @@
         <v>446</v>
       </c>
       <c r="BE6" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="BF6" s="2"/>
       <c r="BG6" s="2"/>
@@ -5528,7 +5525,7 @@
         <v>462</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
@@ -5644,7 +5641,7 @@
         <v>444</v>
       </c>
       <c r="AQ7" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="AR7" s="2" t="s">
         <v>361</v>
@@ -5682,7 +5679,7 @@
         <v>446</v>
       </c>
       <c r="BE7" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="BF7" s="2"/>
       <c r="BG7" s="2"/>
@@ -5731,13 +5728,13 @@
         <v>464</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="D8" s="9" t="s">
+        <v>659</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>660</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>661</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>218</v>
@@ -5851,7 +5848,7 @@
         <v>444</v>
       </c>
       <c r="AQ8" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="AR8" s="2" t="s">
         <v>361</v>
@@ -5889,7 +5886,7 @@
         <v>446</v>
       </c>
       <c r="BE8" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="BF8" s="2"/>
       <c r="BG8" s="2"/>
@@ -5938,7 +5935,7 @@
         <v>466</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -6054,7 +6051,7 @@
         <v>444</v>
       </c>
       <c r="AQ9" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="AR9" s="2" t="s">
         <v>361</v>
@@ -6092,7 +6089,7 @@
         <v>446</v>
       </c>
       <c r="BE9" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="BF9" s="2"/>
       <c r="BG9" s="2"/>
@@ -6141,7 +6138,7 @@
         <v>468</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -6257,7 +6254,7 @@
         <v>444</v>
       </c>
       <c r="AQ10" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="AR10" s="2" t="s">
         <v>361</v>
@@ -6295,7 +6292,7 @@
         <v>446</v>
       </c>
       <c r="BE10" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="BF10" s="2"/>
       <c r="BG10" s="2"/>
@@ -6344,7 +6341,7 @@
         <v>470</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -6460,7 +6457,7 @@
         <v>444</v>
       </c>
       <c r="AQ11" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="AR11" s="2" t="s">
         <v>361</v>
@@ -6498,7 +6495,7 @@
         <v>446</v>
       </c>
       <c r="BE11" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="BF11" s="2"/>
       <c r="BG11" s="2"/>
@@ -6547,7 +6544,7 @@
         <v>470</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -6663,7 +6660,7 @@
         <v>444</v>
       </c>
       <c r="AQ12" s="2" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="AR12" s="2" t="s">
         <v>361</v>
@@ -6701,7 +6698,7 @@
         <v>446</v>
       </c>
       <c r="BE12" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="BF12" s="2"/>
       <c r="BG12" s="2" t="s">
@@ -8724,40 +8721,40 @@
         <v>541</v>
       </c>
       <c r="ER1" s="5" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="ES1" s="4" t="s">
+        <v>661</v>
+      </c>
+      <c r="ET1" s="4" t="s">
         <v>662</v>
       </c>
-      <c r="ET1" s="4" t="s">
+      <c r="EU1" s="4" t="s">
         <v>663</v>
       </c>
-      <c r="EU1" s="4" t="s">
+      <c r="EV1" s="4" t="s">
         <v>664</v>
       </c>
-      <c r="EV1" s="4" t="s">
+      <c r="EW1" s="4" t="s">
         <v>665</v>
       </c>
-      <c r="EW1" s="4" t="s">
+      <c r="EX1" s="4" t="s">
         <v>666</v>
       </c>
-      <c r="EX1" s="4" t="s">
+      <c r="EY1" s="4" t="s">
         <v>667</v>
       </c>
-      <c r="EY1" s="4" t="s">
+      <c r="EZ1" s="4" t="s">
         <v>668</v>
       </c>
-      <c r="EZ1" s="4" t="s">
+      <c r="FA1" s="4" t="s">
         <v>669</v>
       </c>
-      <c r="FA1" s="4" t="s">
+      <c r="FB1" s="4" t="s">
         <v>670</v>
       </c>
-      <c r="FB1" s="4" t="s">
+      <c r="FC1" s="4" t="s">
         <v>671</v>
-      </c>
-      <c r="FC1" s="4" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="2" spans="1:159" ht="90" x14ac:dyDescent="0.25">
@@ -9177,40 +9174,40 @@
         <v>507</v>
       </c>
       <c r="ER2" s="45" t="s">
+        <v>672</v>
+      </c>
+      <c r="ES2" s="9" t="s">
         <v>673</v>
       </c>
-      <c r="ES2" s="9" t="s">
+      <c r="ET2" s="9" t="s">
         <v>674</v>
       </c>
-      <c r="ET2" s="9" t="s">
+      <c r="EU2" s="9" t="s">
         <v>675</v>
-      </c>
-      <c r="EU2" s="9" t="s">
-        <v>676</v>
       </c>
       <c r="EV2" s="9" t="s">
         <v>618</v>
       </c>
       <c r="EW2" s="9" t="s">
+        <v>676</v>
+      </c>
+      <c r="EX2" s="9" t="s">
         <v>677</v>
       </c>
-      <c r="EX2" s="9" t="s">
+      <c r="EY2" s="9" t="s">
         <v>678</v>
       </c>
-      <c r="EY2" s="9" t="s">
+      <c r="EZ2" s="46" t="s">
         <v>679</v>
-      </c>
-      <c r="EZ2" s="46" t="s">
-        <v>680</v>
       </c>
       <c r="FA2" s="9" t="s">
         <v>107</v>
       </c>
       <c r="FB2" s="9" t="s">
+        <v>680</v>
+      </c>
+      <c r="FC2" s="9" t="s">
         <v>681</v>
-      </c>
-      <c r="FC2" s="9" t="s">
-        <v>682</v>
       </c>
     </row>
     <row r="3" spans="1:159" ht="90" x14ac:dyDescent="0.25">
@@ -12222,7 +12219,7 @@
     </row>
     <row r="12" spans="1:159" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>508</v>

</xml_diff>

<commit_message>
edit instituion testdata changes
</commit_message>
<xml_diff>
--- a/src/main/resources/config/stageSA/TestData/TestData.xlsx
+++ b/src/main/resources/config/stageSA/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15105" windowHeight="8985" firstSheet="4" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15105" windowHeight="8985" firstSheet="9" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Prepaid_Application_Upload" sheetId="16" r:id="rId1"/>
@@ -17,18 +17,19 @@
     <sheet name="AccountHead_S205168" sheetId="9" r:id="rId8"/>
     <sheet name="SuspenseAccount_S205193" sheetId="10" r:id="rId9"/>
     <sheet name="Institute" sheetId="5" r:id="rId10"/>
-    <sheet name="ApplicationUpload" sheetId="11" r:id="rId11"/>
-    <sheet name="AmlockDownloads" sheetId="15" r:id="rId12"/>
-    <sheet name="CurrencyExchangeRates" sheetId="12" r:id="rId13"/>
-    <sheet name="CurrencyExchangeRateUpload" sheetId="13" r:id="rId14"/>
-    <sheet name="CurrencyExchangeRateMapping" sheetId="14" r:id="rId15"/>
+    <sheet name="AuditReport" sheetId="17" r:id="rId11"/>
+    <sheet name="ApplicationUpload" sheetId="11" r:id="rId12"/>
+    <sheet name="AmlockDownloads" sheetId="15" r:id="rId13"/>
+    <sheet name="CurrencyExchangeRates" sheetId="12" r:id="rId14"/>
+    <sheet name="CurrencyExchangeRateUpload" sheetId="13" r:id="rId15"/>
+    <sheet name="CurrencyExchangeRateMapping" sheetId="14" r:id="rId16"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2780" uniqueCount="685">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2852" uniqueCount="706">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -1359,9 +1360,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>SDN Name Address [SDN1]</t>
-  </si>
-  <si>
     <t>user</t>
   </si>
   <si>
@@ -2083,6 +2081,72 @@
   </si>
   <si>
     <t>7200022_Role [ROLE000045]</t>
+  </si>
+  <si>
+    <t>Batch [ROLE000052]</t>
+  </si>
+  <si>
+    <t>ISSUINGXH</t>
+  </si>
+  <si>
+    <t>USA,CAN [+1]</t>
+  </si>
+  <si>
+    <t>232527</t>
+  </si>
+  <si>
+    <t>Audit Report</t>
+  </si>
+  <si>
+    <t>MODIFY</t>
+  </si>
+  <si>
+    <t>ravindra1</t>
+  </si>
+  <si>
+    <t>INSTITUTION</t>
+  </si>
+  <si>
+    <t>PDF Format [pdf]</t>
+  </si>
+  <si>
+    <t>Online [O]</t>
+  </si>
+  <si>
+    <t>ReportName</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>ScreenName</t>
+  </si>
+  <si>
+    <t>FileType</t>
+  </si>
+  <si>
+    <t>ReportGenerationMode</t>
+  </si>
+  <si>
+    <t>TC_validate_Audit_Report</t>
+  </si>
+  <si>
+    <t>1122</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>CustCareSTD</t>
+  </si>
+  <si>
+    <t>CustCareIntl</t>
+  </si>
+  <si>
+    <t>CustCareVIP</t>
   </si>
 </sst>
 </file>
@@ -2224,7 +2288,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2312,6 +2376,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2645,49 +2710,49 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>542</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>543</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>194</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>544</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>546</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>547</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>548</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>549</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>552</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>553</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>554</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>555</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>293</v>
@@ -2798,7 +2863,7 @@
         <v>12</v>
       </c>
       <c r="BC1" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="BD1" s="1" t="s">
         <v>13</v>
@@ -2837,7 +2902,7 @@
         <v>22</v>
       </c>
       <c r="BP1" s="4" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="BQ1" s="4" t="s">
         <v>24</v>
@@ -2873,7 +2938,7 @@
         <v>135</v>
       </c>
       <c r="CB1" s="4" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="CC1" s="4" t="s">
         <v>66</v>
@@ -2978,61 +3043,61 @@
         <v>52</v>
       </c>
       <c r="DK1" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="DL1" s="1" t="s">
         <v>559</v>
       </c>
-      <c r="DL1" s="1" t="s">
+      <c r="DM1" s="4" t="s">
         <v>560</v>
-      </c>
-      <c r="DM1" s="4" t="s">
-        <v>561</v>
       </c>
       <c r="DN1" s="1" t="s">
         <v>184</v>
       </c>
       <c r="DO1" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="DP1" s="34" t="s">
         <v>562</v>
       </c>
-      <c r="DP1" s="34" t="s">
+      <c r="DQ1" s="34" t="s">
         <v>563</v>
       </c>
-      <c r="DQ1" s="34" t="s">
+      <c r="DR1" s="34" t="s">
         <v>564</v>
       </c>
-      <c r="DR1" s="34" t="s">
+      <c r="DS1" s="34" t="s">
         <v>565</v>
       </c>
-      <c r="DS1" s="34" t="s">
+      <c r="DT1" s="34" t="s">
         <v>566</v>
       </c>
-      <c r="DT1" s="34" t="s">
+      <c r="DU1" s="34" t="s">
         <v>567</v>
       </c>
-      <c r="DU1" s="34" t="s">
+      <c r="DV1" s="34" t="s">
         <v>568</v>
       </c>
-      <c r="DV1" s="34" t="s">
+      <c r="DW1" s="34" t="s">
         <v>569</v>
       </c>
-      <c r="DW1" s="34" t="s">
+      <c r="DX1" s="34" t="s">
         <v>570</v>
       </c>
-      <c r="DX1" s="34" t="s">
+      <c r="DY1" s="34" t="s">
         <v>571</v>
       </c>
-      <c r="DY1" s="34" t="s">
+      <c r="DZ1" s="34" t="s">
         <v>572</v>
       </c>
-      <c r="DZ1" s="34" t="s">
+      <c r="EA1" s="34" t="s">
         <v>573</v>
       </c>
-      <c r="EA1" s="34" t="s">
+      <c r="EB1" s="34" t="s">
         <v>574</v>
       </c>
-      <c r="EB1" s="34" t="s">
+      <c r="EC1" s="34" t="s">
         <v>575</v>
-      </c>
-      <c r="EC1" s="34" t="s">
-        <v>576</v>
       </c>
       <c r="ED1" s="34" t="s">
         <v>423</v>
@@ -3041,72 +3106,72 @@
         <v>422</v>
       </c>
       <c r="EF1" s="34" t="s">
+        <v>576</v>
+      </c>
+      <c r="EG1" s="34" t="s">
         <v>577</v>
       </c>
-      <c r="EG1" s="34" t="s">
+      <c r="EH1" s="34" t="s">
         <v>578</v>
       </c>
-      <c r="EH1" s="34" t="s">
+      <c r="EI1" s="34" t="s">
         <v>579</v>
       </c>
-      <c r="EI1" s="34" t="s">
+      <c r="EJ1" s="34" t="s">
         <v>580</v>
       </c>
-      <c r="EJ1" s="34" t="s">
+      <c r="EK1" s="34" t="s">
         <v>581</v>
       </c>
-      <c r="EK1" s="34" t="s">
+      <c r="EL1" s="34" t="s">
         <v>582</v>
       </c>
-      <c r="EL1" s="34" t="s">
+      <c r="EM1" s="34" t="s">
         <v>583</v>
-      </c>
-      <c r="EM1" s="34" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="2" spans="1:143" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="B2" t="s">
         <v>585</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" s="2" t="s">
         <v>586</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="35" t="s">
         <v>587</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="E2" s="2" t="s">
         <v>588</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>590</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>591</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>134</v>
       </c>
       <c r="I2" s="28" t="s">
+        <v>591</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>592</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="36" t="s">
         <v>593</v>
       </c>
-      <c r="K2" s="36" t="s">
+      <c r="L2" s="36" t="s">
         <v>594</v>
-      </c>
-      <c r="L2" s="36" t="s">
-        <v>595</v>
       </c>
       <c r="M2" s="36" t="s">
         <v>426</v>
       </c>
       <c r="N2" s="37" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="O2" s="37" t="s">
         <v>428</v>
@@ -3115,16 +3180,16 @@
         <v>428</v>
       </c>
       <c r="Q2" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="R2" s="37" t="s">
+        <v>484</v>
+      </c>
+      <c r="S2" s="37" t="s">
         <v>597</v>
       </c>
-      <c r="R2" s="37" t="s">
-        <v>485</v>
-      </c>
-      <c r="S2" s="37" t="s">
+      <c r="T2" s="37" t="s">
         <v>598</v>
-      </c>
-      <c r="T2" s="37" t="s">
-        <v>599</v>
       </c>
       <c r="U2" s="11">
         <v>50</v>
@@ -3152,16 +3217,16 @@
       </c>
       <c r="AE2" s="12"/>
       <c r="AF2" s="11" t="s">
+        <v>599</v>
+      </c>
+      <c r="AG2" s="12" t="s">
         <v>600</v>
       </c>
-      <c r="AG2" s="12" t="s">
+      <c r="AH2" s="12" t="s">
         <v>601</v>
       </c>
-      <c r="AH2" s="12" t="s">
+      <c r="AI2" s="12" t="s">
         <v>602</v>
-      </c>
-      <c r="AI2" s="12" t="s">
-        <v>603</v>
       </c>
       <c r="AJ2" s="12" t="s">
         <v>36</v>
@@ -3182,7 +3247,7 @@
         <v>121</v>
       </c>
       <c r="AP2" s="12" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AQ2" s="12" t="s">
         <v>120</v>
@@ -3219,7 +3284,7 @@
         <v>1</v>
       </c>
       <c r="BC2" s="12" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="BD2" s="12" t="s">
         <v>16</v>
@@ -3231,7 +3296,7 @@
         <v>12</v>
       </c>
       <c r="BG2" s="12" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="BH2" s="12">
         <v>2</v>
@@ -3249,7 +3314,7 @@
         <v>29</v>
       </c>
       <c r="BM2" s="12" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="BN2" s="12" t="s">
         <v>187</v>
@@ -3279,20 +3344,20 @@
         <v>12345678</v>
       </c>
       <c r="BW2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="BX2" s="40"/>
       <c r="BY2" s="12" t="s">
         <v>143</v>
       </c>
       <c r="BZ2" s="12" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="CA2" s="12" t="s">
         <v>136</v>
       </c>
       <c r="CB2" s="12" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="CC2" s="12" t="s">
         <v>67</v>
@@ -3311,7 +3376,7 @@
         <v>391</v>
       </c>
       <c r="CI2" s="40" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="CJ2" s="38"/>
       <c r="CK2" s="38"/>
@@ -3319,13 +3384,13 @@
         <v>40</v>
       </c>
       <c r="CM2" s="40" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="CN2" s="12" t="s">
         <v>145</v>
       </c>
       <c r="CO2" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="CP2" s="38" t="s">
         <v>341</v>
@@ -3379,40 +3444,40 @@
         <v>53</v>
       </c>
       <c r="DK2" s="11" t="s">
+        <v>609</v>
+      </c>
+      <c r="DL2" s="11" t="s">
         <v>610</v>
       </c>
-      <c r="DL2" s="11" t="s">
+      <c r="DM2" s="12" t="s">
         <v>611</v>
-      </c>
-      <c r="DM2" s="12" t="s">
-        <v>612</v>
       </c>
       <c r="DN2" s="12" t="s">
         <v>185</v>
       </c>
       <c r="DO2" s="11" t="s">
+        <v>612</v>
+      </c>
+      <c r="DP2" s="41" t="s">
         <v>613</v>
       </c>
-      <c r="DP2" s="41" t="s">
+      <c r="DQ2" s="41" t="s">
         <v>614</v>
       </c>
-      <c r="DQ2" s="41" t="s">
+      <c r="DR2" s="41" t="s">
         <v>615</v>
       </c>
-      <c r="DR2" s="41" t="s">
+      <c r="DS2" s="42" t="s">
         <v>616</v>
-      </c>
-      <c r="DS2" s="42" t="s">
-        <v>617</v>
       </c>
       <c r="DT2" s="42" t="s">
         <v>391</v>
       </c>
       <c r="DU2" s="42" t="s">
+        <v>617</v>
+      </c>
+      <c r="DV2" s="41" t="s">
         <v>618</v>
-      </c>
-      <c r="DV2" s="41" t="s">
-        <v>619</v>
       </c>
       <c r="DW2" s="41" t="s">
         <v>134</v>
@@ -3421,24 +3486,24 @@
         <v>390</v>
       </c>
       <c r="DY2" s="42" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="DZ2" s="42" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="EA2" s="42" t="s">
         <v>426</v>
       </c>
       <c r="EB2" s="42" t="s">
+        <v>619</v>
+      </c>
+      <c r="EC2" s="42" t="s">
         <v>620</v>
-      </c>
-      <c r="EC2" s="42" t="s">
-        <v>621</v>
       </c>
       <c r="ED2" s="42"/>
       <c r="EE2" s="42"/>
       <c r="EF2" s="42" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="EG2" s="42"/>
       <c r="EH2" s="42"/>
@@ -3447,51 +3512,51 @@
       <c r="EK2" s="42"/>
       <c r="EL2" s="42"/>
       <c r="EM2" s="41" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="3" spans="1:143" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="B3" t="s">
+        <v>585</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>624</v>
       </c>
-      <c r="B3" t="s">
-        <v>586</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="35" t="s">
         <v>625</v>
       </c>
-      <c r="D3" s="35" t="s">
-        <v>626</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>590</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>591</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>134</v>
       </c>
       <c r="I3" s="28" t="s">
+        <v>591</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>592</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="K3" s="36" t="s">
         <v>593</v>
       </c>
-      <c r="K3" s="36" t="s">
+      <c r="L3" s="36" t="s">
         <v>594</v>
-      </c>
-      <c r="L3" s="36" t="s">
-        <v>595</v>
       </c>
       <c r="M3" s="36" t="s">
         <v>426</v>
       </c>
       <c r="N3" s="37" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="O3" s="37" t="s">
         <v>428</v>
@@ -3500,22 +3565,22 @@
         <v>428</v>
       </c>
       <c r="Q3" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="R3" s="37" t="s">
+        <v>484</v>
+      </c>
+      <c r="S3" s="37" t="s">
         <v>597</v>
       </c>
-      <c r="R3" s="37" t="s">
-        <v>485</v>
-      </c>
-      <c r="S3" s="37" t="s">
+      <c r="T3" s="37" t="s">
         <v>598</v>
-      </c>
-      <c r="T3" s="37" t="s">
-        <v>599</v>
       </c>
       <c r="U3" s="11">
         <v>50</v>
       </c>
       <c r="V3" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="W3" s="11" t="s">
         <v>128</v>
@@ -3537,16 +3602,16 @@
       </c>
       <c r="AE3" s="12"/>
       <c r="AF3" s="11" t="s">
+        <v>599</v>
+      </c>
+      <c r="AG3" s="12" t="s">
         <v>600</v>
       </c>
-      <c r="AG3" s="12" t="s">
+      <c r="AH3" s="12" t="s">
         <v>601</v>
       </c>
-      <c r="AH3" s="12" t="s">
+      <c r="AI3" s="12" t="s">
         <v>602</v>
-      </c>
-      <c r="AI3" s="12" t="s">
-        <v>603</v>
       </c>
       <c r="AJ3" s="12" t="s">
         <v>36</v>
@@ -3567,7 +3632,7 @@
         <v>121</v>
       </c>
       <c r="AP3" s="12" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AQ3" s="12" t="s">
         <v>120</v>
@@ -3604,19 +3669,19 @@
         <v>1</v>
       </c>
       <c r="BC3" s="12" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="BD3" s="12" t="s">
         <v>16</v>
       </c>
       <c r="BE3" s="12" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="BF3" s="12">
         <v>12</v>
       </c>
       <c r="BG3" s="12" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="BH3" s="12">
         <v>2</v>
@@ -3634,7 +3699,7 @@
         <v>29</v>
       </c>
       <c r="BM3" s="12" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="BN3" s="12" t="s">
         <v>187</v>
@@ -3664,20 +3729,20 @@
         <v>12345678</v>
       </c>
       <c r="BW3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="BX3" s="40"/>
       <c r="BY3" s="12" t="s">
         <v>143</v>
       </c>
       <c r="BZ3" s="12" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="CA3" s="12" t="s">
         <v>136</v>
       </c>
       <c r="CB3" s="12" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="CC3" s="12" t="s">
         <v>67</v>
@@ -3696,7 +3761,7 @@
         <v>391</v>
       </c>
       <c r="CI3" s="40" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="CJ3" s="38"/>
       <c r="CK3" s="38"/>
@@ -3704,13 +3769,13 @@
         <v>40</v>
       </c>
       <c r="CM3" s="40" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="CN3" s="12" t="s">
         <v>145</v>
       </c>
       <c r="CO3" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="CP3" s="38" t="s">
         <v>341</v>
@@ -3722,7 +3787,7 @@
         <v>51</v>
       </c>
       <c r="CS3" s="43" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="CT3" s="11"/>
       <c r="CU3" s="11"/>
@@ -3764,40 +3829,40 @@
         <v>53</v>
       </c>
       <c r="DK3" s="11" t="s">
+        <v>609</v>
+      </c>
+      <c r="DL3" s="11" t="s">
         <v>610</v>
       </c>
-      <c r="DL3" s="11" t="s">
+      <c r="DM3" s="12" t="s">
         <v>611</v>
-      </c>
-      <c r="DM3" s="12" t="s">
-        <v>612</v>
       </c>
       <c r="DN3" s="12" t="s">
         <v>185</v>
       </c>
       <c r="DO3" s="11" t="s">
+        <v>612</v>
+      </c>
+      <c r="DP3" s="41" t="s">
         <v>613</v>
       </c>
-      <c r="DP3" s="41" t="s">
+      <c r="DQ3" s="41" t="s">
         <v>614</v>
       </c>
-      <c r="DQ3" s="41" t="s">
+      <c r="DR3" s="41" t="s">
         <v>615</v>
       </c>
-      <c r="DR3" s="41" t="s">
+      <c r="DS3" s="42" t="s">
         <v>616</v>
-      </c>
-      <c r="DS3" s="42" t="s">
-        <v>617</v>
       </c>
       <c r="DT3" s="42" t="s">
         <v>391</v>
       </c>
       <c r="DU3" s="42" t="s">
+        <v>617</v>
+      </c>
+      <c r="DV3" s="41" t="s">
         <v>618</v>
-      </c>
-      <c r="DV3" s="41" t="s">
-        <v>619</v>
       </c>
       <c r="DW3" s="41" t="s">
         <v>134</v>
@@ -3806,89 +3871,89 @@
         <v>390</v>
       </c>
       <c r="DY3" s="42" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="DZ3" s="42" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="EA3" s="42" t="s">
         <v>426</v>
       </c>
       <c r="EB3" s="42" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="EC3" s="42" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="ED3" s="42"/>
       <c r="EE3" s="42"/>
       <c r="EF3" s="42" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="EG3" s="42" t="s">
         <v>395</v>
       </c>
       <c r="EH3" s="42" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="EI3" s="42" t="s">
         <v>51</v>
       </c>
       <c r="EJ3" s="42" t="s">
+        <v>630</v>
+      </c>
+      <c r="EK3" s="42" t="s">
         <v>631</v>
       </c>
-      <c r="EK3" s="42" t="s">
-        <v>632</v>
-      </c>
       <c r="EL3" s="42" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="EM3" s="41" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="4" spans="1:143" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="B4" t="s">
+        <v>585</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>633</v>
       </c>
-      <c r="B4" t="s">
-        <v>586</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="35" t="s">
         <v>634</v>
       </c>
-      <c r="D4" s="35" t="s">
-        <v>635</v>
-      </c>
       <c r="E4" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>589</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>590</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>591</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>134</v>
       </c>
       <c r="I4" s="28" t="s">
+        <v>591</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>592</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="36" t="s">
         <v>593</v>
       </c>
-      <c r="K4" s="36" t="s">
+      <c r="L4" s="36" t="s">
         <v>594</v>
-      </c>
-      <c r="L4" s="36" t="s">
-        <v>595</v>
       </c>
       <c r="M4" s="36" t="s">
         <v>426</v>
       </c>
       <c r="N4" s="37" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="O4" s="37" t="s">
         <v>428</v>
@@ -3897,16 +3962,16 @@
         <v>428</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="R4" s="37" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="S4" s="37" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="T4" s="37" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="U4" s="11">
         <v>50</v>
@@ -3934,16 +3999,16 @@
       </c>
       <c r="AE4" s="12"/>
       <c r="AF4" s="11" t="s">
+        <v>599</v>
+      </c>
+      <c r="AG4" s="12" t="s">
         <v>600</v>
       </c>
-      <c r="AG4" s="12" t="s">
+      <c r="AH4" s="12" t="s">
         <v>601</v>
       </c>
-      <c r="AH4" s="12" t="s">
+      <c r="AI4" s="12" t="s">
         <v>602</v>
-      </c>
-      <c r="AI4" s="12" t="s">
-        <v>603</v>
       </c>
       <c r="AJ4" s="12" t="s">
         <v>36</v>
@@ -3964,7 +4029,7 @@
         <v>121</v>
       </c>
       <c r="AP4" s="12" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="AQ4" s="12" t="s">
         <v>120</v>
@@ -4001,7 +4066,7 @@
         <v>1</v>
       </c>
       <c r="BC4" s="12" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="BD4" s="12" t="s">
         <v>16</v>
@@ -4013,7 +4078,7 @@
         <v>12</v>
       </c>
       <c r="BG4" s="12" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="BH4" s="12">
         <v>2</v>
@@ -4031,7 +4096,7 @@
         <v>29</v>
       </c>
       <c r="BM4" s="12" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="BN4" s="12" t="s">
         <v>187</v>
@@ -4061,20 +4126,20 @@
         <v>12345678</v>
       </c>
       <c r="BW4" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="BX4" s="40"/>
       <c r="BY4" s="12" t="s">
         <v>143</v>
       </c>
       <c r="BZ4" s="12" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="CA4" s="12" t="s">
         <v>136</v>
       </c>
       <c r="CB4" s="12" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="CC4" s="12" t="s">
         <v>67</v>
@@ -4093,7 +4158,7 @@
         <v>391</v>
       </c>
       <c r="CI4" s="40" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="CJ4" s="38"/>
       <c r="CK4" s="38"/>
@@ -4101,13 +4166,13 @@
         <v>40</v>
       </c>
       <c r="CM4" s="40" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="CN4" s="12" t="s">
         <v>145</v>
       </c>
       <c r="CO4" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="CP4" s="38" t="s">
         <v>341</v>
@@ -4161,40 +4226,40 @@
         <v>53</v>
       </c>
       <c r="DK4" s="11" t="s">
+        <v>609</v>
+      </c>
+      <c r="DL4" s="11" t="s">
         <v>610</v>
       </c>
-      <c r="DL4" s="11" t="s">
+      <c r="DM4" s="12" t="s">
         <v>611</v>
-      </c>
-      <c r="DM4" s="12" t="s">
-        <v>612</v>
       </c>
       <c r="DN4" s="12" t="s">
         <v>185</v>
       </c>
       <c r="DO4" s="11" t="s">
+        <v>612</v>
+      </c>
+      <c r="DP4" s="41" t="s">
         <v>613</v>
       </c>
-      <c r="DP4" s="41" t="s">
+      <c r="DQ4" s="41" t="s">
         <v>614</v>
       </c>
-      <c r="DQ4" s="41" t="s">
+      <c r="DR4" s="41" t="s">
         <v>615</v>
       </c>
-      <c r="DR4" s="41" t="s">
+      <c r="DS4" s="42" t="s">
         <v>616</v>
-      </c>
-      <c r="DS4" s="42" t="s">
-        <v>617</v>
       </c>
       <c r="DT4" s="42" t="s">
         <v>391</v>
       </c>
       <c r="DU4" s="42" t="s">
+        <v>617</v>
+      </c>
+      <c r="DV4" s="41" t="s">
         <v>618</v>
-      </c>
-      <c r="DV4" s="41" t="s">
-        <v>619</v>
       </c>
       <c r="DW4" s="41" t="s">
         <v>134</v>
@@ -4203,24 +4268,24 @@
         <v>390</v>
       </c>
       <c r="DY4" s="42" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="DZ4" s="42" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="EA4" s="42" t="s">
         <v>426</v>
       </c>
       <c r="EB4" s="42" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="EC4" s="42" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="ED4" s="42"/>
       <c r="EE4" s="42"/>
       <c r="EF4" s="42" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="EG4" s="42"/>
       <c r="EH4" s="42"/>
@@ -4229,7 +4294,7 @@
       <c r="EK4" s="42"/>
       <c r="EL4" s="42"/>
       <c r="EM4" s="41" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
   </sheetData>
@@ -4239,10 +4304,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BU12"/>
+  <dimension ref="A1:CD12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="BQ1" workbookViewId="0">
+      <selection activeCell="CI15" sqref="CI15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4272,16 +4337,17 @@
     <col min="28" max="28" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="62" max="62" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="15" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="46" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="15" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="15" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="46" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="15" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:73" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:82" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -4289,13 +4355,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>656</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>657</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>658</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>281</v>
@@ -4451,58 +4517,85 @@
         <v>439</v>
       </c>
       <c r="BE1" s="15" t="s">
+        <v>446</v>
+      </c>
+      <c r="BF1" s="15" t="s">
         <v>447</v>
       </c>
-      <c r="BF1" s="15" t="s">
+      <c r="BG1" s="15" t="s">
         <v>448</v>
       </c>
-      <c r="BG1" s="15" t="s">
+      <c r="BH1" s="15" t="s">
         <v>449</v>
       </c>
-      <c r="BH1" s="15" t="s">
+      <c r="BI1" s="15" t="s">
         <v>450</v>
       </c>
-      <c r="BI1" s="15" t="s">
+      <c r="BJ1" s="15" t="s">
         <v>451</v>
       </c>
-      <c r="BJ1" s="15" t="s">
-        <v>452</v>
-      </c>
       <c r="BK1" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="BL1" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="BM1" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="BO1" s="1" t="s">
         <v>638</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>639</v>
       </c>
-      <c r="BM1" s="1" t="s">
-        <v>640</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>643</v>
-      </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="BS1" s="1" t="s">
         <v>645</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>646</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>648</v>
       </c>
-      <c r="BS1" s="1" t="s">
-        <v>649</v>
-      </c>
-      <c r="BT1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="BX1" s="1" t="s">
         <v>653</v>
       </c>
-      <c r="BU1" s="1" t="s">
-        <v>654</v>
-      </c>
-    </row>
-    <row r="2" spans="1:73" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="BY1" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="CC1" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="CD1" s="1" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="2" spans="1:82" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>440</v>
       </c>
@@ -4510,7 +4603,7 @@
         <v>441</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
@@ -4563,10 +4656,10 @@
         <v>16</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>443</v>
+        <v>702</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>218</v>
@@ -4623,10 +4716,10 @@
         <v>124421</v>
       </c>
       <c r="AP2" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AQ2" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="AR2" s="2" t="s">
         <v>361</v>
@@ -4658,13 +4751,13 @@
         <v>366</v>
       </c>
       <c r="BC2" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="BD2" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="BD2" s="2" t="s">
-        <v>446</v>
-      </c>
       <c r="BE2" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="BF2" s="2"/>
       <c r="BG2" s="2"/>
@@ -4672,48 +4765,57 @@
       <c r="BI2" s="2"/>
       <c r="BJ2" s="2"/>
       <c r="BK2" s="9" t="s">
+        <v>686</v>
+      </c>
+      <c r="BL2" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BM2" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BN2" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="BO2" s="9" t="s">
         <v>641</v>
       </c>
-      <c r="BL2" s="9" t="s">
-        <v>642</v>
-      </c>
-      <c r="BM2" s="9" t="s">
+      <c r="BP2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="BN2" s="9" t="s">
-        <v>644</v>
-      </c>
-      <c r="BO2" s="9" t="s">
+      <c r="BQ2" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="BR2" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="BS2" s="9" t="s">
         <v>650</v>
       </c>
-      <c r="BP2" s="9" t="s">
-        <v>651</v>
-      </c>
-      <c r="BQ2" s="9" t="s">
+      <c r="BT2" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BR2" s="9" t="s">
+      <c r="BU2" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BS2" s="9" t="s">
+      <c r="BV2" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BT2" s="44" t="s">
-        <v>655</v>
-      </c>
-      <c r="BU2" s="44" t="s">
+      <c r="BW2" s="44" t="s">
+        <v>654</v>
+      </c>
+      <c r="BX2" s="44" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="3" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>454</v>
-      </c>
       <c r="C3" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="9"/>
@@ -4766,10 +4868,10 @@
         <v>16</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>443</v>
+        <v>702</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="X3" s="2" t="s">
         <v>218</v>
@@ -4826,10 +4928,10 @@
         <v>124421</v>
       </c>
       <c r="AP3" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AQ3" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="AR3" s="2" t="s">
         <v>361</v>
@@ -4861,13 +4963,13 @@
         <v>366</v>
       </c>
       <c r="BC3" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="BD3" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="BD3" s="2" t="s">
-        <v>446</v>
-      </c>
       <c r="BE3" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="BF3" s="2"/>
       <c r="BG3" s="2"/>
@@ -4875,48 +4977,57 @@
       <c r="BI3" s="2"/>
       <c r="BJ3" s="2"/>
       <c r="BK3" s="9" t="s">
+        <v>686</v>
+      </c>
+      <c r="BL3" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BM3" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BN3" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="BO3" s="9" t="s">
         <v>641</v>
       </c>
-      <c r="BL3" s="9" t="s">
-        <v>642</v>
-      </c>
-      <c r="BM3" s="9" t="s">
+      <c r="BP3" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="BN3" s="9" t="s">
-        <v>644</v>
-      </c>
-      <c r="BO3" s="9" t="s">
-        <v>650</v>
-      </c>
-      <c r="BP3" s="9" t="s">
-        <v>652</v>
-      </c>
       <c r="BQ3" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="BR3" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="BS3" s="9" t="s">
+        <v>651</v>
+      </c>
+      <c r="BT3" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BR3" s="9" t="s">
+      <c r="BU3" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BS3" s="9" t="s">
+      <c r="BV3" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BT3" s="44" t="s">
-        <v>655</v>
-      </c>
-      <c r="BU3" s="44" t="s">
+      <c r="BW3" s="44" t="s">
+        <v>654</v>
+      </c>
+      <c r="BX3" s="44" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>456</v>
-      </c>
       <c r="C4" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
@@ -4969,10 +5080,10 @@
         <v>16</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>443</v>
+        <v>702</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="X4" s="2" t="s">
         <v>218</v>
@@ -5029,10 +5140,10 @@
         <v>124421</v>
       </c>
       <c r="AP4" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AQ4" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="AR4" s="2" t="s">
         <v>361</v>
@@ -5064,13 +5175,13 @@
         <v>366</v>
       </c>
       <c r="BC4" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="BD4" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="BD4" s="2" t="s">
-        <v>446</v>
-      </c>
       <c r="BE4" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="BF4" s="2"/>
       <c r="BG4" s="2"/>
@@ -5078,48 +5189,57 @@
       <c r="BI4" s="2"/>
       <c r="BJ4" s="2"/>
       <c r="BK4" s="9" t="s">
+        <v>686</v>
+      </c>
+      <c r="BL4" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BM4" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BN4" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="BO4" s="9" t="s">
         <v>641</v>
       </c>
-      <c r="BL4" s="9" t="s">
-        <v>642</v>
-      </c>
-      <c r="BM4" s="9" t="s">
+      <c r="BP4" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="BN4" s="9" t="s">
-        <v>644</v>
-      </c>
-      <c r="BO4" s="9" t="s">
+      <c r="BQ4" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="BR4" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="BS4" s="9" t="s">
         <v>650</v>
       </c>
-      <c r="BP4" s="9" t="s">
-        <v>651</v>
-      </c>
-      <c r="BQ4" s="9" t="s">
+      <c r="BT4" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BR4" s="9" t="s">
+      <c r="BU4" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BS4" s="9" t="s">
+      <c r="BV4" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BT4" s="44" t="s">
-        <v>655</v>
-      </c>
-      <c r="BU4" s="44" t="s">
+      <c r="BW4" s="44" t="s">
+        <v>654</v>
+      </c>
+      <c r="BX4" s="44" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="5" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>458</v>
-      </c>
       <c r="C5" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -5172,10 +5292,10 @@
         <v>16</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>443</v>
+        <v>702</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="X5" s="2" t="s">
         <v>218</v>
@@ -5232,10 +5352,10 @@
         <v>124421</v>
       </c>
       <c r="AP5" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AQ5" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="AR5" s="2" t="s">
         <v>361</v>
@@ -5267,13 +5387,13 @@
         <v>366</v>
       </c>
       <c r="BC5" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="BD5" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="BD5" s="2" t="s">
-        <v>446</v>
-      </c>
       <c r="BE5" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="BF5" s="2"/>
       <c r="BG5" s="2"/>
@@ -5281,48 +5401,57 @@
       <c r="BI5" s="2"/>
       <c r="BJ5" s="2"/>
       <c r="BK5" s="9" t="s">
+        <v>686</v>
+      </c>
+      <c r="BL5" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BM5" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BN5" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="BO5" s="9" t="s">
         <v>641</v>
       </c>
-      <c r="BL5" s="9" t="s">
-        <v>642</v>
-      </c>
-      <c r="BM5" s="9" t="s">
+      <c r="BP5" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="BN5" s="9" t="s">
-        <v>644</v>
-      </c>
-      <c r="BO5" s="9" t="s">
+      <c r="BQ5" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="BR5" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="BS5" s="9" t="s">
         <v>650</v>
       </c>
-      <c r="BP5" s="9" t="s">
-        <v>651</v>
-      </c>
-      <c r="BQ5" s="9" t="s">
+      <c r="BT5" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BR5" s="9" t="s">
+      <c r="BU5" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BS5" s="9" t="s">
+      <c r="BV5" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BT5" s="44" t="s">
-        <v>655</v>
-      </c>
-      <c r="BU5" s="44" t="s">
+      <c r="BW5" s="44" t="s">
+        <v>654</v>
+      </c>
+      <c r="BX5" s="44" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="6" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>460</v>
-      </c>
       <c r="C6" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -5375,10 +5504,10 @@
         <v>16</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>443</v>
+        <v>702</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="X6" s="2" t="s">
         <v>218</v>
@@ -5435,10 +5564,10 @@
         <v>124421</v>
       </c>
       <c r="AP6" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AQ6" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="AR6" s="2" t="s">
         <v>361</v>
@@ -5470,13 +5599,13 @@
         <v>366</v>
       </c>
       <c r="BC6" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="BD6" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="BD6" s="2" t="s">
-        <v>446</v>
-      </c>
       <c r="BE6" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="BF6" s="2"/>
       <c r="BG6" s="2"/>
@@ -5484,48 +5613,57 @@
       <c r="BI6" s="2"/>
       <c r="BJ6" s="2"/>
       <c r="BK6" s="9" t="s">
+        <v>686</v>
+      </c>
+      <c r="BL6" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BM6" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BN6" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="BO6" s="9" t="s">
         <v>641</v>
       </c>
-      <c r="BL6" s="9" t="s">
-        <v>642</v>
-      </c>
-      <c r="BM6" s="9" t="s">
+      <c r="BP6" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="BN6" s="9" t="s">
-        <v>644</v>
-      </c>
-      <c r="BO6" s="9" t="s">
+      <c r="BQ6" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="BR6" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="BS6" s="9" t="s">
         <v>650</v>
       </c>
-      <c r="BP6" s="9" t="s">
-        <v>651</v>
-      </c>
-      <c r="BQ6" s="9" t="s">
+      <c r="BT6" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BR6" s="9" t="s">
+      <c r="BU6" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BS6" s="9" t="s">
+      <c r="BV6" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BT6" s="44" t="s">
-        <v>655</v>
-      </c>
-      <c r="BU6" s="44" t="s">
+      <c r="BW6" s="44" t="s">
+        <v>654</v>
+      </c>
+      <c r="BX6" s="44" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="7" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>461</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>462</v>
-      </c>
       <c r="C7" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="9"/>
@@ -5578,10 +5716,10 @@
         <v>16</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>443</v>
+        <v>702</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="X7" s="2" t="s">
         <v>218</v>
@@ -5638,10 +5776,10 @@
         <v>124421</v>
       </c>
       <c r="AP7" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AQ7" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="AR7" s="2" t="s">
         <v>361</v>
@@ -5673,13 +5811,13 @@
         <v>366</v>
       </c>
       <c r="BC7" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="BD7" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="BD7" s="2" t="s">
-        <v>446</v>
-      </c>
       <c r="BE7" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="BF7" s="2"/>
       <c r="BG7" s="2"/>
@@ -5687,54 +5825,63 @@
       <c r="BI7" s="2"/>
       <c r="BJ7" s="2"/>
       <c r="BK7" s="9" t="s">
+        <v>686</v>
+      </c>
+      <c r="BL7" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BM7" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BN7" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="BO7" s="9" t="s">
         <v>641</v>
       </c>
-      <c r="BL7" s="9" t="s">
-        <v>642</v>
-      </c>
-      <c r="BM7" s="9" t="s">
+      <c r="BP7" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="BN7" s="9" t="s">
-        <v>644</v>
-      </c>
-      <c r="BO7" s="9" t="s">
+      <c r="BQ7" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="BR7" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="BS7" s="9" t="s">
         <v>650</v>
       </c>
-      <c r="BP7" s="9" t="s">
-        <v>651</v>
-      </c>
-      <c r="BQ7" s="9" t="s">
+      <c r="BT7" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BR7" s="9" t="s">
+      <c r="BU7" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BS7" s="9" t="s">
+      <c r="BV7" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BT7" s="44" t="s">
-        <v>655</v>
-      </c>
-      <c r="BU7" s="44" t="s">
+      <c r="BW7" s="44" t="s">
+        <v>654</v>
+      </c>
+      <c r="BX7" s="44" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="8" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>463</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>464</v>
-      </c>
       <c r="C8" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D8" s="9" t="s">
+        <v>658</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>659</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>660</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>218</v>
@@ -5785,10 +5932,10 @@
         <v>16</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>443</v>
+        <v>702</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="X8" s="2" t="s">
         <v>218</v>
@@ -5845,10 +5992,10 @@
         <v>124421</v>
       </c>
       <c r="AP8" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AQ8" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="AR8" s="2" t="s">
         <v>361</v>
@@ -5880,13 +6027,13 @@
         <v>366</v>
       </c>
       <c r="BC8" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="BD8" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="BD8" s="2" t="s">
-        <v>446</v>
-      </c>
       <c r="BE8" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="BF8" s="2"/>
       <c r="BG8" s="2"/>
@@ -5894,48 +6041,57 @@
       <c r="BI8" s="2"/>
       <c r="BJ8" s="2"/>
       <c r="BK8" s="9" t="s">
+        <v>686</v>
+      </c>
+      <c r="BL8" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BM8" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BN8" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="BO8" s="9" t="s">
         <v>641</v>
       </c>
-      <c r="BL8" s="9" t="s">
-        <v>642</v>
-      </c>
-      <c r="BM8" s="9" t="s">
+      <c r="BP8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="BN8" s="9" t="s">
-        <v>644</v>
-      </c>
-      <c r="BO8" s="9" t="s">
+      <c r="BQ8" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="BR8" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="BS8" s="9" t="s">
         <v>650</v>
       </c>
-      <c r="BP8" s="9" t="s">
-        <v>651</v>
-      </c>
-      <c r="BQ8" s="9" t="s">
+      <c r="BT8" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BR8" s="9" t="s">
+      <c r="BU8" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BS8" s="9" t="s">
+      <c r="BV8" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BT8" s="44" t="s">
-        <v>655</v>
-      </c>
-      <c r="BU8" s="44" t="s">
+      <c r="BW8" s="44" t="s">
+        <v>654</v>
+      </c>
+      <c r="BX8" s="44" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="9" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>466</v>
-      </c>
       <c r="C9" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="9"/>
@@ -5988,10 +6144,10 @@
         <v>16</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>443</v>
+        <v>702</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="X9" s="2" t="s">
         <v>218</v>
@@ -6048,10 +6204,10 @@
         <v>124421</v>
       </c>
       <c r="AP9" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AQ9" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="AR9" s="2" t="s">
         <v>361</v>
@@ -6083,13 +6239,13 @@
         <v>366</v>
       </c>
       <c r="BC9" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="BD9" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="BD9" s="2" t="s">
-        <v>446</v>
-      </c>
       <c r="BE9" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="BF9" s="2"/>
       <c r="BG9" s="2"/>
@@ -6097,48 +6253,57 @@
       <c r="BI9" s="2"/>
       <c r="BJ9" s="2"/>
       <c r="BK9" s="9" t="s">
+        <v>686</v>
+      </c>
+      <c r="BL9" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BM9" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BN9" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="BO9" s="9" t="s">
         <v>641</v>
       </c>
-      <c r="BL9" s="9" t="s">
-        <v>642</v>
-      </c>
-      <c r="BM9" s="9" t="s">
+      <c r="BP9" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="BN9" s="9" t="s">
-        <v>644</v>
-      </c>
-      <c r="BO9" s="9" t="s">
+      <c r="BQ9" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="BR9" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="BS9" s="9" t="s">
         <v>650</v>
       </c>
-      <c r="BP9" s="9" t="s">
-        <v>651</v>
-      </c>
-      <c r="BQ9" s="9" t="s">
+      <c r="BT9" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BR9" s="9" t="s">
+      <c r="BU9" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BS9" s="9" t="s">
+      <c r="BV9" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BT9" s="44" t="s">
-        <v>655</v>
-      </c>
-      <c r="BU9" s="44" t="s">
+      <c r="BW9" s="44" t="s">
+        <v>654</v>
+      </c>
+      <c r="BX9" s="44" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="10" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>467</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>468</v>
-      </c>
       <c r="C10" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -6191,10 +6356,10 @@
         <v>16</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>443</v>
+        <v>702</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="X10" s="2" t="s">
         <v>218</v>
@@ -6251,10 +6416,10 @@
         <v>124421</v>
       </c>
       <c r="AP10" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AQ10" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="AR10" s="2" t="s">
         <v>361</v>
@@ -6286,13 +6451,13 @@
         <v>366</v>
       </c>
       <c r="BC10" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="BD10" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="BD10" s="2" t="s">
-        <v>446</v>
-      </c>
       <c r="BE10" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="BF10" s="2"/>
       <c r="BG10" s="2"/>
@@ -6300,48 +6465,57 @@
       <c r="BI10" s="2"/>
       <c r="BJ10" s="2"/>
       <c r="BK10" s="9" t="s">
+        <v>686</v>
+      </c>
+      <c r="BL10" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BM10" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BN10" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="BO10" s="9" t="s">
         <v>641</v>
       </c>
-      <c r="BL10" s="9" t="s">
-        <v>642</v>
-      </c>
-      <c r="BM10" s="9" t="s">
+      <c r="BP10" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="BN10" s="9" t="s">
-        <v>644</v>
-      </c>
-      <c r="BO10" s="9" t="s">
+      <c r="BQ10" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="BR10" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="BS10" s="9" t="s">
         <v>650</v>
       </c>
-      <c r="BP10" s="9" t="s">
-        <v>651</v>
-      </c>
-      <c r="BQ10" s="9" t="s">
+      <c r="BT10" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BR10" s="9" t="s">
+      <c r="BU10" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BS10" s="9" t="s">
+      <c r="BV10" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BT10" s="44" t="s">
-        <v>655</v>
-      </c>
-      <c r="BU10" s="44" t="s">
+      <c r="BW10" s="44" t="s">
+        <v>654</v>
+      </c>
+      <c r="BX10" s="44" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="11" spans="1:73" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:82" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>469</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>470</v>
-      </c>
       <c r="C11" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
@@ -6394,10 +6568,10 @@
         <v>16</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>443</v>
+        <v>702</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="X11" s="2" t="s">
         <v>218</v>
@@ -6454,10 +6628,10 @@
         <v>124421</v>
       </c>
       <c r="AP11" s="2" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AQ11" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="AR11" s="2" t="s">
         <v>361</v>
@@ -6489,13 +6663,13 @@
         <v>366</v>
       </c>
       <c r="BC11" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="BD11" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="BD11" s="2" t="s">
-        <v>446</v>
-      </c>
       <c r="BE11" s="2" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="BF11" s="2"/>
       <c r="BG11" s="2"/>
@@ -6503,257 +6677,391 @@
       <c r="BI11" s="2"/>
       <c r="BJ11" s="2"/>
       <c r="BK11" s="9" t="s">
+        <v>686</v>
+      </c>
+      <c r="BL11" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BM11" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BN11" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="BO11" s="9" t="s">
         <v>641</v>
       </c>
-      <c r="BL11" s="9" t="s">
-        <v>642</v>
-      </c>
-      <c r="BM11" s="9" t="s">
+      <c r="BP11" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="BN11" s="9" t="s">
-        <v>644</v>
-      </c>
-      <c r="BO11" s="9" t="s">
+      <c r="BQ11" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="BR11" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="BS11" s="9" t="s">
         <v>650</v>
       </c>
-      <c r="BP11" s="9" t="s">
-        <v>651</v>
-      </c>
-      <c r="BQ11" s="9" t="s">
+      <c r="BT11" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BR11" s="9" t="s">
+      <c r="BU11" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BS11" s="9" t="s">
+      <c r="BV11" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BT11" s="44" t="s">
-        <v>655</v>
-      </c>
-      <c r="BU11" s="44" t="s">
+      <c r="BW11" s="44" t="s">
+        <v>654</v>
+      </c>
+      <c r="BX11" s="44" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="12" spans="1:73" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="B12" s="2" t="s">
+    <row r="12" spans="1:82" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
         <v>470</v>
       </c>
+      <c r="B12" s="9" t="s">
+        <v>469</v>
+      </c>
       <c r="C12" s="9" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="9" t="s">
         <v>442</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="9" t="s">
         <v>442</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="L12" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="M12" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="N12" s="2" t="s">
+      <c r="N12" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="O12" s="2" t="s">
+      <c r="O12" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="P12" s="2" t="s">
+      <c r="P12" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="Q12" s="2" t="s">
+      <c r="Q12" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="R12" s="2" t="s">
+      <c r="R12" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="S12" s="2" t="s">
+      <c r="S12" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="T12" s="2">
+      <c r="T12" s="9">
         <v>16</v>
       </c>
-      <c r="U12" s="2">
+      <c r="U12" s="9">
         <v>16</v>
       </c>
       <c r="V12" s="2" t="s">
+        <v>702</v>
+      </c>
+      <c r="W12" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="X12" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="Y12" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="Z12" s="9">
+        <v>1100440052</v>
+      </c>
+      <c r="AA12" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="AB12" s="9">
+        <v>45665456</v>
+      </c>
+      <c r="AC12" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="AD12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE12" s="9">
+        <v>1113332</v>
+      </c>
+      <c r="AF12" s="9">
+        <v>23564589</v>
+      </c>
+      <c r="AG12" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="AH12" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="AI12" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="AJ12" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="AK12" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="AL12" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM12" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="AN12" s="9">
+        <v>411006</v>
+      </c>
+      <c r="AO12" s="9">
+        <v>124421</v>
+      </c>
+      <c r="AP12" s="9" t="s">
         <v>443</v>
       </c>
-      <c r="W12" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="X12" s="2" t="s">
+      <c r="AQ12" s="9" t="s">
+        <v>684</v>
+      </c>
+      <c r="AR12" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="AS12" s="9" t="s">
+        <v>362</v>
+      </c>
+      <c r="AT12" s="9"/>
+      <c r="AU12" s="9"/>
+      <c r="AV12" s="9" t="s">
+        <v>363</v>
+      </c>
+      <c r="AW12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AX12" s="9">
+        <v>5431267812</v>
+      </c>
+      <c r="AY12" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="AZ12" s="9" t="s">
+        <v>365</v>
+      </c>
+      <c r="BA12" s="9">
+        <v>999</v>
+      </c>
+      <c r="BB12" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="BC12" s="9" t="s">
+        <v>444</v>
+      </c>
+      <c r="BD12" s="9" t="s">
+        <v>445</v>
+      </c>
+      <c r="BE12" s="9" t="s">
+        <v>685</v>
+      </c>
+      <c r="BF12" s="9"/>
+      <c r="BG12" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="BH12" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="Y12" s="2" t="s">
+      <c r="BI12" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="Z12" s="2">
-        <v>1100440052</v>
-      </c>
-      <c r="AA12" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="AB12" s="2">
-        <v>45665456</v>
-      </c>
-      <c r="AC12" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="AD12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AE12" s="2">
-        <v>1113332</v>
-      </c>
-      <c r="AF12" s="2">
-        <v>23564589</v>
-      </c>
-      <c r="AG12" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="AH12" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="AI12" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="AJ12" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="AK12" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="AL12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AM12" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="AN12" s="2">
-        <v>411006</v>
-      </c>
-      <c r="AO12" s="2">
-        <v>124421</v>
-      </c>
-      <c r="AP12" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="AQ12" s="2" t="s">
-        <v>684</v>
-      </c>
-      <c r="AR12" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="AS12" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="AT12" s="2"/>
-      <c r="AU12" s="2"/>
-      <c r="AV12" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="AW12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AX12" s="2">
-        <v>5431267812</v>
-      </c>
-      <c r="AY12" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="AZ12" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="BA12" s="2">
-        <v>999</v>
-      </c>
-      <c r="BB12" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="BC12" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="BD12" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="BE12" s="2" t="s">
-        <v>660</v>
-      </c>
-      <c r="BF12" s="2"/>
-      <c r="BG12" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="BH12" s="2" t="s">
+      <c r="BJ12" s="9" t="s">
+        <v>587</v>
+      </c>
+      <c r="BK12" s="9" t="s">
+        <v>686</v>
+      </c>
+      <c r="BL12" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BM12" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="BN12" s="9" t="s">
+        <v>640</v>
+      </c>
+      <c r="BO12" s="9" t="s">
+        <v>641</v>
+      </c>
+      <c r="BP12" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="BQ12" s="9" t="s">
+        <v>643</v>
+      </c>
+      <c r="BR12" s="9" t="s">
+        <v>649</v>
+      </c>
+      <c r="BS12" s="9" t="s">
+        <v>650</v>
+      </c>
+      <c r="BT12" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BI12" s="2" t="s">
+      <c r="BU12" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BJ12" s="2">
-        <v>121212</v>
-      </c>
-      <c r="BK12" s="9" t="s">
-        <v>641</v>
-      </c>
-      <c r="BL12" s="9" t="s">
-        <v>642</v>
-      </c>
-      <c r="BM12" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="BN12" s="9" t="s">
-        <v>644</v>
-      </c>
-      <c r="BO12" s="9" t="s">
-        <v>650</v>
-      </c>
-      <c r="BP12" s="9" t="s">
-        <v>651</v>
-      </c>
-      <c r="BQ12" s="9" t="s">
+      <c r="BV12" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="BR12" s="9" t="s">
+      <c r="BW12" s="9" t="s">
+        <v>654</v>
+      </c>
+      <c r="BX12" s="44" t="s">
         <v>218</v>
       </c>
-      <c r="BS12" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="BT12" s="44" t="s">
-        <v>655</v>
-      </c>
-      <c r="BU12" s="44" t="s">
-        <v>218</v>
+      <c r="BY12" s="44" t="s">
+        <v>688</v>
+      </c>
+      <c r="BZ12" s="44" t="s">
+        <v>689</v>
+      </c>
+      <c r="CA12" s="44" t="s">
+        <v>690</v>
+      </c>
+      <c r="CB12" s="44" t="s">
+        <v>691</v>
+      </c>
+      <c r="CC12" s="44" t="s">
+        <v>692</v>
+      </c>
+      <c r="CD12" s="44" t="s">
+        <v>693</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="AA12" r:id="rId1"/>
+    <hyperlink ref="AG12" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>585</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>586</v>
+      </c>
+      <c r="D2" s="2">
+        <v>110088</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>688</v>
+      </c>
+      <c r="F2" s="44" t="s">
+        <v>689</v>
+      </c>
+      <c r="G2" s="44" t="s">
+        <v>690</v>
+      </c>
+      <c r="H2" s="44" t="s">
+        <v>691</v>
+      </c>
+      <c r="I2" s="44" t="s">
+        <v>692</v>
+      </c>
+      <c r="J2" s="44" t="s">
+        <v>693</v>
+      </c>
+      <c r="K2" s="44" t="s">
+        <v>690</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>701</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R6"/>
   <sheetViews>
@@ -7090,7 +7398,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
@@ -7274,7 +7582,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q13"/>
   <sheetViews>
@@ -7412,7 +7720,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O3"/>
   <sheetViews>
@@ -7571,7 +7879,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -8631,130 +8939,130 @@
         <v>413</v>
       </c>
       <c r="DN1" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="DO1" s="4" t="s">
         <v>512</v>
       </c>
-      <c r="DO1" s="4" t="s">
+      <c r="DP1" s="4" t="s">
         <v>513</v>
       </c>
-      <c r="DP1" s="4" t="s">
+      <c r="DQ1" s="4" t="s">
         <v>514</v>
       </c>
-      <c r="DQ1" s="4" t="s">
+      <c r="DR1" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="DR1" s="4" t="s">
+      <c r="DS1" s="4" t="s">
         <v>516</v>
       </c>
-      <c r="DS1" s="4" t="s">
+      <c r="DT1" s="4" t="s">
         <v>517</v>
       </c>
-      <c r="DT1" s="4" t="s">
+      <c r="DU1" s="4" t="s">
         <v>518</v>
       </c>
-      <c r="DU1" s="4" t="s">
+      <c r="DV1" s="4" t="s">
         <v>519</v>
       </c>
-      <c r="DV1" s="4" t="s">
+      <c r="DW1" s="4" t="s">
         <v>520</v>
       </c>
-      <c r="DW1" s="4" t="s">
+      <c r="DX1" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="DX1" s="4" t="s">
+      <c r="DY1" s="4" t="s">
         <v>522</v>
       </c>
-      <c r="DY1" s="4" t="s">
+      <c r="DZ1" s="4" t="s">
         <v>523</v>
       </c>
-      <c r="DZ1" s="4" t="s">
+      <c r="EA1" s="4" t="s">
         <v>524</v>
       </c>
-      <c r="EA1" s="4" t="s">
+      <c r="EB1" s="4" t="s">
         <v>525</v>
       </c>
-      <c r="EB1" s="4" t="s">
+      <c r="EC1" s="4" t="s">
         <v>526</v>
       </c>
-      <c r="EC1" s="4" t="s">
+      <c r="ED1" s="4" t="s">
         <v>527</v>
       </c>
-      <c r="ED1" s="4" t="s">
+      <c r="EE1" s="4" t="s">
         <v>528</v>
       </c>
-      <c r="EE1" s="4" t="s">
+      <c r="EF1" s="4" t="s">
         <v>529</v>
       </c>
-      <c r="EF1" s="4" t="s">
+      <c r="EG1" s="4" t="s">
         <v>530</v>
       </c>
-      <c r="EG1" s="4" t="s">
+      <c r="EH1" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="EH1" s="4" t="s">
+      <c r="EI1" s="4" t="s">
         <v>532</v>
       </c>
-      <c r="EI1" s="4" t="s">
+      <c r="EJ1" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="EJ1" s="4" t="s">
+      <c r="EK1" s="4" t="s">
         <v>534</v>
       </c>
-      <c r="EK1" s="4" t="s">
+      <c r="EL1" s="4" t="s">
         <v>535</v>
       </c>
-      <c r="EL1" s="4" t="s">
+      <c r="EM1" s="4" t="s">
         <v>536</v>
       </c>
-      <c r="EM1" s="4" t="s">
+      <c r="EN1" s="4" t="s">
         <v>537</v>
       </c>
-      <c r="EN1" s="4" t="s">
+      <c r="EO1" s="4" t="s">
         <v>538</v>
       </c>
-      <c r="EO1" s="4" t="s">
+      <c r="EP1" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="EP1" s="4" t="s">
+      <c r="EQ1" s="4" t="s">
         <v>540</v>
       </c>
-      <c r="EQ1" s="4" t="s">
-        <v>541</v>
-      </c>
       <c r="ER1" s="5" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="ES1" s="4" t="s">
+        <v>660</v>
+      </c>
+      <c r="ET1" s="4" t="s">
         <v>661</v>
       </c>
-      <c r="ET1" s="4" t="s">
+      <c r="EU1" s="4" t="s">
         <v>662</v>
       </c>
-      <c r="EU1" s="4" t="s">
+      <c r="EV1" s="4" t="s">
         <v>663</v>
       </c>
-      <c r="EV1" s="4" t="s">
+      <c r="EW1" s="4" t="s">
         <v>664</v>
       </c>
-      <c r="EW1" s="4" t="s">
+      <c r="EX1" s="4" t="s">
         <v>665</v>
       </c>
-      <c r="EX1" s="4" t="s">
+      <c r="EY1" s="4" t="s">
         <v>666</v>
       </c>
-      <c r="EY1" s="4" t="s">
+      <c r="EZ1" s="4" t="s">
         <v>667</v>
       </c>
-      <c r="EZ1" s="4" t="s">
+      <c r="FA1" s="4" t="s">
         <v>668</v>
       </c>
-      <c r="FA1" s="4" t="s">
+      <c r="FB1" s="4" t="s">
         <v>669</v>
       </c>
-      <c r="FB1" s="4" t="s">
+      <c r="FC1" s="4" t="s">
         <v>670</v>
-      </c>
-      <c r="FC1" s="4" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="2" spans="1:159" ht="90" x14ac:dyDescent="0.25">
@@ -8762,10 +9070,10 @@
         <v>132</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>473</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>474</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>475</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>385</v>
@@ -8956,7 +9264,7 @@
         <v>391</v>
       </c>
       <c r="BR2" s="28" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="BS2" s="28"/>
       <c r="BT2" s="9"/>
@@ -9042,7 +9350,7 @@
         <v>414</v>
       </c>
       <c r="CZ2" s="9" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="DA2" s="9" t="s">
         <v>391</v>
@@ -9057,70 +9365,70 @@
         <v>416</v>
       </c>
       <c r="DE2" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="DF2" s="9" t="s">
         <v>477</v>
       </c>
-      <c r="DF2" s="9" t="s">
+      <c r="DG2" s="9" t="s">
         <v>478</v>
       </c>
-      <c r="DG2" s="9" t="s">
+      <c r="DH2" s="9" t="s">
         <v>479</v>
       </c>
-      <c r="DH2" s="9" t="s">
-        <v>480</v>
-      </c>
       <c r="DI2" s="9" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="DJ2" s="9" t="s">
         <v>418</v>
       </c>
       <c r="DK2" s="9" t="s">
+        <v>480</v>
+      </c>
+      <c r="DL2" s="9" t="s">
         <v>481</v>
       </c>
-      <c r="DL2" s="9" t="s">
+      <c r="DM2" s="9" t="s">
         <v>482</v>
       </c>
-      <c r="DM2" s="9" t="s">
+      <c r="DN2" s="9" t="s">
         <v>483</v>
       </c>
-      <c r="DN2" s="9" t="s">
+      <c r="DO2" s="9" t="s">
         <v>484</v>
       </c>
-      <c r="DO2" s="9" t="s">
+      <c r="DP2" s="9" t="s">
         <v>485</v>
-      </c>
-      <c r="DP2" s="9" t="s">
-        <v>486</v>
       </c>
       <c r="DQ2" s="9">
         <v>1234567890123450</v>
       </c>
       <c r="DR2" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="DS2" s="9" t="s">
         <v>487</v>
-      </c>
-      <c r="DS2" s="9" t="s">
-        <v>488</v>
       </c>
       <c r="DT2" s="9">
         <v>11</v>
       </c>
       <c r="DU2" s="9" t="s">
+        <v>488</v>
+      </c>
+      <c r="DV2" s="9" t="s">
         <v>489</v>
       </c>
-      <c r="DV2" s="9" t="s">
+      <c r="DW2" s="9" t="s">
         <v>490</v>
       </c>
-      <c r="DW2" s="9" t="s">
+      <c r="DX2" s="9" t="s">
         <v>491</v>
       </c>
-      <c r="DX2" s="9" t="s">
+      <c r="DY2" s="9" t="s">
         <v>492</v>
       </c>
-      <c r="DY2" s="9" t="s">
+      <c r="DZ2" s="9" t="s">
         <v>493</v>
-      </c>
-      <c r="DZ2" s="9" t="s">
-        <v>494</v>
       </c>
       <c r="EA2" s="9">
         <v>123456</v>
@@ -9135,79 +9443,79 @@
         <v>1</v>
       </c>
       <c r="EE2" s="9" t="s">
+        <v>494</v>
+      </c>
+      <c r="EF2" s="9" t="s">
         <v>495</v>
       </c>
-      <c r="EF2" s="9" t="s">
+      <c r="EG2" s="9" t="s">
         <v>496</v>
       </c>
-      <c r="EG2" s="9" t="s">
+      <c r="EH2" s="9" t="s">
         <v>497</v>
       </c>
-      <c r="EH2" s="9" t="s">
+      <c r="EI2" s="9" t="s">
         <v>498</v>
       </c>
-      <c r="EI2" s="9" t="s">
+      <c r="EJ2" s="9" t="s">
         <v>499</v>
       </c>
-      <c r="EJ2" s="9" t="s">
+      <c r="EK2" s="9" t="s">
         <v>500</v>
       </c>
-      <c r="EK2" s="9" t="s">
+      <c r="EL2" s="9" t="s">
         <v>501</v>
       </c>
-      <c r="EL2" s="9" t="s">
+      <c r="EM2" s="9" t="s">
         <v>502</v>
       </c>
-      <c r="EM2" s="9" t="s">
+      <c r="EN2" s="9" t="s">
         <v>503</v>
       </c>
-      <c r="EN2" s="9" t="s">
+      <c r="EO2" s="9" t="s">
         <v>504</v>
       </c>
-      <c r="EO2" s="9" t="s">
+      <c r="EP2" s="9" t="s">
         <v>505</v>
       </c>
-      <c r="EP2" s="9" t="s">
+      <c r="EQ2" s="9" t="s">
         <v>506</v>
       </c>
-      <c r="EQ2" s="9" t="s">
-        <v>507</v>
-      </c>
       <c r="ER2" s="45" t="s">
+        <v>671</v>
+      </c>
+      <c r="ES2" s="9" t="s">
         <v>672</v>
       </c>
-      <c r="ES2" s="9" t="s">
+      <c r="ET2" s="9" t="s">
         <v>673</v>
       </c>
-      <c r="ET2" s="9" t="s">
+      <c r="EU2" s="9" t="s">
         <v>674</v>
       </c>
-      <c r="EU2" s="9" t="s">
+      <c r="EV2" s="9" t="s">
+        <v>617</v>
+      </c>
+      <c r="EW2" s="9" t="s">
         <v>675</v>
       </c>
-      <c r="EV2" s="9" t="s">
-        <v>618</v>
-      </c>
-      <c r="EW2" s="9" t="s">
+      <c r="EX2" s="9" t="s">
         <v>676</v>
       </c>
-      <c r="EX2" s="9" t="s">
+      <c r="EY2" s="9" t="s">
         <v>677</v>
       </c>
-      <c r="EY2" s="9" t="s">
+      <c r="EZ2" s="46" t="s">
         <v>678</v>
-      </c>
-      <c r="EZ2" s="46" t="s">
-        <v>679</v>
       </c>
       <c r="FA2" s="9" t="s">
         <v>107</v>
       </c>
       <c r="FB2" s="9" t="s">
+        <v>679</v>
+      </c>
+      <c r="FC2" s="9" t="s">
         <v>680</v>
-      </c>
-      <c r="FC2" s="9" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="3" spans="1:159" ht="90" x14ac:dyDescent="0.25">
@@ -12219,19 +12527,19 @@
     </row>
     <row r="12" spans="1:159" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D12" s="9">
         <v>8520</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F12" s="9">
         <v>50</v>
@@ -12363,7 +12671,7 @@
         <v>187</v>
       </c>
       <c r="AY12" s="9" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="AZ12" s="9" t="s">
         <v>30</v>
@@ -12488,7 +12796,7 @@
         <v>188</v>
       </c>
       <c r="CV12" s="9" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="CW12" s="9" t="s">
         <v>53</v>
@@ -12518,13 +12826,13 @@
         <v>6</v>
       </c>
       <c r="DF12" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="DG12" s="9">
         <v>9</v>
       </c>
       <c r="DH12" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="DI12" s="9">
         <v>6</v>
@@ -12536,10 +12844,10 @@
         <v>3</v>
       </c>
       <c r="DL12" s="9" t="s">
+        <v>481</v>
+      </c>
+      <c r="DM12" s="9" t="s">
         <v>482</v>
-      </c>
-      <c r="DM12" s="9" t="s">
-        <v>483</v>
       </c>
       <c r="DN12" s="9">
         <v>4</v>
@@ -12554,31 +12862,31 @@
         <v>1234567890123450</v>
       </c>
       <c r="DR12" s="9" t="s">
+        <v>486</v>
+      </c>
+      <c r="DS12" s="9" t="s">
         <v>487</v>
-      </c>
-      <c r="DS12" s="9" t="s">
-        <v>488</v>
       </c>
       <c r="DT12" s="9">
         <v>11</v>
       </c>
       <c r="DU12" s="9" t="s">
+        <v>488</v>
+      </c>
+      <c r="DV12" s="9" t="s">
         <v>489</v>
       </c>
-      <c r="DV12" s="9" t="s">
+      <c r="DW12" s="9" t="s">
         <v>490</v>
       </c>
-      <c r="DW12" s="9" t="s">
+      <c r="DX12" s="9" t="s">
         <v>491</v>
       </c>
-      <c r="DX12" s="9" t="s">
+      <c r="DY12" s="9" t="s">
         <v>492</v>
       </c>
-      <c r="DY12" s="9" t="s">
+      <c r="DZ12" s="9" t="s">
         <v>493</v>
-      </c>
-      <c r="DZ12" s="9" t="s">
-        <v>494</v>
       </c>
       <c r="EA12" s="9">
         <v>123456</v>
@@ -12593,43 +12901,43 @@
         <v>1</v>
       </c>
       <c r="EE12" s="9" t="s">
+        <v>494</v>
+      </c>
+      <c r="EF12" s="9" t="s">
         <v>495</v>
       </c>
-      <c r="EF12" s="9" t="s">
+      <c r="EG12" s="9" t="s">
         <v>496</v>
       </c>
-      <c r="EG12" s="9" t="s">
+      <c r="EH12" s="9" t="s">
         <v>497</v>
       </c>
-      <c r="EH12" s="9" t="s">
+      <c r="EI12" s="9" t="s">
         <v>498</v>
       </c>
-      <c r="EI12" s="9" t="s">
+      <c r="EJ12" s="9" t="s">
         <v>499</v>
       </c>
-      <c r="EJ12" s="9" t="s">
+      <c r="EK12" s="9" t="s">
         <v>500</v>
       </c>
-      <c r="EK12" s="9" t="s">
+      <c r="EL12" s="9" t="s">
         <v>501</v>
       </c>
-      <c r="EL12" s="9" t="s">
+      <c r="EM12" s="9" t="s">
         <v>502</v>
       </c>
-      <c r="EM12" s="9" t="s">
+      <c r="EN12" s="9" t="s">
         <v>503</v>
       </c>
-      <c r="EN12" s="9" t="s">
+      <c r="EO12" s="9" t="s">
         <v>504</v>
       </c>
-      <c r="EO12" s="9" t="s">
+      <c r="EP12" s="9" t="s">
         <v>505</v>
       </c>
-      <c r="EP12" s="9" t="s">
+      <c r="EQ12" s="9" t="s">
         <v>506</v>
-      </c>
-      <c r="EQ12" s="9" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="13" spans="1:159" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added story for ATC
</commit_message>
<xml_diff>
--- a/src/main/resources/config/stageSA/TestData/TestData.xlsx
+++ b/src/main/resources/config/stageSA/TestData/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4185" uniqueCount="859">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4196" uniqueCount="869">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -2609,6 +2609,36 @@
   </si>
   <si>
     <t>load</t>
+  </si>
+  <si>
+    <t>5377162908346911</t>
+  </si>
+  <si>
+    <t>207</t>
+  </si>
+  <si>
+    <t>853</t>
+  </si>
+  <si>
+    <t>098</t>
+  </si>
+  <si>
+    <t>2812</t>
+  </si>
+  <si>
+    <t>%s</t>
+  </si>
+  <si>
+    <t>null</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>%Sale</t>
+  </si>
+  <si>
+    <t>%Load</t>
   </si>
 </sst>
 </file>
@@ -3216,9 +3246,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="55" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="18.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56" x14ac:dyDescent="0.3">
@@ -5805,7 +5835,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="34.6640625" customWidth="1"/>
+    <col min="7" max="7" customWidth="true" width="34.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -5909,9 +5939,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="30.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="32.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -5989,39 +6019,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.5546875" customWidth="1"/>
-    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="28.5546875" customWidth="1"/>
-    <col min="26" max="26" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="15" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="46" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="15" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="5.44140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="17.88671875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="19.5546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="23.5546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="23.5546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="29.33203125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="21.88671875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="19.5546875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="14.44140625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="28.88671875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="16.6640625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="13.109375" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="28.5546875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="62" max="62" bestFit="true" customWidth="true" width="20.5546875" collapsed="true"/>
+    <col min="63" max="63" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="64" max="64" bestFit="true" customWidth="true" width="21.44140625" collapsed="true"/>
+    <col min="65" max="65" bestFit="true" customWidth="true" width="18.109375" collapsed="true"/>
+    <col min="66" max="66" bestFit="true" customWidth="true" width="46.0" collapsed="true"/>
+    <col min="71" max="71" bestFit="true" customWidth="true" width="17.5546875" collapsed="true"/>
+    <col min="72" max="72" bestFit="true" customWidth="true" width="22.88671875" collapsed="true"/>
+    <col min="73" max="73" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="75" max="75" bestFit="true" customWidth="true" width="20.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:75" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -8570,7 +8600,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="51.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
@@ -8907,13 +8937,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.6640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="33" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="33" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="33" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="31"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="31" width="61.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="33" width="22.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="33" width="9.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="33" width="9.6640625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="31" width="19.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="31" width="20.44140625" collapsed="true"/>
+    <col min="7" max="16384" style="31" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -9091,22 +9121,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" style="24" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="24" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="24" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="24" customWidth="1"/>
-    <col min="5" max="5" width="15" style="24" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="24" customWidth="1"/>
-    <col min="7" max="7" width="18.88671875" style="24" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="24"/>
-    <col min="10" max="10" width="9.6640625" style="24" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" style="24" customWidth="1"/>
-    <col min="12" max="12" width="20.33203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="24" customWidth="1"/>
-    <col min="14" max="14" width="20.33203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="9.109375" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="24"/>
+    <col min="1" max="1" customWidth="true" style="24" width="29.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="24" width="22.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="24" width="9.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="24" width="9.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="24" width="15.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="24" width="14.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="24" width="18.88671875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="24" width="10.33203125" collapsed="true"/>
+    <col min="9" max="9" style="24" width="8.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="24" width="9.6640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="24" width="8.5546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="24" width="20.33203125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="24" width="11.109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" style="24" width="20.33203125" collapsed="true"/>
+    <col min="15" max="17" customWidth="true" width="9.109375" collapsed="true"/>
+    <col min="18" max="16384" style="24" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -9229,19 +9259,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.109375" style="24" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="24" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="24" customWidth="1"/>
-    <col min="4" max="5" width="15" style="24" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="24" customWidth="1"/>
-    <col min="7" max="7" width="15" style="24" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" style="24" customWidth="1"/>
-    <col min="9" max="9" width="15" style="24" customWidth="1"/>
-    <col min="10" max="12" width="9.33203125" style="24" customWidth="1"/>
-    <col min="13" max="13" width="28.6640625" style="24" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" style="24" customWidth="1"/>
-    <col min="15" max="15" width="18.6640625" style="24" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="24"/>
+    <col min="1" max="1" customWidth="true" style="24" width="29.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="24" width="9.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="24" width="9.6640625" collapsed="true"/>
+    <col min="4" max="5" customWidth="true" style="24" width="15.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="24" width="14.109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="24" width="15.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="24" width="19.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="24" width="15.0" collapsed="true"/>
+    <col min="10" max="12" customWidth="true" style="24" width="9.33203125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="24" width="28.6640625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="24" width="11.6640625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="24" width="18.6640625" collapsed="true"/>
+    <col min="16" max="16384" style="24" width="8.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -9388,15 +9418,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="38.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="25.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="17.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="10.109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="14.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
@@ -9492,74 +9522,74 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5546875" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="23.5546875" customWidth="1"/>
-    <col min="17" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="14.44140625" customWidth="1"/>
-    <col min="28" max="28" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="28.5546875" customWidth="1"/>
-    <col min="33" max="33" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="39" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="21.88671875" customWidth="1"/>
-    <col min="59" max="59" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="15.88671875" customWidth="1"/>
-    <col min="61" max="61" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="17.5546875" customWidth="1"/>
-    <col min="69" max="69" width="15" customWidth="1"/>
-    <col min="71" max="71" width="19.6640625" customWidth="1"/>
-    <col min="72" max="72" width="12.88671875" customWidth="1"/>
-    <col min="73" max="73" width="16.6640625" customWidth="1"/>
-    <col min="74" max="74" width="17.109375" customWidth="1"/>
-    <col min="75" max="75" width="12.88671875" customWidth="1"/>
-    <col min="76" max="76" width="15.88671875" customWidth="1"/>
-    <col min="77" max="77" width="14.109375" style="24" customWidth="1"/>
-    <col min="78" max="78" width="15" style="24" customWidth="1"/>
-    <col min="79" max="79" width="19.33203125" style="24" customWidth="1"/>
-    <col min="80" max="80" width="15" style="24" customWidth="1"/>
-    <col min="81" max="83" width="9.33203125" style="24" customWidth="1"/>
-    <col min="84" max="84" width="8.88671875" style="24" customWidth="1"/>
-    <col min="85" max="85" width="10.5546875" style="24" customWidth="1"/>
-    <col min="86" max="86" width="18.6640625" style="24" customWidth="1"/>
-    <col min="87" max="87" width="16.88671875" style="24" customWidth="1"/>
-    <col min="88" max="88" width="10.33203125" style="24" customWidth="1"/>
-    <col min="89" max="89" width="16.88671875" style="24" customWidth="1"/>
-    <col min="90" max="90" width="9.44140625" style="24" customWidth="1"/>
-    <col min="91" max="91" width="14.44140625" style="24" customWidth="1"/>
-    <col min="92" max="92" width="10.33203125" style="24" customWidth="1"/>
-    <col min="93" max="93" width="17.6640625" style="24" customWidth="1"/>
-    <col min="94" max="94" width="16.109375" style="24" customWidth="1"/>
-    <col min="95" max="95" width="18.44140625" style="24" customWidth="1"/>
-    <col min="97" max="97" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="40.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="17.33203125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="6.44140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="17.88671875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="19.5546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="23.5546875" collapsed="true"/>
+    <col min="15" max="16" customWidth="true" width="23.5546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="19.33203125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="29.33203125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="21.88671875" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="19.5546875" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="23.109375" collapsed="true"/>
+    <col min="25" max="27" customWidth="true" width="14.44140625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="28.88671875" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="16.6640625" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="21.88671875" collapsed="true"/>
+    <col min="32" max="32" customWidth="true" width="28.5546875" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="9.33203125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="36" max="39" bestFit="true" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="10.88671875" collapsed="true"/>
+    <col min="48" max="48" bestFit="true" customWidth="true" width="17.6640625" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" width="22.109375" collapsed="true"/>
+    <col min="55" max="55" bestFit="true" customWidth="true" width="23.109375" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="57" max="57" bestFit="true" customWidth="true" width="21.88671875" collapsed="true"/>
+    <col min="58" max="58" customWidth="true" width="21.88671875" collapsed="true"/>
+    <col min="59" max="59" bestFit="true" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="60" max="60" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="61" max="61" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="63" max="63" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="64" max="64" bestFit="true" customWidth="true" width="22.109375" collapsed="true"/>
+    <col min="68" max="68" customWidth="true" width="17.5546875" collapsed="true"/>
+    <col min="69" max="69" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="71" max="71" customWidth="true" width="19.6640625" collapsed="true"/>
+    <col min="72" max="72" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="73" max="73" customWidth="true" width="16.6640625" collapsed="true"/>
+    <col min="74" max="74" customWidth="true" width="17.109375" collapsed="true"/>
+    <col min="75" max="75" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="76" max="76" customWidth="true" width="15.88671875" collapsed="true"/>
+    <col min="77" max="77" customWidth="true" style="24" width="14.109375" collapsed="true"/>
+    <col min="78" max="78" customWidth="true" style="24" width="15.0" collapsed="true"/>
+    <col min="79" max="79" customWidth="true" style="24" width="19.33203125" collapsed="true"/>
+    <col min="80" max="80" customWidth="true" style="24" width="15.0" collapsed="true"/>
+    <col min="81" max="83" customWidth="true" style="24" width="9.33203125" collapsed="true"/>
+    <col min="84" max="84" customWidth="true" style="24" width="8.88671875" collapsed="true"/>
+    <col min="85" max="85" customWidth="true" style="24" width="10.5546875" collapsed="true"/>
+    <col min="86" max="86" customWidth="true" style="24" width="18.6640625" collapsed="true"/>
+    <col min="87" max="87" customWidth="true" style="24" width="16.88671875" collapsed="true"/>
+    <col min="88" max="88" customWidth="true" style="24" width="10.33203125" collapsed="true"/>
+    <col min="89" max="89" customWidth="true" style="24" width="16.88671875" collapsed="true"/>
+    <col min="90" max="90" customWidth="true" style="24" width="9.44140625" collapsed="true"/>
+    <col min="91" max="91" customWidth="true" style="24" width="14.44140625" collapsed="true"/>
+    <col min="92" max="92" customWidth="true" style="24" width="10.33203125" collapsed="true"/>
+    <col min="93" max="93" customWidth="true" style="24" width="17.6640625" collapsed="true"/>
+    <col min="94" max="94" customWidth="true" style="24" width="16.109375" collapsed="true"/>
+    <col min="95" max="95" customWidth="true" style="24" width="18.44140625" collapsed="true"/>
+    <col min="97" max="97" customWidth="true" width="11.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:97" s="47" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -13023,6 +13053,44 @@
         <v>858</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2" t="s">
+        <v>865</v>
+      </c>
+      <c r="E2" t="s">
+        <v>859</v>
+      </c>
+      <c r="F2" t="s">
+        <v>861</v>
+      </c>
+      <c r="G2" t="s">
+        <v>860</v>
+      </c>
+      <c r="H2" t="s">
+        <v>862</v>
+      </c>
+      <c r="I2" t="s">
+        <v>391</v>
+      </c>
+      <c r="J2" t="s">
+        <v>863</v>
+      </c>
+      <c r="K2" t="s">
+        <v>864</v>
+      </c>
+      <c r="L2" t="s">
+        <v>866</v>
+      </c>
+      <c r="M2" t="s">
+        <v>867</v>
+      </c>
+      <c r="N2" t="s">
+        <v>868</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13038,13 +13106,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="56.109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.5546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.5546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="21.109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.44140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.88671875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:143" ht="57.6" x14ac:dyDescent="0.3">
@@ -14660,15 +14728,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.5546875" customWidth="1"/>
-    <col min="2" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1"/>
-    <col min="11" max="11" width="25.33203125" customWidth="1"/>
-    <col min="12" max="13" width="15.5546875" customWidth="1"/>
-    <col min="15" max="15" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="44.5546875" collapsed="true"/>
+    <col min="2" max="6" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="11.88671875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="25.33203125" collapsed="true"/>
+    <col min="12" max="13" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="12.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" ht="57.6" x14ac:dyDescent="0.3">
@@ -15240,17 +15308,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.109375" customWidth="1"/>
-    <col min="2" max="2" width="21.5546875" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="19" max="19" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="7.44140625" customWidth="1"/>
-    <col min="66" max="66" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="17.5546875" customWidth="1"/>
-    <col min="97" max="97" width="10.6640625" style="4" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="37.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="17.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="20.6640625" collapsed="true"/>
+    <col min="49" max="49" customWidth="true" width="7.44140625" collapsed="true"/>
+    <col min="66" max="66" bestFit="true" customWidth="true" width="14.109375" collapsed="true"/>
+    <col min="67" max="67" customWidth="true" width="17.5546875" collapsed="true"/>
+    <col min="97" max="97" customWidth="true" style="4" width="10.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:159" ht="57.6" x14ac:dyDescent="0.3">
@@ -20254,12 +20322,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="43.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -20414,14 +20482,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="52" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.6640625" customWidth="1"/>
-    <col min="17" max="17" width="47" customWidth="1"/>
-    <col min="18" max="18" width="37.6640625" customWidth="1"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="52.0" collapsed="true"/>
+    <col min="9" max="10" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="20.6640625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="47.0" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="37.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.3">
@@ -20743,8 +20811,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.88671875" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="35.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -20820,7 +20888,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="9" max="9" customWidth="true" width="16.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added code for Inactivated Device range
</commit_message>
<xml_diff>
--- a/src/main/resources/config/stageSA/TestData/TestData.xlsx
+++ b/src/main/resources/config/stageSA/TestData/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4209" uniqueCount="876">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4223" uniqueCount="880">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -2620,9 +2620,6 @@
     <t>Active</t>
   </si>
   <si>
-    <t>magnetic stripe card</t>
-  </si>
-  <si>
     <t>ScenarioID</t>
   </si>
   <si>
@@ -2660,6 +2657,21 @@
   </si>
   <si>
     <t>%Load</t>
+  </si>
+  <si>
+    <t>5377164381219417</t>
+  </si>
+  <si>
+    <t>597</t>
+  </si>
+  <si>
+    <t>441</t>
+  </si>
+  <si>
+    <t>ClearPin</t>
+  </si>
+  <si>
+    <t>8862</t>
   </si>
 </sst>
 </file>
@@ -3267,9 +3279,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56" x14ac:dyDescent="0.25">
@@ -5856,7 +5868,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="7" max="7" width="34.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -5960,9 +5972,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="32.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6040,39 +6052,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="5.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="29.28515625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="28.85546875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="62" max="62" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
-    <col min="63" max="63" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="64" max="64" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
-    <col min="65" max="65" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="66" max="66" bestFit="true" customWidth="true" width="46.0" collapsed="true"/>
-    <col min="71" max="71" bestFit="true" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="72" max="72" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
-    <col min="73" max="73" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="75" max="75" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="1" max="1" width="37" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="23.5703125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="28.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="28.5703125" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="46" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="72" max="72" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="73" max="73" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="75" max="75" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:75" s="31" customFormat="1" x14ac:dyDescent="0.25">
@@ -8621,7 +8633,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="51.5703125" collapsed="true"/>
+    <col min="1" max="1" width="51.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -8958,13 +8970,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="31" width="61.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="33" width="22.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="33" width="9.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="33" width="9.7109375" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="31" width="19.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="31" width="20.42578125" collapsed="true"/>
-    <col min="7" max="16384" style="31" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="61.7109375" style="31" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.7109375" style="33" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.28515625" style="33" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.7109375" style="33" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.28515625" style="31" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.42578125" style="31" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="8.85546875" style="31" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -9142,22 +9154,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="24" width="29.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="24" width="22.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="24" width="9.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="24" width="9.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="24" width="15.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="24" width="14.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="24" width="18.85546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="24" width="10.28515625" collapsed="true"/>
-    <col min="9" max="9" style="24" width="8.85546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="24" width="9.7109375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="24" width="8.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="24" width="20.28515625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="24" width="11.140625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="24" width="20.28515625" collapsed="true"/>
-    <col min="15" max="17" customWidth="true" width="9.140625" collapsed="true"/>
-    <col min="18" max="16384" style="24" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="29.7109375" style="24" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.7109375" style="24" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.28515625" style="24" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9.7109375" style="24" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15" style="24" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.7109375" style="24" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18.85546875" style="24" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.28515625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="8.85546875" style="24" collapsed="1"/>
+    <col min="10" max="10" width="9.7109375" style="24" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="8.5703125" style="24" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="20.28515625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="11.140625" style="24" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="20.28515625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="17" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="18" max="16384" width="8.85546875" style="24" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -9280,19 +9292,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="24" width="29.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="24" width="9.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="24" width="9.7109375" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" style="24" width="15.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="24" width="14.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="24" width="15.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="24" width="19.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="24" width="15.0" collapsed="true"/>
-    <col min="10" max="12" customWidth="true" style="24" width="9.28515625" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="24" width="28.7109375" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="24" width="11.7109375" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="24" width="18.7109375" collapsed="true"/>
-    <col min="16" max="16384" style="24" width="8.85546875" collapsed="true"/>
+    <col min="1" max="1" width="29.140625" style="24" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.28515625" style="24" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.7109375" style="24" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="15" style="24" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="14.140625" style="24" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="15" style="24" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.28515625" style="24" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="15" style="24" customWidth="1" collapsed="1"/>
+    <col min="10" max="12" width="9.28515625" style="24" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="28.7109375" style="24" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.7109375" style="24" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="18.7109375" style="24" customWidth="1" collapsed="1"/>
+    <col min="16" max="16384" width="8.85546875" style="24" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -9439,15 +9451,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="38.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="25.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="1" max="1" width="38.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="19" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -9543,74 +9555,74 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="40.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="15" max="16" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="29.28515625" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="25" max="27" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="28.85546875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="32" max="32" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="36" max="39" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="58" max="58" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="60" max="60" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="61" max="61" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="63" max="63" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="64" max="64" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="68" max="68" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="69" max="69" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="71" max="71" customWidth="true" width="19.7109375" collapsed="true"/>
-    <col min="72" max="72" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="73" max="73" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="74" max="74" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="75" max="75" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="76" max="76" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="77" max="77" customWidth="true" style="24" width="14.140625" collapsed="true"/>
-    <col min="78" max="78" customWidth="true" style="24" width="15.0" collapsed="true"/>
-    <col min="79" max="79" customWidth="true" style="24" width="19.28515625" collapsed="true"/>
-    <col min="80" max="80" customWidth="true" style="24" width="15.0" collapsed="true"/>
-    <col min="81" max="83" customWidth="true" style="24" width="9.28515625" collapsed="true"/>
-    <col min="84" max="84" customWidth="true" style="24" width="8.85546875" collapsed="true"/>
-    <col min="85" max="85" customWidth="true" style="24" width="10.5703125" collapsed="true"/>
-    <col min="86" max="86" customWidth="true" style="24" width="18.7109375" collapsed="true"/>
-    <col min="87" max="87" customWidth="true" style="24" width="16.85546875" collapsed="true"/>
-    <col min="88" max="88" customWidth="true" style="24" width="10.28515625" collapsed="true"/>
-    <col min="89" max="89" customWidth="true" style="24" width="16.85546875" collapsed="true"/>
-    <col min="90" max="90" customWidth="true" style="24" width="9.42578125" collapsed="true"/>
-    <col min="91" max="91" customWidth="true" style="24" width="14.42578125" collapsed="true"/>
-    <col min="92" max="92" customWidth="true" style="24" width="10.28515625" collapsed="true"/>
-    <col min="93" max="93" customWidth="true" style="24" width="17.7109375" collapsed="true"/>
-    <col min="94" max="94" customWidth="true" style="24" width="16.140625" collapsed="true"/>
-    <col min="95" max="95" customWidth="true" style="24" width="18.42578125" collapsed="true"/>
-    <col min="97" max="97" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="6" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="16" width="23.5703125" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="27" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="28.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="28.5703125" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="39" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="68" max="68" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="69" max="69" width="15" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="19.7109375" customWidth="1" collapsed="1"/>
+    <col min="72" max="72" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="73" max="73" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="74" max="74" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="75" max="75" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="76" max="76" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="77" max="77" width="14.140625" style="24" customWidth="1" collapsed="1"/>
+    <col min="78" max="78" width="15" style="24" customWidth="1" collapsed="1"/>
+    <col min="79" max="79" width="19.28515625" style="24" customWidth="1" collapsed="1"/>
+    <col min="80" max="80" width="15" style="24" customWidth="1" collapsed="1"/>
+    <col min="81" max="83" width="9.28515625" style="24" customWidth="1" collapsed="1"/>
+    <col min="84" max="84" width="8.85546875" style="24" customWidth="1" collapsed="1"/>
+    <col min="85" max="85" width="10.5703125" style="24" customWidth="1" collapsed="1"/>
+    <col min="86" max="86" width="18.7109375" style="24" customWidth="1" collapsed="1"/>
+    <col min="87" max="87" width="16.85546875" style="24" customWidth="1" collapsed="1"/>
+    <col min="88" max="88" width="10.28515625" style="24" customWidth="1" collapsed="1"/>
+    <col min="89" max="89" width="16.85546875" style="24" customWidth="1" collapsed="1"/>
+    <col min="90" max="90" width="9.42578125" style="24" customWidth="1" collapsed="1"/>
+    <col min="91" max="91" width="14.42578125" style="24" customWidth="1" collapsed="1"/>
+    <col min="92" max="92" width="10.28515625" style="24" customWidth="1" collapsed="1"/>
+    <col min="93" max="93" width="17.7109375" style="24" customWidth="1" collapsed="1"/>
+    <col min="94" max="94" width="16.140625" style="24" customWidth="1" collapsed="1"/>
+    <col min="95" max="95" width="18.42578125" style="24" customWidth="1" collapsed="1"/>
+    <col min="97" max="97" width="11.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:97" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -13022,34 +13034,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="4.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="5.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="5.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="4.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="5.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.28515625" customWidth="1"/>
+    <col min="14" max="14" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="4.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="68" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B1" s="68" t="s">
         <v>847</v>
@@ -13085,25 +13098,25 @@
         <v>856</v>
       </c>
       <c r="M1" s="68" t="s">
+        <v>878</v>
+      </c>
+      <c r="N1" s="68" t="s">
         <v>242</v>
       </c>
-      <c r="N1" s="68" t="s">
+      <c r="O1" s="68" t="s">
         <v>857</v>
       </c>
-      <c r="O1" s="68" t="s">
+      <c r="P1" s="68" t="s">
         <v>858</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>863</v>
+      </c>
+      <c r="B2" t="s">
         <v>864</v>
       </c>
-      <c r="B2" t="s">
-        <v>862</v>
-      </c>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
       <c r="F2" s="69" t="s">
         <v>859</v>
       </c>
@@ -13114,93 +13127,112 @@
         <v>615</v>
       </c>
       <c r="I2" s="69" t="s">
-        <v>866</v>
-      </c>
-      <c r="J2"/>
+        <v>865</v>
+      </c>
       <c r="K2">
         <v>2812</v>
       </c>
       <c r="L2" t="s">
         <v>860</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="69" t="s">
+        <v>879</v>
+      </c>
+      <c r="N2" t="s">
         <v>861</v>
       </c>
-      <c r="N2"/>
-      <c r="O2"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>864</v>
       </c>
-      <c r="B3" t="s">
-        <v>865</v>
-      </c>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3" s="69" t="s">
-        <v>859</v>
-      </c>
-      <c r="G3">
-        <v>546</v>
-      </c>
-      <c r="H3">
-        <v>615</v>
-      </c>
-      <c r="I3" s="69" t="s">
+      <c r="E3" t="s">
+        <v>872</v>
+      </c>
+      <c r="F3" t="s">
         <v>866</v>
       </c>
-      <c r="J3"/>
-      <c r="K3">
-        <v>2812</v>
+      <c r="G3" t="s">
+        <v>868</v>
+      </c>
+      <c r="H3" t="s">
+        <v>867</v>
+      </c>
+      <c r="I3" t="s">
+        <v>869</v>
+      </c>
+      <c r="J3" t="s">
+        <v>391</v>
+      </c>
+      <c r="K3" t="s">
+        <v>870</v>
       </c>
       <c r="L3" t="s">
-        <v>860</v>
-      </c>
-      <c r="M3" t="s">
+        <v>871</v>
+      </c>
+      <c r="N3" t="s">
         <v>861</v>
       </c>
-      <c r="N3"/>
-      <c r="O3"/>
-    </row>
-    <row r="4">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4" t="s">
+      <c r="O3" t="s">
         <v>873</v>
       </c>
+      <c r="P3" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>864</v>
+      </c>
       <c r="F4" t="s">
-        <v>867</v>
+        <v>875</v>
       </c>
       <c r="G4" t="s">
-        <v>869</v>
+        <v>877</v>
       </c>
       <c r="H4" t="s">
-        <v>868</v>
-      </c>
-      <c r="I4" t="s">
+        <v>876</v>
+      </c>
+      <c r="N4" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>864</v>
+      </c>
+      <c r="E5" t="s">
+        <v>872</v>
+      </c>
+      <c r="F5" t="s">
+        <v>875</v>
+      </c>
+      <c r="G5" t="s">
+        <v>877</v>
+      </c>
+      <c r="H5" t="s">
+        <v>876</v>
+      </c>
+      <c r="I5" t="s">
+        <v>872</v>
+      </c>
+      <c r="J5" t="s">
+        <v>872</v>
+      </c>
+      <c r="K5" t="s">
         <v>870</v>
       </c>
-      <c r="J4" t="s">
-        <v>391</v>
-      </c>
-      <c r="K4" t="s">
+      <c r="L5" t="s">
         <v>871</v>
       </c>
-      <c r="L4" t="s">
-        <v>872</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="N5" t="s">
         <v>861</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O5" t="s">
+        <v>873</v>
+      </c>
+      <c r="P5" t="s">
         <v>874</v>
-      </c>
-      <c r="O4" t="s">
-        <v>875</v>
       </c>
     </row>
   </sheetData>
@@ -13219,13 +13251,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="56.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="1" max="1" width="35" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="56.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:143" ht="60" x14ac:dyDescent="0.25">
@@ -14841,15 +14873,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="44.5703125" collapsed="true"/>
-    <col min="2" max="6" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="12" max="13" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="1" max="1" width="44.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="6" width="15" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="12" max="13" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" ht="60" x14ac:dyDescent="0.25">
@@ -15421,17 +15453,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="49" max="49" customWidth="true" width="7.42578125" collapsed="true"/>
-    <col min="66" max="66" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="67" max="67" customWidth="true" width="17.5703125" collapsed="true"/>
-    <col min="97" max="97" customWidth="true" style="4" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="37.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="7.42578125" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="17.5703125" customWidth="1" collapsed="1"/>
+    <col min="97" max="97" width="10.7109375" style="4" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:159" ht="60" x14ac:dyDescent="0.25">
@@ -20435,12 +20467,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="43.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="22.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="1" max="1" width="43.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
@@ -20595,14 +20627,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="52.0" collapsed="true"/>
-    <col min="9" max="10" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="20.7109375" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="47.0" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="7" max="7" width="52" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="47" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="37.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.25">
@@ -20924,8 +20956,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="35.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="1" max="1" width="35.85546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -21001,7 +21033,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="9" max="9" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="9" max="9" width="16" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
copied from original branch
</commit_message>
<xml_diff>
--- a/src/main/resources/config/stageSA/TestData/TestData.xlsx
+++ b/src/main/resources/config/stageSA/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15105" windowHeight="8985" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15108" windowHeight="8988" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CardHolder" sheetId="19" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4223" uniqueCount="880">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4185" uniqueCount="859">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -2609,69 +2609,6 @@
   </si>
   <si>
     <t>load</t>
-  </si>
-  <si>
-    <t>5377169900945210</t>
-  </si>
-  <si>
-    <t>16928FFFFFFFFFFF</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>ScenarioID</t>
-  </si>
-  <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>EMV</t>
-  </si>
-  <si>
-    <t>020</t>
-  </si>
-  <si>
-    <t>5377161157986716</t>
-  </si>
-  <si>
-    <t>660</t>
-  </si>
-  <si>
-    <t>163</t>
-  </si>
-  <si>
-    <t>080</t>
-  </si>
-  <si>
-    <t>2812</t>
-  </si>
-  <si>
-    <t>%s</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>%Sale</t>
-  </si>
-  <si>
-    <t>%Load</t>
-  </si>
-  <si>
-    <t>5377164381219417</t>
-  </si>
-  <si>
-    <t>597</t>
-  </si>
-  <si>
-    <t>441</t>
-  </si>
-  <si>
-    <t>ClearPin</t>
-  </si>
-  <si>
-    <t>8862</t>
   </si>
 </sst>
 </file>
@@ -2966,7 +2903,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
@@ -3277,14 +3214,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="55" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="18.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="55" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A1" s="52" t="s">
         <v>1</v>
       </c>
@@ -3454,7 +3391,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A2" s="58" t="s">
         <v>783</v>
       </c>
@@ -3548,7 +3485,7 @@
       <c r="BC2" s="58"/>
       <c r="BD2" s="58"/>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>794</v>
       </c>
@@ -3622,7 +3559,7 @@
       <c r="BC3" s="2"/>
       <c r="BD3" s="2"/>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>795</v>
       </c>
@@ -3696,7 +3633,7 @@
       <c r="BC4" s="2"/>
       <c r="BD4" s="2"/>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>797</v>
       </c>
@@ -3786,7 +3723,7 @@
       <c r="BC5" s="2"/>
       <c r="BD5" s="2"/>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>802</v>
       </c>
@@ -3860,7 +3797,7 @@
       <c r="BC6" s="2"/>
       <c r="BD6" s="2"/>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>803</v>
       </c>
@@ -3940,7 +3877,7 @@
       <c r="BC7" s="2"/>
       <c r="BD7" s="2"/>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>806</v>
       </c>
@@ -4024,7 +3961,7 @@
       <c r="BC8" s="2"/>
       <c r="BD8" s="2"/>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>809</v>
       </c>
@@ -4116,7 +4053,7 @@
       <c r="BC9" s="2"/>
       <c r="BD9" s="2"/>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>814</v>
       </c>
@@ -4208,7 +4145,7 @@
       <c r="BC10" s="2"/>
       <c r="BD10" s="2"/>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>815</v>
       </c>
@@ -4306,7 +4243,7 @@
       <c r="BC11" s="2"/>
       <c r="BD11" s="2"/>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>818</v>
       </c>
@@ -4404,7 +4341,7 @@
       <c r="BC12" s="2"/>
       <c r="BD12" s="2"/>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>820</v>
       </c>
@@ -4504,7 +4441,7 @@
       <c r="BC13" s="2"/>
       <c r="BD13" s="2"/>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>822</v>
       </c>
@@ -4604,7 +4541,7 @@
       <c r="BC14" s="2"/>
       <c r="BD14" s="2"/>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>823</v>
       </c>
@@ -4704,7 +4641,7 @@
       <c r="BC15" s="2"/>
       <c r="BD15" s="2"/>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>824</v>
       </c>
@@ -4808,7 +4745,7 @@
       <c r="BC16" s="2"/>
       <c r="BD16" s="2"/>
     </row>
-    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A17" s="58" t="s">
         <v>835</v>
       </c>
@@ -4916,7 +4853,7 @@
       <c r="BC17" s="58"/>
       <c r="BD17" s="58"/>
     </row>
-    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>836</v>
       </c>
@@ -5024,7 +4961,7 @@
       <c r="BC18" s="2"/>
       <c r="BD18" s="2"/>
     </row>
-    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>837</v>
       </c>
@@ -5132,7 +5069,7 @@
       <c r="BC19" s="2"/>
       <c r="BD19" s="2"/>
     </row>
-    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>838</v>
       </c>
@@ -5240,7 +5177,7 @@
       <c r="BC20" s="2"/>
       <c r="BD20" s="2"/>
     </row>
-    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>839</v>
       </c>
@@ -5314,7 +5251,7 @@
       <c r="BC21" s="2"/>
       <c r="BD21" s="2"/>
     </row>
-    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>840</v>
       </c>
@@ -5388,7 +5325,7 @@
       <c r="BC22" s="2"/>
       <c r="BD22" s="2"/>
     </row>
-    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>841</v>
       </c>
@@ -5462,7 +5399,7 @@
       <c r="BC23" s="2"/>
       <c r="BD23" s="2"/>
     </row>
-    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>842</v>
       </c>
@@ -5536,7 +5473,7 @@
       <c r="BC24" s="2"/>
       <c r="BD24" s="2"/>
     </row>
-    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>843</v>
       </c>
@@ -5610,7 +5547,7 @@
       <c r="BC25" s="2"/>
       <c r="BD25" s="2"/>
     </row>
-    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>844</v>
       </c>
@@ -5684,7 +5621,7 @@
       <c r="BC26" s="2"/>
       <c r="BD26" s="2"/>
     </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>845</v>
       </c>
@@ -5758,7 +5695,7 @@
       <c r="BC27" s="2"/>
       <c r="BD27" s="2"/>
     </row>
-    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:56" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>846</v>
       </c>
@@ -5866,12 +5803,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="34.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -5894,7 +5831,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>254</v>
       </c>
@@ -5917,7 +5854,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>258</v>
       </c>
@@ -5938,7 +5875,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>260</v>
       </c>
@@ -5970,14 +5907,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="15.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="30.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -5997,7 +5934,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>244</v>
       </c>
@@ -6017,7 +5954,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>248</v>
       </c>
@@ -6050,44 +5987,44 @@
       <selection activeCell="BV5" sqref="BV5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="23.5703125" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="28.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="28.5703125" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="64" max="64" width="21.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="65" max="65" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="66" max="66" width="46" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="17.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="72" max="72" width="22.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="73" max="73" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="75" max="75" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.5546875" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.5546875" customWidth="1"/>
+    <col min="26" max="26" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="15" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="46" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="15" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:75" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -6314,7 +6251,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="2" spans="1:75" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:75" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>440</v>
       </c>
@@ -6523,7 +6460,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="3" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>454</v>
       </c>
@@ -6730,7 +6667,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="4" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>456</v>
       </c>
@@ -6937,7 +6874,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="5" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>458</v>
       </c>
@@ -7146,7 +7083,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="6" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>461</v>
       </c>
@@ -7355,7 +7292,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="7" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>463</v>
       </c>
@@ -7564,7 +7501,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="8" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>465</v>
       </c>
@@ -7777,7 +7714,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="9" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>467</v>
       </c>
@@ -7984,7 +7921,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="10" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>469</v>
       </c>
@@ -8191,7 +8128,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="11" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>471</v>
       </c>
@@ -8400,7 +8337,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="12" spans="1:75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:75" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>473</v>
       </c>
@@ -8631,12 +8568,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="51.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="51.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -8690,7 +8627,7 @@
       </c>
       <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:18" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>287</v>
       </c>
@@ -8743,7 +8680,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>288</v>
       </c>
@@ -8796,7 +8733,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>289</v>
       </c>
@@ -8849,7 +8786,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>290</v>
       </c>
@@ -8902,7 +8839,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>291</v>
       </c>
@@ -8968,18 +8905,18 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.7109375" style="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.7109375" style="33" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.28515625" style="33" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.7109375" style="33" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.28515625" style="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.42578125" style="31" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="8.85546875" style="31" collapsed="1"/>
+    <col min="1" max="1" width="61.6640625" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="33" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="33" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="33" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -8999,7 +8936,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
         <v>368</v>
       </c>
@@ -9019,7 +8956,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>369</v>
       </c>
@@ -9039,7 +8976,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
         <v>376</v>
       </c>
@@ -9059,7 +8996,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
         <v>370</v>
       </c>
@@ -9079,7 +9016,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="31" t="s">
         <v>371</v>
       </c>
@@ -9099,7 +9036,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="31" t="s">
         <v>372</v>
       </c>
@@ -9119,7 +9056,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="31" t="s">
         <v>373</v>
       </c>
@@ -9152,27 +9089,27 @@
       <selection activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" style="24" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.7109375" style="24" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.28515625" style="24" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.7109375" style="24" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15" style="24" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.7109375" style="24" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="18.85546875" style="24" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.28515625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="8.85546875" style="24" collapsed="1"/>
-    <col min="10" max="10" width="9.7109375" style="24" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="8.5703125" style="24" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="20.28515625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="11.140625" style="24" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.28515625" style="24" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="17" width="9.140625" customWidth="1" collapsed="1"/>
-    <col min="18" max="16384" width="8.85546875" style="24" collapsed="1"/>
+    <col min="1" max="1" width="29.6640625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="24" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="24" customWidth="1"/>
+    <col min="5" max="5" width="15" style="24" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="24" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" style="24" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="24"/>
+    <col min="10" max="10" width="9.6640625" style="24" customWidth="1"/>
+    <col min="11" max="11" width="8.5546875" style="24" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="24" customWidth="1"/>
+    <col min="14" max="14" width="20.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="9.109375" customWidth="1"/>
+    <col min="18" max="16384" width="8.88671875" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
@@ -9219,7 +9156,7 @@
       <c r="P1" s="24"/>
       <c r="Q1" s="24"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>303</v>
       </c>
@@ -9262,17 +9199,17 @@
       <c r="P2" s="24"/>
       <c r="Q2" s="24"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="O3" s="24"/>
       <c r="P3" s="24"/>
       <c r="Q3" s="24"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="O4" s="24"/>
       <c r="P4" s="24"/>
       <c r="Q4" s="24"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="O13" s="24"/>
       <c r="P13" s="24"/>
       <c r="Q13" s="24"/>
@@ -9290,24 +9227,24 @@
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.140625" style="24" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9.28515625" style="24" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.7109375" style="24" customWidth="1" collapsed="1"/>
-    <col min="4" max="5" width="15" style="24" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="14.140625" style="24" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="15" style="24" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.28515625" style="24" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="15" style="24" customWidth="1" collapsed="1"/>
-    <col min="10" max="12" width="9.28515625" style="24" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="28.7109375" style="24" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="11.7109375" style="24" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.7109375" style="24" customWidth="1" collapsed="1"/>
-    <col min="16" max="16384" width="8.85546875" style="24" collapsed="1"/>
+    <col min="1" max="1" width="29.109375" style="24" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="24" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="24" customWidth="1"/>
+    <col min="4" max="5" width="15" style="24" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="24" customWidth="1"/>
+    <col min="7" max="7" width="15" style="24" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" style="24" customWidth="1"/>
+    <col min="9" max="9" width="15" style="24" customWidth="1"/>
+    <col min="10" max="12" width="9.33203125" style="24" customWidth="1"/>
+    <col min="13" max="13" width="28.6640625" style="24" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" style="24" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" style="24" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
@@ -9354,7 +9291,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>320</v>
       </c>
@@ -9395,7 +9332,7 @@
       <c r="N2" s="25"/>
       <c r="O2" s="25"/>
     </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="25" t="s">
         <v>326</v>
       </c>
@@ -9449,20 +9386,20 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="19" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
@@ -9497,7 +9434,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
         <v>331</v>
       </c>
@@ -9553,79 +9490,79 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="23.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="16" width="23.5703125" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="27" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="28.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="28.5703125" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="39" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="17.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="21.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="61" max="61" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="64" max="64" width="22.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="68" max="68" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="69" max="69" width="15" customWidth="1" collapsed="1"/>
-    <col min="71" max="71" width="19.7109375" customWidth="1" collapsed="1"/>
-    <col min="72" max="72" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="73" max="73" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="74" max="74" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="75" max="75" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="76" max="76" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="77" max="77" width="14.140625" style="24" customWidth="1" collapsed="1"/>
-    <col min="78" max="78" width="15" style="24" customWidth="1" collapsed="1"/>
-    <col min="79" max="79" width="19.28515625" style="24" customWidth="1" collapsed="1"/>
-    <col min="80" max="80" width="15" style="24" customWidth="1" collapsed="1"/>
-    <col min="81" max="83" width="9.28515625" style="24" customWidth="1" collapsed="1"/>
-    <col min="84" max="84" width="8.85546875" style="24" customWidth="1" collapsed="1"/>
-    <col min="85" max="85" width="10.5703125" style="24" customWidth="1" collapsed="1"/>
-    <col min="86" max="86" width="18.7109375" style="24" customWidth="1" collapsed="1"/>
-    <col min="87" max="87" width="16.85546875" style="24" customWidth="1" collapsed="1"/>
-    <col min="88" max="88" width="10.28515625" style="24" customWidth="1" collapsed="1"/>
-    <col min="89" max="89" width="16.85546875" style="24" customWidth="1" collapsed="1"/>
-    <col min="90" max="90" width="9.42578125" style="24" customWidth="1" collapsed="1"/>
-    <col min="91" max="91" width="14.42578125" style="24" customWidth="1" collapsed="1"/>
-    <col min="92" max="92" width="10.28515625" style="24" customWidth="1" collapsed="1"/>
-    <col min="93" max="93" width="17.7109375" style="24" customWidth="1" collapsed="1"/>
-    <col min="94" max="94" width="16.140625" style="24" customWidth="1" collapsed="1"/>
-    <col min="95" max="95" width="18.42578125" style="24" customWidth="1" collapsed="1"/>
-    <col min="97" max="97" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="40.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="23.5546875" customWidth="1"/>
+    <col min="17" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="14.44140625" customWidth="1"/>
+    <col min="28" max="28" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="28.5546875" customWidth="1"/>
+    <col min="33" max="33" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="39" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="21.88671875" customWidth="1"/>
+    <col min="59" max="59" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="15.88671875" customWidth="1"/>
+    <col min="61" max="61" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="17.5546875" customWidth="1"/>
+    <col min="69" max="69" width="15" customWidth="1"/>
+    <col min="71" max="71" width="19.6640625" customWidth="1"/>
+    <col min="72" max="72" width="12.88671875" customWidth="1"/>
+    <col min="73" max="73" width="16.6640625" customWidth="1"/>
+    <col min="74" max="74" width="17.109375" customWidth="1"/>
+    <col min="75" max="75" width="12.88671875" customWidth="1"/>
+    <col min="76" max="76" width="15.88671875" customWidth="1"/>
+    <col min="77" max="77" width="14.109375" style="24" customWidth="1"/>
+    <col min="78" max="78" width="15" style="24" customWidth="1"/>
+    <col min="79" max="79" width="19.33203125" style="24" customWidth="1"/>
+    <col min="80" max="80" width="15" style="24" customWidth="1"/>
+    <col min="81" max="83" width="9.33203125" style="24" customWidth="1"/>
+    <col min="84" max="84" width="8.88671875" style="24" customWidth="1"/>
+    <col min="85" max="85" width="10.5546875" style="24" customWidth="1"/>
+    <col min="86" max="86" width="18.6640625" style="24" customWidth="1"/>
+    <col min="87" max="87" width="16.88671875" style="24" customWidth="1"/>
+    <col min="88" max="88" width="10.33203125" style="24" customWidth="1"/>
+    <col min="89" max="89" width="16.88671875" style="24" customWidth="1"/>
+    <col min="90" max="90" width="9.44140625" style="24" customWidth="1"/>
+    <col min="91" max="91" width="14.44140625" style="24" customWidth="1"/>
+    <col min="92" max="92" width="10.33203125" style="24" customWidth="1"/>
+    <col min="93" max="93" width="17.6640625" style="24" customWidth="1"/>
+    <col min="94" max="94" width="16.109375" style="24" customWidth="1"/>
+    <col min="95" max="95" width="18.44140625" style="24" customWidth="1"/>
+    <col min="97" max="97" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:97" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:97" s="47" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="46" t="s">
         <v>1</v>
       </c>
@@ -9918,7 +9855,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="44" t="s">
         <v>440</v>
       </c>
@@ -10189,7 +10126,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="3" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="44" t="s">
         <v>454</v>
       </c>
@@ -10458,7 +10395,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="4" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="44" t="s">
         <v>456</v>
       </c>
@@ -10727,7 +10664,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="5" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="44" t="s">
         <v>458</v>
       </c>
@@ -10998,7 +10935,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="6" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="44" t="s">
         <v>461</v>
       </c>
@@ -11269,7 +11206,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="7" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="44" t="s">
         <v>463</v>
       </c>
@@ -11540,7 +11477,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="8" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="44" t="s">
         <v>465</v>
       </c>
@@ -11811,7 +11748,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="9" spans="1:97" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:97" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="44" t="s">
         <v>467</v>
       </c>
@@ -12080,7 +12017,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="10" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="44" t="s">
         <v>469</v>
       </c>
@@ -12349,7 +12286,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="11" spans="1:97" s="49" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:97" s="49" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="44" t="s">
         <v>471</v>
       </c>
@@ -12620,7 +12557,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="12" spans="1:97" s="31" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:97" s="31" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>473</v>
       </c>
@@ -12899,7 +12836,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="18" spans="81:81" x14ac:dyDescent="0.25">
+    <row r="18" spans="81:81" x14ac:dyDescent="0.3">
       <c r="CC18" s="24" t="s">
         <v>711</v>
       </c>
@@ -12946,9 +12883,9 @@
       <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -12986,7 +12923,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>718</v>
       </c>
@@ -13034,210 +12971,60 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="5.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="17.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.28515625" customWidth="1"/>
-    <col min="14" max="14" width="6.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="4.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="68" t="s">
-        <v>862</v>
+        <v>847</v>
       </c>
       <c r="B1" s="68" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="C1" s="68" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="D1" s="68" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="E1" s="68" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="F1" s="68" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="G1" s="68" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="H1" s="68" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="I1" s="68" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="J1" s="68" t="s">
-        <v>855</v>
+        <v>50</v>
       </c>
       <c r="K1" s="68" t="s">
-        <v>50</v>
+        <v>856</v>
       </c>
       <c r="L1" s="68" t="s">
-        <v>856</v>
-      </c>
-      <c r="M1" s="68" t="s">
-        <v>878</v>
-      </c>
-      <c r="N1" s="68" t="s">
         <v>242</v>
       </c>
-      <c r="O1" s="68" t="s">
+      <c r="M1" s="69" t="s">
         <v>857</v>
       </c>
-      <c r="P1" s="68" t="s">
+      <c r="N1" s="69" t="s">
         <v>858</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>863</v>
-      </c>
-      <c r="B2" t="s">
-        <v>864</v>
-      </c>
-      <c r="F2" s="69" t="s">
-        <v>859</v>
-      </c>
-      <c r="G2">
-        <v>546</v>
-      </c>
-      <c r="H2">
-        <v>615</v>
-      </c>
-      <c r="I2" s="69" t="s">
-        <v>865</v>
-      </c>
-      <c r="K2">
-        <v>2812</v>
-      </c>
-      <c r="L2" t="s">
-        <v>860</v>
-      </c>
-      <c r="M2" s="69" t="s">
-        <v>879</v>
-      </c>
-      <c r="N2" t="s">
-        <v>861</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>864</v>
-      </c>
-      <c r="E3" t="s">
-        <v>872</v>
-      </c>
-      <c r="F3" t="s">
-        <v>866</v>
-      </c>
-      <c r="G3" t="s">
-        <v>868</v>
-      </c>
-      <c r="H3" t="s">
-        <v>867</v>
-      </c>
-      <c r="I3" t="s">
-        <v>869</v>
-      </c>
-      <c r="J3" t="s">
-        <v>391</v>
-      </c>
-      <c r="K3" t="s">
-        <v>870</v>
-      </c>
-      <c r="L3" t="s">
-        <v>871</v>
-      </c>
-      <c r="N3" t="s">
-        <v>861</v>
-      </c>
-      <c r="O3" t="s">
-        <v>873</v>
-      </c>
-      <c r="P3" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>864</v>
-      </c>
-      <c r="F4" t="s">
-        <v>875</v>
-      </c>
-      <c r="G4" t="s">
-        <v>877</v>
-      </c>
-      <c r="H4" t="s">
-        <v>876</v>
-      </c>
-      <c r="N4" t="s">
-        <v>861</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>864</v>
-      </c>
-      <c r="E5" t="s">
-        <v>872</v>
-      </c>
-      <c r="F5" t="s">
-        <v>875</v>
-      </c>
-      <c r="G5" t="s">
-        <v>877</v>
-      </c>
-      <c r="H5" t="s">
-        <v>876</v>
-      </c>
-      <c r="I5" t="s">
-        <v>872</v>
-      </c>
-      <c r="J5" t="s">
-        <v>872</v>
-      </c>
-      <c r="K5" t="s">
-        <v>870</v>
-      </c>
-      <c r="L5" t="s">
-        <v>871</v>
-      </c>
-      <c r="N5" t="s">
-        <v>861</v>
-      </c>
-      <c r="O5" t="s">
-        <v>873</v>
-      </c>
-      <c r="P5" t="s">
-        <v>874</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13249,18 +13036,18 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="56.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:143" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:143" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -13691,7 +13478,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="2" spans="1:143" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:143" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>585</v>
       </c>
@@ -14076,7 +13863,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="3" spans="1:143" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:143" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>624</v>
       </c>
@@ -14473,7 +14260,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="4" spans="1:143" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:143" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>633</v>
       </c>
@@ -14871,20 +14658,20 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="6" width="15" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="13" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12.5703125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="44.5546875" customWidth="1"/>
+    <col min="2" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1"/>
+    <col min="11" max="11" width="25.33203125" customWidth="1"/>
+    <col min="12" max="13" width="15.5546875" customWidth="1"/>
+    <col min="15" max="15" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:63" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -15075,7 +14862,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:63" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -15262,7 +15049,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:63" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>87</v>
       </c>
@@ -15451,22 +15238,22 @@
       <selection activeCell="B2" sqref="B2:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="7.42578125" customWidth="1" collapsed="1"/>
-    <col min="66" max="66" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="67" max="67" width="17.5703125" customWidth="1" collapsed="1"/>
-    <col min="97" max="97" width="10.7109375" style="4" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="37.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="19" max="19" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="7.44140625" customWidth="1"/>
+    <col min="66" max="66" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="17.5546875" customWidth="1"/>
+    <col min="97" max="97" width="10.6640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:159" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:159" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -15945,7 +15732,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="2" spans="1:159" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:159" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>132</v>
       </c>
@@ -16398,7 +16185,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="3" spans="1:159" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:159" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>429</v>
       </c>
@@ -16769,7 +16556,7 @@
       <c r="FB3" s="2"/>
       <c r="FC3" s="2"/>
     </row>
-    <row r="4" spans="1:159" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:159" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>140</v>
       </c>
@@ -17114,7 +16901,7 @@
       <c r="FB4" s="2"/>
       <c r="FC4" s="2"/>
     </row>
-    <row r="5" spans="1:159" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:159" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>431</v>
       </c>
@@ -17459,7 +17246,7 @@
       <c r="FB5" s="2"/>
       <c r="FC5" s="2"/>
     </row>
-    <row r="6" spans="1:159" ht="105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:159" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>150</v>
       </c>
@@ -17804,7 +17591,7 @@
       <c r="FB6" s="2"/>
       <c r="FC6" s="2"/>
     </row>
-    <row r="7" spans="1:159" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:159" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>432</v>
       </c>
@@ -18149,7 +17936,7 @@
       <c r="FB7" s="2"/>
       <c r="FC7" s="2"/>
     </row>
-    <row r="8" spans="1:159" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:159" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>156</v>
       </c>
@@ -18494,7 +18281,7 @@
       <c r="FB8" s="2"/>
       <c r="FC8" s="2"/>
     </row>
-    <row r="9" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>433</v>
       </c>
@@ -18839,7 +18626,7 @@
       <c r="FB9" s="2"/>
       <c r="FC9" s="2"/>
     </row>
-    <row r="10" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>163</v>
       </c>
@@ -19184,7 +18971,7 @@
       <c r="FB10" s="2"/>
       <c r="FC10" s="2"/>
     </row>
-    <row r="11" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>434</v>
       </c>
@@ -19529,7 +19316,7 @@
       <c r="FB11" s="2"/>
       <c r="FC11" s="2"/>
     </row>
-    <row r="12" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:159" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>684</v>
       </c>
@@ -19956,499 +19743,499 @@
       <c r="FB12" s="2"/>
       <c r="FC12" s="2"/>
     </row>
-    <row r="13" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:159" x14ac:dyDescent="0.3">
       <c r="CS13"/>
     </row>
-    <row r="14" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:159" x14ac:dyDescent="0.3">
       <c r="CS14"/>
     </row>
-    <row r="15" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:159" x14ac:dyDescent="0.3">
       <c r="CS15"/>
     </row>
-    <row r="16" spans="1:159" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:159" x14ac:dyDescent="0.3">
       <c r="CS16"/>
     </row>
-    <row r="17" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="17" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS17"/>
     </row>
-    <row r="18" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="18" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS18"/>
     </row>
-    <row r="19" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="19" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS19"/>
     </row>
-    <row r="20" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="20" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS20"/>
     </row>
-    <row r="21" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="21" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS21"/>
     </row>
-    <row r="22" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="22" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS22"/>
     </row>
-    <row r="23" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="23" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS23"/>
     </row>
-    <row r="24" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="24" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS24"/>
     </row>
-    <row r="25" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="25" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS25"/>
     </row>
-    <row r="26" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="26" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS26"/>
     </row>
-    <row r="27" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="27" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS27"/>
     </row>
-    <row r="28" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="28" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS28"/>
     </row>
-    <row r="29" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="29" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS29"/>
     </row>
-    <row r="30" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="30" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS30"/>
     </row>
-    <row r="31" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="31" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS31"/>
     </row>
-    <row r="32" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="32" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS32"/>
     </row>
-    <row r="33" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="33" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS33"/>
     </row>
-    <row r="34" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="34" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS34"/>
     </row>
-    <row r="35" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="35" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS35"/>
     </row>
-    <row r="36" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="36" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS36"/>
     </row>
-    <row r="37" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="37" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS37"/>
     </row>
-    <row r="38" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="38" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS38"/>
     </row>
-    <row r="39" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="39" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS39"/>
     </row>
-    <row r="40" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="40" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS40"/>
     </row>
-    <row r="41" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="41" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS41"/>
     </row>
-    <row r="42" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="42" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS42"/>
     </row>
-    <row r="43" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="43" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS43"/>
     </row>
-    <row r="44" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="44" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS44"/>
     </row>
-    <row r="45" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="45" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS45"/>
     </row>
-    <row r="46" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="46" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS46"/>
     </row>
-    <row r="47" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="47" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS47"/>
     </row>
-    <row r="48" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="48" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS48"/>
     </row>
-    <row r="49" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="49" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS49"/>
     </row>
-    <row r="50" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="50" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS50"/>
     </row>
-    <row r="51" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="51" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS51"/>
     </row>
-    <row r="52" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="52" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS52"/>
     </row>
-    <row r="53" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="53" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS53"/>
     </row>
-    <row r="54" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="54" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS54"/>
     </row>
-    <row r="55" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="55" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS55"/>
     </row>
-    <row r="56" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="56" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS56"/>
     </row>
-    <row r="57" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="57" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS57"/>
     </row>
-    <row r="58" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="58" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS58"/>
     </row>
-    <row r="59" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="59" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS59"/>
     </row>
-    <row r="60" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="60" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS60"/>
     </row>
-    <row r="61" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="61" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS61"/>
     </row>
-    <row r="62" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="62" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS62"/>
     </row>
-    <row r="63" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="63" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS63"/>
     </row>
-    <row r="64" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="64" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS64"/>
     </row>
-    <row r="65" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="65" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS65"/>
     </row>
-    <row r="66" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="66" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS66"/>
     </row>
-    <row r="67" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="67" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS67"/>
     </row>
-    <row r="68" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="68" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS68"/>
     </row>
-    <row r="69" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="69" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS69"/>
     </row>
-    <row r="70" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="70" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS70"/>
     </row>
-    <row r="71" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="71" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS71"/>
     </row>
-    <row r="72" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="72" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS72"/>
     </row>
-    <row r="73" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="73" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS73"/>
     </row>
-    <row r="74" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="74" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS74"/>
     </row>
-    <row r="75" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="75" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS75"/>
     </row>
-    <row r="76" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="76" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS76"/>
     </row>
-    <row r="77" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="77" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS77"/>
     </row>
-    <row r="78" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="78" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS78"/>
     </row>
-    <row r="79" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="79" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS79"/>
     </row>
-    <row r="80" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="80" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS80"/>
     </row>
-    <row r="81" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="81" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS81"/>
     </row>
-    <row r="82" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="82" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS82"/>
     </row>
-    <row r="83" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="83" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS83"/>
     </row>
-    <row r="84" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="84" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS84"/>
     </row>
-    <row r="85" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="85" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS85"/>
     </row>
-    <row r="86" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="86" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS86"/>
     </row>
-    <row r="87" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="87" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS87"/>
     </row>
-    <row r="88" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="88" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS88"/>
     </row>
-    <row r="89" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="89" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS89"/>
     </row>
-    <row r="90" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="90" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS90"/>
     </row>
-    <row r="91" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="91" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS91"/>
     </row>
-    <row r="92" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="92" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS92"/>
     </row>
-    <row r="93" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="93" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS93"/>
     </row>
-    <row r="94" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="94" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS94"/>
     </row>
-    <row r="95" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="95" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS95"/>
     </row>
-    <row r="96" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="96" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS96"/>
     </row>
-    <row r="97" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="97" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS97"/>
     </row>
-    <row r="98" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="98" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS98"/>
     </row>
-    <row r="99" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="99" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS99"/>
     </row>
-    <row r="100" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="100" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS100"/>
     </row>
-    <row r="101" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="101" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS101"/>
     </row>
-    <row r="102" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="102" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS102"/>
     </row>
-    <row r="103" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="103" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS103"/>
     </row>
-    <row r="104" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="104" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS104"/>
     </row>
-    <row r="105" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="105" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS105"/>
     </row>
-    <row r="106" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="106" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS106"/>
     </row>
-    <row r="107" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="107" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS107"/>
     </row>
-    <row r="108" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="108" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS108"/>
     </row>
-    <row r="109" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="109" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS109"/>
     </row>
-    <row r="110" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="110" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS110"/>
     </row>
-    <row r="111" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="111" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS111"/>
     </row>
-    <row r="112" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="112" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS112"/>
     </row>
-    <row r="113" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="113" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS113"/>
     </row>
-    <row r="114" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="114" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS114"/>
     </row>
-    <row r="115" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="115" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS115"/>
     </row>
-    <row r="116" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="116" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS116"/>
     </row>
-    <row r="117" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="117" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS117"/>
     </row>
-    <row r="118" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="118" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS118"/>
     </row>
-    <row r="119" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="119" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS119"/>
     </row>
-    <row r="120" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="120" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS120"/>
     </row>
-    <row r="121" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="121" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS121"/>
     </row>
-    <row r="122" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="122" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS122"/>
     </row>
-    <row r="123" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="123" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS123"/>
     </row>
-    <row r="124" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="124" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS124"/>
     </row>
-    <row r="125" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="125" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS125"/>
     </row>
-    <row r="126" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="126" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS126"/>
     </row>
-    <row r="127" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="127" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS127"/>
     </row>
-    <row r="128" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="128" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS128"/>
     </row>
-    <row r="129" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="129" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS129"/>
     </row>
-    <row r="130" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="130" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS130"/>
     </row>
-    <row r="131" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="131" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS131"/>
     </row>
-    <row r="132" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="132" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS132"/>
     </row>
-    <row r="133" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="133" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS133"/>
     </row>
-    <row r="134" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="134" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS134"/>
     </row>
-    <row r="135" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="135" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS135"/>
     </row>
-    <row r="136" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="136" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS136"/>
     </row>
-    <row r="137" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="137" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS137"/>
     </row>
-    <row r="138" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="138" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS138"/>
     </row>
-    <row r="139" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="139" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS139"/>
     </row>
-    <row r="140" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="140" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS140"/>
     </row>
-    <row r="141" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="141" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS141"/>
     </row>
-    <row r="142" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="142" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS142"/>
     </row>
-    <row r="143" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="143" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS143"/>
     </row>
-    <row r="144" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="144" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS144"/>
     </row>
-    <row r="145" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="145" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS145"/>
     </row>
-    <row r="146" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="146" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS146"/>
     </row>
-    <row r="147" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="147" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS147"/>
     </row>
-    <row r="148" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="148" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS148"/>
     </row>
-    <row r="149" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="149" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS149"/>
     </row>
-    <row r="150" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="150" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS150"/>
     </row>
-    <row r="151" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="151" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS151"/>
     </row>
-    <row r="152" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="152" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS152"/>
     </row>
-    <row r="153" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="153" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS153"/>
     </row>
-    <row r="154" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="154" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS154"/>
     </row>
-    <row r="155" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="155" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS155"/>
     </row>
-    <row r="156" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="156" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS156"/>
     </row>
-    <row r="157" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="157" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS157"/>
     </row>
-    <row r="158" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="158" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS158"/>
     </row>
-    <row r="159" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="159" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS159"/>
     </row>
-    <row r="160" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="160" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS160"/>
     </row>
-    <row r="161" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="161" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS161"/>
     </row>
-    <row r="162" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="162" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS162"/>
     </row>
-    <row r="163" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="163" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS163"/>
     </row>
-    <row r="164" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="164" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS164"/>
     </row>
-    <row r="165" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="165" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS165"/>
     </row>
-    <row r="166" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="166" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS166"/>
     </row>
-    <row r="167" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="167" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS167"/>
     </row>
-    <row r="168" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="168" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS168"/>
     </row>
-    <row r="169" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="169" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS169"/>
     </row>
-    <row r="170" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="170" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS170"/>
     </row>
-    <row r="171" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="171" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS171"/>
     </row>
-    <row r="172" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="172" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS172"/>
     </row>
-    <row r="173" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="173" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS173"/>
     </row>
-    <row r="174" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="174" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS174"/>
     </row>
-    <row r="175" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="175" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS175"/>
     </row>
-    <row r="176" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="176" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS176"/>
     </row>
-    <row r="177" spans="97:97" x14ac:dyDescent="0.25">
+    <row r="177" spans="97:97" x14ac:dyDescent="0.3">
       <c r="CS177"/>
     </row>
   </sheetData>
@@ -20465,17 +20252,17 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="43.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="21.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -20510,7 +20297,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>174</v>
       </c>
@@ -20537,7 +20324,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>178</v>
       </c>
@@ -20568,7 +20355,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>179</v>
       </c>
@@ -20589,7 +20376,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>180</v>
       </c>
@@ -20625,19 +20412,19 @@
       <selection sqref="A1:Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="52" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="10" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="47" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="37.7109375" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="52" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.6640625" customWidth="1"/>
+    <col min="17" max="17" width="47" customWidth="1"/>
+    <col min="18" max="18" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -20688,7 +20475,7 @@
       </c>
       <c r="R1" s="20"/>
     </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>189</v>
       </c>
@@ -20739,7 +20526,7 @@
       </c>
       <c r="R2" s="18"/>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>189</v>
       </c>
@@ -20790,7 +20577,7 @@
       </c>
       <c r="R3" s="16"/>
     </row>
-    <row r="4" spans="2:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>189</v>
       </c>
@@ -20841,7 +20628,7 @@
       </c>
       <c r="R4" s="17"/>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>189</v>
       </c>
@@ -20892,7 +20679,7 @@
       </c>
       <c r="R5" s="16"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>189</v>
       </c>
@@ -20954,13 +20741,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="35.88671875" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -20980,7 +20767,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>244</v>
       </c>
@@ -21000,7 +20787,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>248</v>
       </c>
@@ -21031,12 +20818,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="9" width="16" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -21065,7 +20852,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>250</v>
       </c>

</xml_diff>

<commit_message>
Added code for excel driven approach
</commit_message>
<xml_diff>
--- a/src/main/resources/config/stageSA/TestData/TestData.xlsx
+++ b/src/main/resources/config/stageSA/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15108" windowHeight="8988" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15105" windowHeight="8985" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CardHolder" sheetId="19" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4185" uniqueCount="859">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4198" uniqueCount="869">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -2609,6 +2609,36 @@
   </si>
   <si>
     <t>load</t>
+  </si>
+  <si>
+    <t>ScenarioID</t>
+  </si>
+  <si>
+    <t>ClearPin</t>
+  </si>
+  <si>
+    <t>5377164791627316</t>
+  </si>
+  <si>
+    <t>644</t>
+  </si>
+  <si>
+    <t>398</t>
+  </si>
+  <si>
+    <t>925</t>
+  </si>
+  <si>
+    <t>4271</t>
+  </si>
+  <si>
+    <t>13942FFFFFFFFFFF</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>SurchargeWithSystemCalculatedPlan</t>
   </si>
 </sst>
 </file>
@@ -2793,7 +2823,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -2903,7 +2933,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
@@ -3214,14 +3247,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="55" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A1" s="52" t="s">
         <v>1</v>
       </c>
@@ -3391,7 +3424,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A2" s="58" t="s">
         <v>783</v>
       </c>
@@ -3485,7 +3518,7 @@
       <c r="BC2" s="58"/>
       <c r="BD2" s="58"/>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>794</v>
       </c>
@@ -3559,7 +3592,7 @@
       <c r="BC3" s="2"/>
       <c r="BD3" s="2"/>
     </row>
-    <row r="4" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>795</v>
       </c>
@@ -3633,7 +3666,7 @@
       <c r="BC4" s="2"/>
       <c r="BD4" s="2"/>
     </row>
-    <row r="5" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>797</v>
       </c>
@@ -3723,7 +3756,7 @@
       <c r="BC5" s="2"/>
       <c r="BD5" s="2"/>
     </row>
-    <row r="6" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>802</v>
       </c>
@@ -3797,7 +3830,7 @@
       <c r="BC6" s="2"/>
       <c r="BD6" s="2"/>
     </row>
-    <row r="7" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>803</v>
       </c>
@@ -3877,7 +3910,7 @@
       <c r="BC7" s="2"/>
       <c r="BD7" s="2"/>
     </row>
-    <row r="8" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>806</v>
       </c>
@@ -3961,7 +3994,7 @@
       <c r="BC8" s="2"/>
       <c r="BD8" s="2"/>
     </row>
-    <row r="9" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>809</v>
       </c>
@@ -4053,7 +4086,7 @@
       <c r="BC9" s="2"/>
       <c r="BD9" s="2"/>
     </row>
-    <row r="10" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>814</v>
       </c>
@@ -4145,7 +4178,7 @@
       <c r="BC10" s="2"/>
       <c r="BD10" s="2"/>
     </row>
-    <row r="11" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>815</v>
       </c>
@@ -4243,7 +4276,7 @@
       <c r="BC11" s="2"/>
       <c r="BD11" s="2"/>
     </row>
-    <row r="12" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>818</v>
       </c>
@@ -4341,7 +4374,7 @@
       <c r="BC12" s="2"/>
       <c r="BD12" s="2"/>
     </row>
-    <row r="13" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>820</v>
       </c>
@@ -4441,7 +4474,7 @@
       <c r="BC13" s="2"/>
       <c r="BD13" s="2"/>
     </row>
-    <row r="14" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>822</v>
       </c>
@@ -4541,7 +4574,7 @@
       <c r="BC14" s="2"/>
       <c r="BD14" s="2"/>
     </row>
-    <row r="15" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>823</v>
       </c>
@@ -4641,7 +4674,7 @@
       <c r="BC15" s="2"/>
       <c r="BD15" s="2"/>
     </row>
-    <row r="16" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>824</v>
       </c>
@@ -4745,7 +4778,7 @@
       <c r="BC16" s="2"/>
       <c r="BD16" s="2"/>
     </row>
-    <row r="17" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A17" s="58" t="s">
         <v>835</v>
       </c>
@@ -4853,7 +4886,7 @@
       <c r="BC17" s="58"/>
       <c r="BD17" s="58"/>
     </row>
-    <row r="18" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>836</v>
       </c>
@@ -4961,7 +4994,7 @@
       <c r="BC18" s="2"/>
       <c r="BD18" s="2"/>
     </row>
-    <row r="19" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>837</v>
       </c>
@@ -5069,7 +5102,7 @@
       <c r="BC19" s="2"/>
       <c r="BD19" s="2"/>
     </row>
-    <row r="20" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>838</v>
       </c>
@@ -5177,7 +5210,7 @@
       <c r="BC20" s="2"/>
       <c r="BD20" s="2"/>
     </row>
-    <row r="21" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>839</v>
       </c>
@@ -5251,7 +5284,7 @@
       <c r="BC21" s="2"/>
       <c r="BD21" s="2"/>
     </row>
-    <row r="22" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>840</v>
       </c>
@@ -5325,7 +5358,7 @@
       <c r="BC22" s="2"/>
       <c r="BD22" s="2"/>
     </row>
-    <row r="23" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>841</v>
       </c>
@@ -5399,7 +5432,7 @@
       <c r="BC23" s="2"/>
       <c r="BD23" s="2"/>
     </row>
-    <row r="24" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>842</v>
       </c>
@@ -5473,7 +5506,7 @@
       <c r="BC24" s="2"/>
       <c r="BD24" s="2"/>
     </row>
-    <row r="25" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>843</v>
       </c>
@@ -5547,7 +5580,7 @@
       <c r="BC25" s="2"/>
       <c r="BD25" s="2"/>
     </row>
-    <row r="26" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>844</v>
       </c>
@@ -5621,7 +5654,7 @@
       <c r="BC26" s="2"/>
       <c r="BD26" s="2"/>
     </row>
-    <row r="27" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>845</v>
       </c>
@@ -5695,7 +5728,7 @@
       <c r="BC27" s="2"/>
       <c r="BD27" s="2"/>
     </row>
-    <row r="28" spans="1:56" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>846</v>
       </c>
@@ -5803,12 +5836,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="34.6640625" customWidth="1"/>
+    <col min="7" max="7" width="34.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -5831,7 +5864,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>254</v>
       </c>
@@ -5854,7 +5887,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>258</v>
       </c>
@@ -5875,7 +5908,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>260</v>
       </c>
@@ -5907,14 +5940,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="6" max="6" width="32.6640625" customWidth="1"/>
+    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="32.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -5934,7 +5967,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>244</v>
       </c>
@@ -5954,7 +5987,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>248</v>
       </c>
@@ -5987,44 +6020,44 @@
       <selection activeCell="BV5" sqref="BV5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.5546875" customWidth="1"/>
-    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="28.5546875" customWidth="1"/>
-    <col min="26" max="26" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.5703125" customWidth="1"/>
+    <col min="26" max="26" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="63" max="63" width="15" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="66" max="66" width="46" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="73" max="73" width="15" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:75" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:75" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -6251,7 +6284,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="2" spans="1:75" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:75" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>440</v>
       </c>
@@ -6460,7 +6493,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="3" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>454</v>
       </c>
@@ -6667,7 +6700,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="4" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>456</v>
       </c>
@@ -6874,7 +6907,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="5" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>458</v>
       </c>
@@ -7083,7 +7116,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="6" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>461</v>
       </c>
@@ -7292,7 +7325,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="7" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>463</v>
       </c>
@@ -7501,7 +7534,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="8" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>465</v>
       </c>
@@ -7714,7 +7747,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="9" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>467</v>
       </c>
@@ -7921,7 +7954,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="10" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>469</v>
       </c>
@@ -8128,7 +8161,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="11" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>471</v>
       </c>
@@ -8337,7 +8370,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="12" spans="1:75" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>473</v>
       </c>
@@ -8568,12 +8601,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -8627,7 +8660,7 @@
       </c>
       <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:18" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>287</v>
       </c>
@@ -8680,7 +8713,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>288</v>
       </c>
@@ -8733,7 +8766,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>289</v>
       </c>
@@ -8786,7 +8819,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>290</v>
       </c>
@@ -8839,7 +8872,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>291</v>
       </c>
@@ -8905,18 +8938,18 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.6640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="33" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="33" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="33" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" style="31" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="31"/>
+    <col min="1" max="1" width="61.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="33" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="33" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="33" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -8936,7 +8969,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
         <v>368</v>
       </c>
@@ -8956,7 +8989,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>369</v>
       </c>
@@ -8976,7 +9009,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>376</v>
       </c>
@@ -8996,7 +9029,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>370</v>
       </c>
@@ -9016,7 +9049,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>371</v>
       </c>
@@ -9036,7 +9069,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>372</v>
       </c>
@@ -9056,7 +9089,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>373</v>
       </c>
@@ -9089,27 +9122,27 @@
       <selection activeCell="B1" sqref="B1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" style="24" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="24" customWidth="1"/>
-    <col min="3" max="3" width="9.33203125" style="24" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="24" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" style="24" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" style="24" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="24" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="24" customWidth="1"/>
     <col min="5" max="5" width="15" style="24" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" style="24" customWidth="1"/>
-    <col min="7" max="7" width="18.88671875" style="24" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" style="24"/>
-    <col min="10" max="10" width="9.6640625" style="24" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" style="24" customWidth="1"/>
-    <col min="12" max="12" width="20.33203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.109375" style="24" customWidth="1"/>
-    <col min="14" max="14" width="20.33203125" style="24" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="9.109375" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="24"/>
+    <col min="6" max="6" width="14.7109375" style="24" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" style="24" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" style="24"/>
+    <col min="10" max="10" width="9.7109375" style="24" customWidth="1"/>
+    <col min="11" max="11" width="8.5703125" style="24" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" style="24" customWidth="1"/>
+    <col min="14" max="14" width="20.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="9.140625" customWidth="1"/>
+    <col min="18" max="16384" width="8.85546875" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
@@ -9156,7 +9189,7 @@
       <c r="P1" s="24"/>
       <c r="Q1" s="24"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>303</v>
       </c>
@@ -9199,17 +9232,17 @@
       <c r="P2" s="24"/>
       <c r="Q2" s="24"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O3" s="24"/>
       <c r="P3" s="24"/>
       <c r="Q3" s="24"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O4" s="24"/>
       <c r="P4" s="24"/>
       <c r="Q4" s="24"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="O13" s="24"/>
       <c r="P13" s="24"/>
       <c r="Q13" s="24"/>
@@ -9227,24 +9260,24 @@
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.109375" style="24" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="24" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" style="24" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="9.28515625" style="24" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="24" customWidth="1"/>
     <col min="4" max="5" width="15" style="24" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="24" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="24" customWidth="1"/>
     <col min="7" max="7" width="15" style="24" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" style="24" customWidth="1"/>
+    <col min="8" max="8" width="19.28515625" style="24" customWidth="1"/>
     <col min="9" max="9" width="15" style="24" customWidth="1"/>
-    <col min="10" max="12" width="9.33203125" style="24" customWidth="1"/>
-    <col min="13" max="13" width="28.6640625" style="24" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" style="24" customWidth="1"/>
-    <col min="15" max="15" width="18.6640625" style="24" customWidth="1"/>
-    <col min="16" max="16384" width="8.88671875" style="24"/>
+    <col min="10" max="12" width="9.28515625" style="24" customWidth="1"/>
+    <col min="13" max="13" width="28.7109375" style="24" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" style="24" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" style="24" customWidth="1"/>
+    <col min="16" max="16384" width="8.85546875" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
@@ -9291,7 +9324,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>320</v>
       </c>
@@ -9332,7 +9365,7 @@
       <c r="N2" s="25"/>
       <c r="O2" s="25"/>
     </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="25" t="s">
         <v>326</v>
       </c>
@@ -9386,20 +9419,20 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.33203125" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" customWidth="1"/>
-    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
@@ -9434,7 +9467,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>331</v>
       </c>
@@ -9490,79 +9523,79 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5546875" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="23.5546875" customWidth="1"/>
-    <col min="17" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="23.5703125" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="14.44140625" customWidth="1"/>
-    <col min="28" max="28" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="28.5546875" customWidth="1"/>
-    <col min="33" max="33" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="39" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="21.88671875" customWidth="1"/>
-    <col min="59" max="59" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="15.88671875" customWidth="1"/>
-    <col min="61" max="61" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="17.5546875" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="14.42578125" customWidth="1"/>
+    <col min="28" max="28" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="28.5703125" customWidth="1"/>
+    <col min="33" max="33" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="39" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="21.85546875" customWidth="1"/>
+    <col min="59" max="59" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="15.85546875" customWidth="1"/>
+    <col min="61" max="61" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="17.5703125" customWidth="1"/>
     <col min="69" max="69" width="15" customWidth="1"/>
-    <col min="71" max="71" width="19.6640625" customWidth="1"/>
-    <col min="72" max="72" width="12.88671875" customWidth="1"/>
-    <col min="73" max="73" width="16.6640625" customWidth="1"/>
-    <col min="74" max="74" width="17.109375" customWidth="1"/>
-    <col min="75" max="75" width="12.88671875" customWidth="1"/>
-    <col min="76" max="76" width="15.88671875" customWidth="1"/>
-    <col min="77" max="77" width="14.109375" style="24" customWidth="1"/>
+    <col min="71" max="71" width="19.7109375" customWidth="1"/>
+    <col min="72" max="72" width="12.85546875" customWidth="1"/>
+    <col min="73" max="73" width="16.7109375" customWidth="1"/>
+    <col min="74" max="74" width="17.140625" customWidth="1"/>
+    <col min="75" max="75" width="12.85546875" customWidth="1"/>
+    <col min="76" max="76" width="15.85546875" customWidth="1"/>
+    <col min="77" max="77" width="14.140625" style="24" customWidth="1"/>
     <col min="78" max="78" width="15" style="24" customWidth="1"/>
-    <col min="79" max="79" width="19.33203125" style="24" customWidth="1"/>
+    <col min="79" max="79" width="19.28515625" style="24" customWidth="1"/>
     <col min="80" max="80" width="15" style="24" customWidth="1"/>
-    <col min="81" max="83" width="9.33203125" style="24" customWidth="1"/>
-    <col min="84" max="84" width="8.88671875" style="24" customWidth="1"/>
-    <col min="85" max="85" width="10.5546875" style="24" customWidth="1"/>
-    <col min="86" max="86" width="18.6640625" style="24" customWidth="1"/>
-    <col min="87" max="87" width="16.88671875" style="24" customWidth="1"/>
-    <col min="88" max="88" width="10.33203125" style="24" customWidth="1"/>
-    <col min="89" max="89" width="16.88671875" style="24" customWidth="1"/>
-    <col min="90" max="90" width="9.44140625" style="24" customWidth="1"/>
-    <col min="91" max="91" width="14.44140625" style="24" customWidth="1"/>
-    <col min="92" max="92" width="10.33203125" style="24" customWidth="1"/>
-    <col min="93" max="93" width="17.6640625" style="24" customWidth="1"/>
-    <col min="94" max="94" width="16.109375" style="24" customWidth="1"/>
-    <col min="95" max="95" width="18.44140625" style="24" customWidth="1"/>
-    <col min="97" max="97" width="11.6640625" customWidth="1"/>
+    <col min="81" max="83" width="9.28515625" style="24" customWidth="1"/>
+    <col min="84" max="84" width="8.85546875" style="24" customWidth="1"/>
+    <col min="85" max="85" width="10.5703125" style="24" customWidth="1"/>
+    <col min="86" max="86" width="18.7109375" style="24" customWidth="1"/>
+    <col min="87" max="87" width="16.85546875" style="24" customWidth="1"/>
+    <col min="88" max="88" width="10.28515625" style="24" customWidth="1"/>
+    <col min="89" max="89" width="16.85546875" style="24" customWidth="1"/>
+    <col min="90" max="90" width="9.42578125" style="24" customWidth="1"/>
+    <col min="91" max="91" width="14.42578125" style="24" customWidth="1"/>
+    <col min="92" max="92" width="10.28515625" style="24" customWidth="1"/>
+    <col min="93" max="93" width="17.7109375" style="24" customWidth="1"/>
+    <col min="94" max="94" width="16.140625" style="24" customWidth="1"/>
+    <col min="95" max="95" width="18.42578125" style="24" customWidth="1"/>
+    <col min="97" max="97" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:97" s="47" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:97" s="47" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="46" t="s">
         <v>1</v>
       </c>
@@ -9855,7 +9888,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="s">
         <v>440</v>
       </c>
@@ -10126,7 +10159,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="3" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
         <v>454</v>
       </c>
@@ -10395,7 +10428,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="4" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="44" t="s">
         <v>456</v>
       </c>
@@ -10664,7 +10697,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="5" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="44" t="s">
         <v>458</v>
       </c>
@@ -10935,7 +10968,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="6" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="44" t="s">
         <v>461</v>
       </c>
@@ -11206,7 +11239,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="7" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="44" t="s">
         <v>463</v>
       </c>
@@ -11477,7 +11510,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="8" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="44" t="s">
         <v>465</v>
       </c>
@@ -11748,7 +11781,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="9" spans="1:97" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:97" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="44" t="s">
         <v>467</v>
       </c>
@@ -12017,7 +12050,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="10" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:97" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="s">
         <v>469</v>
       </c>
@@ -12286,7 +12319,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="11" spans="1:97" s="49" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:97" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="44" t="s">
         <v>471</v>
       </c>
@@ -12557,7 +12590,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="12" spans="1:97" s="31" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:97" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>473</v>
       </c>
@@ -12836,7 +12869,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="18" spans="81:81" x14ac:dyDescent="0.3">
+    <row r="18" spans="81:81" x14ac:dyDescent="0.25">
       <c r="CC18" s="24" t="s">
         <v>711</v>
       </c>
@@ -12883,9 +12916,9 @@
       <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -12923,7 +12956,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>718</v>
       </c>
@@ -12971,56 +13004,122 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="4.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="68" t="s">
+        <v>859</v>
+      </c>
+      <c r="B1" s="68" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="68" t="s">
         <v>847</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="D1" s="68" t="s">
         <v>848</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="E1" s="68" t="s">
         <v>849</v>
       </c>
-      <c r="D1" s="68" t="s">
+      <c r="F1" s="68" t="s">
         <v>850</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="G1" s="68" t="s">
         <v>851</v>
       </c>
-      <c r="F1" s="68" t="s">
+      <c r="H1" s="68" t="s">
         <v>852</v>
       </c>
-      <c r="G1" s="68" t="s">
+      <c r="I1" s="68" t="s">
         <v>853</v>
       </c>
-      <c r="H1" s="68" t="s">
+      <c r="J1" s="68" t="s">
         <v>854</v>
       </c>
-      <c r="I1" s="68" t="s">
+      <c r="K1" s="68" t="s">
         <v>855</v>
       </c>
-      <c r="J1" s="68" t="s">
+      <c r="L1" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="K1" s="68" t="s">
+      <c r="M1" s="68" t="s">
+        <v>860</v>
+      </c>
+      <c r="N1" s="68" t="s">
         <v>856</v>
       </c>
-      <c r="L1" s="68" t="s">
+      <c r="O1" s="68" t="s">
         <v>242</v>
       </c>
-      <c r="M1" s="69" t="s">
+      <c r="P1" s="68" t="s">
         <v>857</v>
       </c>
-      <c r="N1" s="69" t="s">
+      <c r="Q1" s="68" t="s">
         <v>858</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>868</v>
+      </c>
+      <c r="B2" t="s">
+        <v>282</v>
+      </c>
+      <c r="C2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" s="69" t="s">
+        <v>861</v>
+      </c>
+      <c r="H2" s="70" t="s">
+        <v>862</v>
+      </c>
+      <c r="I2" s="70" t="s">
+        <v>863</v>
+      </c>
+      <c r="J2" s="70" t="s">
+        <v>864</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>2901</v>
+      </c>
+      <c r="M2" s="70" t="s">
+        <v>865</v>
+      </c>
+      <c r="N2" s="70" t="s">
+        <v>866</v>
+      </c>
+      <c r="O2" t="s">
+        <v>867</v>
       </c>
     </row>
   </sheetData>
@@ -13036,18 +13135,18 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:143" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:143" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -13478,7 +13577,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="2" spans="1:143" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:143" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>585</v>
       </c>
@@ -13863,7 +13962,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="3" spans="1:143" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:143" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>624</v>
       </c>
@@ -14260,7 +14359,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="4" spans="1:143" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:143" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>633</v>
       </c>
@@ -14658,20 +14757,20 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.5546875" customWidth="1"/>
+    <col min="1" max="1" width="44.5703125" customWidth="1"/>
     <col min="2" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1"/>
-    <col min="11" max="11" width="25.33203125" customWidth="1"/>
-    <col min="12" max="13" width="15.5546875" customWidth="1"/>
-    <col min="15" max="15" width="12.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="25.28515625" customWidth="1"/>
+    <col min="12" max="13" width="15.5703125" customWidth="1"/>
+    <col min="15" max="15" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:63" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -14862,7 +14961,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:63" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:63" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -15049,7 +15148,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:63" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:63" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>87</v>
       </c>
@@ -15238,22 +15337,22 @@
       <selection activeCell="B2" sqref="B2:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.109375" customWidth="1"/>
-    <col min="2" max="2" width="21.5546875" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="17.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
-    <col min="19" max="19" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="7.44140625" customWidth="1"/>
-    <col min="66" max="66" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="17.5546875" customWidth="1"/>
-    <col min="97" max="97" width="10.6640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="37.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="7.42578125" customWidth="1"/>
+    <col min="66" max="66" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="17.5703125" customWidth="1"/>
+    <col min="97" max="97" width="10.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:159" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:159" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -15732,7 +15831,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="2" spans="1:159" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:159" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>132</v>
       </c>
@@ -16185,7 +16284,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="3" spans="1:159" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:159" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>429</v>
       </c>
@@ -16556,7 +16655,7 @@
       <c r="FB3" s="2"/>
       <c r="FC3" s="2"/>
     </row>
-    <row r="4" spans="1:159" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:159" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>140</v>
       </c>
@@ -16901,7 +17000,7 @@
       <c r="FB4" s="2"/>
       <c r="FC4" s="2"/>
     </row>
-    <row r="5" spans="1:159" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:159" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>431</v>
       </c>
@@ -17246,7 +17345,7 @@
       <c r="FB5" s="2"/>
       <c r="FC5" s="2"/>
     </row>
-    <row r="6" spans="1:159" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:159" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>150</v>
       </c>
@@ -17591,7 +17690,7 @@
       <c r="FB6" s="2"/>
       <c r="FC6" s="2"/>
     </row>
-    <row r="7" spans="1:159" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:159" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>432</v>
       </c>
@@ -17936,7 +18035,7 @@
       <c r="FB7" s="2"/>
       <c r="FC7" s="2"/>
     </row>
-    <row r="8" spans="1:159" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:159" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>156</v>
       </c>
@@ -18281,7 +18380,7 @@
       <c r="FB8" s="2"/>
       <c r="FC8" s="2"/>
     </row>
-    <row r="9" spans="1:159" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:159" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>433</v>
       </c>
@@ -18626,7 +18725,7 @@
       <c r="FB9" s="2"/>
       <c r="FC9" s="2"/>
     </row>
-    <row r="10" spans="1:159" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:159" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>163</v>
       </c>
@@ -18971,7 +19070,7 @@
       <c r="FB10" s="2"/>
       <c r="FC10" s="2"/>
     </row>
-    <row r="11" spans="1:159" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:159" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>434</v>
       </c>
@@ -19316,7 +19415,7 @@
       <c r="FB11" s="2"/>
       <c r="FC11" s="2"/>
     </row>
-    <row r="12" spans="1:159" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:159" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>684</v>
       </c>
@@ -19743,499 +19842,499 @@
       <c r="FB12" s="2"/>
       <c r="FC12" s="2"/>
     </row>
-    <row r="13" spans="1:159" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:159" x14ac:dyDescent="0.25">
       <c r="CS13"/>
     </row>
-    <row r="14" spans="1:159" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:159" x14ac:dyDescent="0.25">
       <c r="CS14"/>
     </row>
-    <row r="15" spans="1:159" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:159" x14ac:dyDescent="0.25">
       <c r="CS15"/>
     </row>
-    <row r="16" spans="1:159" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:159" x14ac:dyDescent="0.25">
       <c r="CS16"/>
     </row>
-    <row r="17" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="17" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS17"/>
     </row>
-    <row r="18" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="18" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS18"/>
     </row>
-    <row r="19" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="19" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS19"/>
     </row>
-    <row r="20" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="20" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS20"/>
     </row>
-    <row r="21" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="21" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS21"/>
     </row>
-    <row r="22" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="22" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS22"/>
     </row>
-    <row r="23" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="23" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS23"/>
     </row>
-    <row r="24" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="24" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS24"/>
     </row>
-    <row r="25" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="25" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS25"/>
     </row>
-    <row r="26" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="26" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS26"/>
     </row>
-    <row r="27" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="27" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS27"/>
     </row>
-    <row r="28" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="28" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS28"/>
     </row>
-    <row r="29" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="29" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS29"/>
     </row>
-    <row r="30" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="30" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS30"/>
     </row>
-    <row r="31" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="31" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS31"/>
     </row>
-    <row r="32" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="32" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS32"/>
     </row>
-    <row r="33" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="33" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS33"/>
     </row>
-    <row r="34" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="34" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS34"/>
     </row>
-    <row r="35" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="35" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS35"/>
     </row>
-    <row r="36" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="36" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS36"/>
     </row>
-    <row r="37" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="37" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS37"/>
     </row>
-    <row r="38" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="38" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS38"/>
     </row>
-    <row r="39" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="39" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS39"/>
     </row>
-    <row r="40" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="40" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS40"/>
     </row>
-    <row r="41" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="41" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS41"/>
     </row>
-    <row r="42" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="42" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS42"/>
     </row>
-    <row r="43" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="43" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS43"/>
     </row>
-    <row r="44" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="44" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS44"/>
     </row>
-    <row r="45" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="45" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS45"/>
     </row>
-    <row r="46" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="46" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS46"/>
     </row>
-    <row r="47" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="47" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS47"/>
     </row>
-    <row r="48" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="48" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS48"/>
     </row>
-    <row r="49" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="49" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS49"/>
     </row>
-    <row r="50" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="50" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS50"/>
     </row>
-    <row r="51" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="51" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS51"/>
     </row>
-    <row r="52" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="52" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS52"/>
     </row>
-    <row r="53" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="53" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS53"/>
     </row>
-    <row r="54" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="54" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS54"/>
     </row>
-    <row r="55" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="55" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS55"/>
     </row>
-    <row r="56" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="56" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS56"/>
     </row>
-    <row r="57" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="57" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS57"/>
     </row>
-    <row r="58" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="58" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS58"/>
     </row>
-    <row r="59" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="59" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS59"/>
     </row>
-    <row r="60" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="60" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS60"/>
     </row>
-    <row r="61" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="61" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS61"/>
     </row>
-    <row r="62" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="62" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS62"/>
     </row>
-    <row r="63" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="63" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS63"/>
     </row>
-    <row r="64" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="64" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS64"/>
     </row>
-    <row r="65" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="65" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS65"/>
     </row>
-    <row r="66" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="66" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS66"/>
     </row>
-    <row r="67" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="67" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS67"/>
     </row>
-    <row r="68" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="68" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS68"/>
     </row>
-    <row r="69" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="69" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS69"/>
     </row>
-    <row r="70" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="70" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS70"/>
     </row>
-    <row r="71" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="71" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS71"/>
     </row>
-    <row r="72" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="72" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS72"/>
     </row>
-    <row r="73" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="73" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS73"/>
     </row>
-    <row r="74" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="74" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS74"/>
     </row>
-    <row r="75" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="75" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS75"/>
     </row>
-    <row r="76" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="76" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS76"/>
     </row>
-    <row r="77" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="77" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS77"/>
     </row>
-    <row r="78" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="78" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS78"/>
     </row>
-    <row r="79" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="79" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS79"/>
     </row>
-    <row r="80" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="80" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS80"/>
     </row>
-    <row r="81" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="81" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS81"/>
     </row>
-    <row r="82" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="82" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS82"/>
     </row>
-    <row r="83" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="83" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS83"/>
     </row>
-    <row r="84" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="84" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS84"/>
     </row>
-    <row r="85" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="85" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS85"/>
     </row>
-    <row r="86" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="86" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS86"/>
     </row>
-    <row r="87" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="87" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS87"/>
     </row>
-    <row r="88" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="88" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS88"/>
     </row>
-    <row r="89" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="89" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS89"/>
     </row>
-    <row r="90" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="90" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS90"/>
     </row>
-    <row r="91" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="91" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS91"/>
     </row>
-    <row r="92" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="92" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS92"/>
     </row>
-    <row r="93" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="93" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS93"/>
     </row>
-    <row r="94" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="94" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS94"/>
     </row>
-    <row r="95" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="95" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS95"/>
     </row>
-    <row r="96" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="96" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS96"/>
     </row>
-    <row r="97" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="97" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS97"/>
     </row>
-    <row r="98" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="98" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS98"/>
     </row>
-    <row r="99" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="99" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS99"/>
     </row>
-    <row r="100" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="100" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS100"/>
     </row>
-    <row r="101" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="101" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS101"/>
     </row>
-    <row r="102" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="102" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS102"/>
     </row>
-    <row r="103" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="103" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS103"/>
     </row>
-    <row r="104" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="104" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS104"/>
     </row>
-    <row r="105" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="105" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS105"/>
     </row>
-    <row r="106" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="106" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS106"/>
     </row>
-    <row r="107" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="107" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS107"/>
     </row>
-    <row r="108" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="108" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS108"/>
     </row>
-    <row r="109" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="109" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS109"/>
     </row>
-    <row r="110" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="110" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS110"/>
     </row>
-    <row r="111" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="111" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS111"/>
     </row>
-    <row r="112" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="112" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS112"/>
     </row>
-    <row r="113" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="113" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS113"/>
     </row>
-    <row r="114" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="114" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS114"/>
     </row>
-    <row r="115" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="115" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS115"/>
     </row>
-    <row r="116" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="116" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS116"/>
     </row>
-    <row r="117" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="117" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS117"/>
     </row>
-    <row r="118" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="118" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS118"/>
     </row>
-    <row r="119" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="119" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS119"/>
     </row>
-    <row r="120" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="120" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS120"/>
     </row>
-    <row r="121" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="121" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS121"/>
     </row>
-    <row r="122" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="122" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS122"/>
     </row>
-    <row r="123" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="123" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS123"/>
     </row>
-    <row r="124" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="124" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS124"/>
     </row>
-    <row r="125" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="125" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS125"/>
     </row>
-    <row r="126" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="126" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS126"/>
     </row>
-    <row r="127" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="127" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS127"/>
     </row>
-    <row r="128" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="128" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS128"/>
     </row>
-    <row r="129" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="129" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS129"/>
     </row>
-    <row r="130" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="130" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS130"/>
     </row>
-    <row r="131" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="131" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS131"/>
     </row>
-    <row r="132" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="132" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS132"/>
     </row>
-    <row r="133" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="133" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS133"/>
     </row>
-    <row r="134" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="134" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS134"/>
     </row>
-    <row r="135" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="135" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS135"/>
     </row>
-    <row r="136" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="136" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS136"/>
     </row>
-    <row r="137" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="137" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS137"/>
     </row>
-    <row r="138" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="138" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS138"/>
     </row>
-    <row r="139" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="139" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS139"/>
     </row>
-    <row r="140" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="140" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS140"/>
     </row>
-    <row r="141" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="141" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS141"/>
     </row>
-    <row r="142" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="142" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS142"/>
     </row>
-    <row r="143" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="143" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS143"/>
     </row>
-    <row r="144" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="144" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS144"/>
     </row>
-    <row r="145" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="145" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS145"/>
     </row>
-    <row r="146" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="146" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS146"/>
     </row>
-    <row r="147" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="147" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS147"/>
     </row>
-    <row r="148" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="148" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS148"/>
     </row>
-    <row r="149" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="149" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS149"/>
     </row>
-    <row r="150" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="150" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS150"/>
     </row>
-    <row r="151" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="151" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS151"/>
     </row>
-    <row r="152" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="152" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS152"/>
     </row>
-    <row r="153" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="153" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS153"/>
     </row>
-    <row r="154" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="154" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS154"/>
     </row>
-    <row r="155" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="155" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS155"/>
     </row>
-    <row r="156" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="156" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS156"/>
     </row>
-    <row r="157" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="157" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS157"/>
     </row>
-    <row r="158" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="158" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS158"/>
     </row>
-    <row r="159" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="159" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS159"/>
     </row>
-    <row r="160" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="160" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS160"/>
     </row>
-    <row r="161" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="161" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS161"/>
     </row>
-    <row r="162" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="162" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS162"/>
     </row>
-    <row r="163" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="163" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS163"/>
     </row>
-    <row r="164" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="164" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS164"/>
     </row>
-    <row r="165" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="165" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS165"/>
     </row>
-    <row r="166" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="166" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS166"/>
     </row>
-    <row r="167" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="167" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS167"/>
     </row>
-    <row r="168" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="168" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS168"/>
     </row>
-    <row r="169" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="169" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS169"/>
     </row>
-    <row r="170" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="170" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS170"/>
     </row>
-    <row r="171" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="171" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS171"/>
     </row>
-    <row r="172" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="172" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS172"/>
     </row>
-    <row r="173" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="173" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS173"/>
     </row>
-    <row r="174" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="174" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS174"/>
     </row>
-    <row r="175" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="175" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS175"/>
     </row>
-    <row r="176" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="176" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS176"/>
     </row>
-    <row r="177" spans="97:97" x14ac:dyDescent="0.3">
+    <row r="177" spans="97:97" x14ac:dyDescent="0.25">
       <c r="CS177"/>
     </row>
   </sheetData>
@@ -20252,17 +20351,17 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.33203125" customWidth="1"/>
-    <col min="2" max="2" width="22.109375" customWidth="1"/>
-    <col min="3" max="3" width="21.88671875" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="43.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -20297,7 +20396,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>174</v>
       </c>
@@ -20324,7 +20423,7 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
     </row>
-    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>178</v>
       </c>
@@ -20355,7 +20454,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>179</v>
       </c>
@@ -20376,7 +20475,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>180</v>
       </c>
@@ -20412,19 +20511,19 @@
       <selection sqref="A1:Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="52" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="9" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.6640625" customWidth="1"/>
+    <col min="16" max="16" width="20.7109375" customWidth="1"/>
     <col min="17" max="17" width="47" customWidth="1"/>
-    <col min="18" max="18" width="37.6640625" customWidth="1"/>
+    <col min="18" max="18" width="37.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
@@ -20475,7 +20574,7 @@
       </c>
       <c r="R1" s="20"/>
     </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>189</v>
       </c>
@@ -20526,7 +20625,7 @@
       </c>
       <c r="R2" s="18"/>
     </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>189</v>
       </c>
@@ -20577,7 +20676,7 @@
       </c>
       <c r="R3" s="16"/>
     </row>
-    <row r="4" spans="2:18" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:18" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>189</v>
       </c>
@@ -20628,7 +20727,7 @@
       </c>
       <c r="R4" s="17"/>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>189</v>
       </c>
@@ -20679,7 +20778,7 @@
       </c>
       <c r="R5" s="16"/>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>189</v>
       </c>
@@ -20741,13 +20840,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.88671875" customWidth="1"/>
-    <col min="6" max="6" width="20.109375" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -20767,7 +20866,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>244</v>
       </c>
@@ -20787,7 +20886,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>248</v>
       </c>
@@ -20818,12 +20917,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
@@ -20852,7 +20951,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>250</v>
       </c>

</xml_diff>

<commit_message>
change reversals to reversal and added numbering
</commit_message>
<xml_diff>
--- a/src/main/resources/config/stageSA/TestData/TestData.xlsx
+++ b/src/main/resources/config/stageSA/TestData/TestData.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4196" uniqueCount="869">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4185" uniqueCount="859">
   <si>
     <t>TC01_MI-ISS-Embossing File-Additional Parameters in Embossing File Template</t>
   </si>
@@ -2609,36 +2609,6 @@
   </si>
   <si>
     <t>load</t>
-  </si>
-  <si>
-    <t>5377162908346911</t>
-  </si>
-  <si>
-    <t>207</t>
-  </si>
-  <si>
-    <t>853</t>
-  </si>
-  <si>
-    <t>098</t>
-  </si>
-  <si>
-    <t>2812</t>
-  </si>
-  <si>
-    <t>%s</t>
-  </si>
-  <si>
-    <t>null</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>%Sale</t>
-  </si>
-  <si>
-    <t>%Load</t>
   </si>
 </sst>
 </file>
@@ -3246,9 +3216,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="55.0" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="18.33203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="2" max="2" width="55" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:56" x14ac:dyDescent="0.3">
@@ -5835,7 +5805,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" customWidth="true" width="34.6640625" collapsed="true"/>
+    <col min="7" max="7" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -5939,9 +5909,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="30.88671875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="15.33203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="1" max="1" width="30.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -6019,39 +5989,39 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="5.44140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.88671875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="19.5546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="23.5546875" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="23.5546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="13.6640625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="29.33203125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="21.88671875" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="19.5546875" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="14.44140625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="28.88671875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="16.6640625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="13.109375" collapsed="true"/>
-    <col min="25" max="25" customWidth="true" width="28.5546875" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="62" max="62" bestFit="true" customWidth="true" width="20.5546875" collapsed="true"/>
-    <col min="63" max="63" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="64" max="64" bestFit="true" customWidth="true" width="21.44140625" collapsed="true"/>
-    <col min="65" max="65" bestFit="true" customWidth="true" width="18.109375" collapsed="true"/>
-    <col min="66" max="66" bestFit="true" customWidth="true" width="46.0" collapsed="true"/>
-    <col min="71" max="71" bestFit="true" customWidth="true" width="17.5546875" collapsed="true"/>
-    <col min="72" max="72" bestFit="true" customWidth="true" width="22.88671875" collapsed="true"/>
-    <col min="73" max="73" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="75" max="75" bestFit="true" customWidth="true" width="20.6640625" collapsed="true"/>
+    <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.5546875" customWidth="1"/>
+    <col min="14" max="14" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="28.5546875" customWidth="1"/>
+    <col min="26" max="26" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="15" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="46" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="15" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:75" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -8600,7 +8570,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="51.5546875" collapsed="true"/>
+    <col min="1" max="1" width="51.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
@@ -8937,13 +8907,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="31" width="61.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="33" width="22.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="33" width="9.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="33" width="9.6640625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="31" width="19.33203125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="31" width="20.44140625" collapsed="true"/>
-    <col min="7" max="16384" style="31" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="61.6640625" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="33" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="33" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="33" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.44140625" style="31" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -9121,22 +9091,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="24" width="29.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="24" width="22.6640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="24" width="9.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="24" width="9.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="24" width="15.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="24" width="14.6640625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="24" width="18.88671875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="24" width="10.33203125" collapsed="true"/>
-    <col min="9" max="9" style="24" width="8.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="24" width="9.6640625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" style="24" width="8.5546875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="24" width="20.33203125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="24" width="11.109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="24" width="20.33203125" collapsed="true"/>
-    <col min="15" max="17" customWidth="true" width="9.109375" collapsed="true"/>
-    <col min="18" max="16384" style="24" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="29.6640625" style="24" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="24" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="24" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="24" customWidth="1"/>
+    <col min="5" max="5" width="15" style="24" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" style="24" customWidth="1"/>
+    <col min="7" max="7" width="18.88671875" style="24" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" style="24"/>
+    <col min="10" max="10" width="9.6640625" style="24" customWidth="1"/>
+    <col min="11" max="11" width="8.5546875" style="24" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.109375" style="24" customWidth="1"/>
+    <col min="14" max="14" width="20.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="9.109375" customWidth="1"/>
+    <col min="18" max="16384" width="8.88671875" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -9259,19 +9229,19 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="24" width="29.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="24" width="9.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="24" width="9.6640625" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" style="24" width="15.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="24" width="14.109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="24" width="15.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="24" width="19.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="24" width="15.0" collapsed="true"/>
-    <col min="10" max="12" customWidth="true" style="24" width="9.33203125" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" style="24" width="28.6640625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="24" width="11.6640625" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" style="24" width="18.6640625" collapsed="true"/>
-    <col min="16" max="16384" style="24" width="8.88671875" collapsed="true"/>
+    <col min="1" max="1" width="29.109375" style="24" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" style="24" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="24" customWidth="1"/>
+    <col min="4" max="5" width="15" style="24" customWidth="1"/>
+    <col min="6" max="6" width="14.109375" style="24" customWidth="1"/>
+    <col min="7" max="7" width="15" style="24" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" style="24" customWidth="1"/>
+    <col min="9" max="9" width="15" style="24" customWidth="1"/>
+    <col min="10" max="12" width="9.33203125" style="24" customWidth="1"/>
+    <col min="13" max="13" width="28.6640625" style="24" customWidth="1"/>
+    <col min="14" max="14" width="11.6640625" style="24" customWidth="1"/>
+    <col min="15" max="15" width="18.6640625" style="24" customWidth="1"/>
+    <col min="16" max="16384" width="8.88671875" style="24"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -9418,15 +9388,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="38.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="25.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="17.6640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="10.109375" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" customWidth="1"/>
+    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="24" customFormat="1" x14ac:dyDescent="0.3">
@@ -9522,74 +9492,74 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="40.44140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="6.44140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="17.88671875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="19.5546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="23.5546875" collapsed="true"/>
-    <col min="15" max="16" customWidth="true" width="23.5546875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="19.33203125" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="13.6640625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="29.33203125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="21.88671875" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="19.5546875" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="23.109375" collapsed="true"/>
-    <col min="25" max="27" customWidth="true" width="14.44140625" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="28.88671875" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="16.6640625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="21.88671875" collapsed="true"/>
-    <col min="32" max="32" customWidth="true" width="28.5546875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="9.33203125" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
-    <col min="36" max="39" bestFit="true" customWidth="true" width="12.5546875" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="17.6640625" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="22.109375" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" width="23.109375" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="23.33203125" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="21.88671875" collapsed="true"/>
-    <col min="58" max="58" customWidth="true" width="21.88671875" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" width="15.88671875" collapsed="true"/>
-    <col min="60" max="60" customWidth="true" width="15.88671875" collapsed="true"/>
-    <col min="61" max="61" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="63" max="63" bestFit="true" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="64" max="64" bestFit="true" customWidth="true" width="22.109375" collapsed="true"/>
-    <col min="68" max="68" customWidth="true" width="17.5546875" collapsed="true"/>
-    <col min="69" max="69" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="71" max="71" customWidth="true" width="19.6640625" collapsed="true"/>
-    <col min="72" max="72" customWidth="true" width="12.88671875" collapsed="true"/>
-    <col min="73" max="73" customWidth="true" width="16.6640625" collapsed="true"/>
-    <col min="74" max="74" customWidth="true" width="17.109375" collapsed="true"/>
-    <col min="75" max="75" customWidth="true" width="12.88671875" collapsed="true"/>
-    <col min="76" max="76" customWidth="true" width="15.88671875" collapsed="true"/>
-    <col min="77" max="77" customWidth="true" style="24" width="14.109375" collapsed="true"/>
-    <col min="78" max="78" customWidth="true" style="24" width="15.0" collapsed="true"/>
-    <col min="79" max="79" customWidth="true" style="24" width="19.33203125" collapsed="true"/>
-    <col min="80" max="80" customWidth="true" style="24" width="15.0" collapsed="true"/>
-    <col min="81" max="83" customWidth="true" style="24" width="9.33203125" collapsed="true"/>
-    <col min="84" max="84" customWidth="true" style="24" width="8.88671875" collapsed="true"/>
-    <col min="85" max="85" customWidth="true" style="24" width="10.5546875" collapsed="true"/>
-    <col min="86" max="86" customWidth="true" style="24" width="18.6640625" collapsed="true"/>
-    <col min="87" max="87" customWidth="true" style="24" width="16.88671875" collapsed="true"/>
-    <col min="88" max="88" customWidth="true" style="24" width="10.33203125" collapsed="true"/>
-    <col min="89" max="89" customWidth="true" style="24" width="16.88671875" collapsed="true"/>
-    <col min="90" max="90" customWidth="true" style="24" width="9.44140625" collapsed="true"/>
-    <col min="91" max="91" customWidth="true" style="24" width="14.44140625" collapsed="true"/>
-    <col min="92" max="92" customWidth="true" style="24" width="10.33203125" collapsed="true"/>
-    <col min="93" max="93" customWidth="true" style="24" width="17.6640625" collapsed="true"/>
-    <col min="94" max="94" customWidth="true" style="24" width="16.109375" collapsed="true"/>
-    <col min="95" max="95" customWidth="true" style="24" width="18.44140625" collapsed="true"/>
-    <col min="97" max="97" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="1" max="1" width="40.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="23.5546875" customWidth="1"/>
+    <col min="17" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="14.44140625" customWidth="1"/>
+    <col min="28" max="28" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="28.5546875" customWidth="1"/>
+    <col min="33" max="33" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="39" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="21.88671875" customWidth="1"/>
+    <col min="59" max="59" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="15.88671875" customWidth="1"/>
+    <col min="61" max="61" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="17.5546875" customWidth="1"/>
+    <col min="69" max="69" width="15" customWidth="1"/>
+    <col min="71" max="71" width="19.6640625" customWidth="1"/>
+    <col min="72" max="72" width="12.88671875" customWidth="1"/>
+    <col min="73" max="73" width="16.6640625" customWidth="1"/>
+    <col min="74" max="74" width="17.109375" customWidth="1"/>
+    <col min="75" max="75" width="12.88671875" customWidth="1"/>
+    <col min="76" max="76" width="15.88671875" customWidth="1"/>
+    <col min="77" max="77" width="14.109375" style="24" customWidth="1"/>
+    <col min="78" max="78" width="15" style="24" customWidth="1"/>
+    <col min="79" max="79" width="19.33203125" style="24" customWidth="1"/>
+    <col min="80" max="80" width="15" style="24" customWidth="1"/>
+    <col min="81" max="83" width="9.33203125" style="24" customWidth="1"/>
+    <col min="84" max="84" width="8.88671875" style="24" customWidth="1"/>
+    <col min="85" max="85" width="10.5546875" style="24" customWidth="1"/>
+    <col min="86" max="86" width="18.6640625" style="24" customWidth="1"/>
+    <col min="87" max="87" width="16.88671875" style="24" customWidth="1"/>
+    <col min="88" max="88" width="10.33203125" style="24" customWidth="1"/>
+    <col min="89" max="89" width="16.88671875" style="24" customWidth="1"/>
+    <col min="90" max="90" width="9.44140625" style="24" customWidth="1"/>
+    <col min="91" max="91" width="14.44140625" style="24" customWidth="1"/>
+    <col min="92" max="92" width="10.33203125" style="24" customWidth="1"/>
+    <col min="93" max="93" width="17.6640625" style="24" customWidth="1"/>
+    <col min="94" max="94" width="16.109375" style="24" customWidth="1"/>
+    <col min="95" max="95" width="18.44140625" style="24" customWidth="1"/>
+    <col min="97" max="97" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:97" s="47" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -13053,44 +13023,6 @@
         <v>858</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2" t="s">
-        <v>865</v>
-      </c>
-      <c r="E2" t="s">
-        <v>859</v>
-      </c>
-      <c r="F2" t="s">
-        <v>861</v>
-      </c>
-      <c r="G2" t="s">
-        <v>860</v>
-      </c>
-      <c r="H2" t="s">
-        <v>862</v>
-      </c>
-      <c r="I2" t="s">
-        <v>391</v>
-      </c>
-      <c r="J2" t="s">
-        <v>863</v>
-      </c>
-      <c r="K2" t="s">
-        <v>864</v>
-      </c>
-      <c r="L2" t="s">
-        <v>866</v>
-      </c>
-      <c r="M2" t="s">
-        <v>867</v>
-      </c>
-      <c r="N2" t="s">
-        <v>868</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13106,13 +13038,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="56.109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="16.5546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.5546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="21.109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.44140625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.88671875" collapsed="true"/>
+    <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:143" ht="57.6" x14ac:dyDescent="0.3">
@@ -14728,15 +14660,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="44.5546875" collapsed="true"/>
-    <col min="2" max="6" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="11.88671875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="25.33203125" collapsed="true"/>
-    <col min="12" max="13" customWidth="true" width="15.5546875" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="1" max="1" width="44.5546875" customWidth="1"/>
+    <col min="2" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1"/>
+    <col min="11" max="11" width="25.33203125" customWidth="1"/>
+    <col min="12" max="13" width="15.5546875" customWidth="1"/>
+    <col min="15" max="15" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" ht="57.6" x14ac:dyDescent="0.3">
@@ -15308,17 +15240,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="37.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="17.44140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="20.6640625" collapsed="true"/>
-    <col min="49" max="49" customWidth="true" width="7.44140625" collapsed="true"/>
-    <col min="66" max="66" bestFit="true" customWidth="true" width="14.109375" collapsed="true"/>
-    <col min="67" max="67" customWidth="true" width="17.5546875" collapsed="true"/>
-    <col min="97" max="97" customWidth="true" style="4" width="10.6640625" collapsed="true"/>
+    <col min="1" max="1" width="37.109375" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="19" max="19" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="7.44140625" customWidth="1"/>
+    <col min="66" max="66" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="17.5546875" customWidth="1"/>
+    <col min="97" max="97" width="10.6640625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:159" ht="57.6" x14ac:dyDescent="0.3">
@@ -20322,12 +20254,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="43.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="22.109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.88671875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.6640625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.109375" collapsed="true"/>
+    <col min="1" max="1" width="43.33203125" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
+    <col min="3" max="3" width="21.88671875" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -20482,14 +20414,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="52.0" collapsed="true"/>
-    <col min="9" max="10" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="20.6640625" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="47.0" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="37.6640625" collapsed="true"/>
+    <col min="7" max="7" width="52" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.6640625" customWidth="1"/>
+    <col min="17" max="17" width="47" customWidth="1"/>
+    <col min="18" max="18" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:18" x14ac:dyDescent="0.3">
@@ -20811,8 +20743,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="35.88671875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="20.109375" collapsed="true"/>
+    <col min="1" max="1" width="35.88671875" customWidth="1"/>
+    <col min="6" max="6" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -20888,7 +20820,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="9" max="9" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>